<commit_message>
28/20 Speedy4 Markov OK
</commit_message>
<xml_diff>
--- a/MEDY.xlsx
+++ b/MEDY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F8DEAB-6FF9-4249-A198-775D40B866FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B2D171-2A23-134B-8353-9E462AB92E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-900" yWindow="680" windowWidth="29860" windowHeight="18500" xr2:uid="{A82D0DB8-8028-8749-AD8E-3907692F5E1B}"/>
   </bookViews>
@@ -4998,8 +4998,8 @@
     <v>1.0864</v>
     <v>0.19</v>
     <v>7.0680000000000005E-4</v>
-    <v>-0.35</v>
-    <v>-1.3009999999999999E-3</v>
+    <v>-0.47</v>
+    <v>-1.7469999999999999E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, visionOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. The Company operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+, and Apple TV+. Its products include iPhone 16 Pro, iPhone 16, iPhone 15, iPhone 14, iPhone SE, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, iPad Pro, iPad Air, AirPods, AirPods Pro, AirPods Max, Apple TV and Apple Vision Pro.</v>
     <v>164000</v>
@@ -5010,7 +5010,7 @@
     <v>269.89</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45958.909980022654</v>
+    <v>45958.9436489</v>
     <v>0</v>
     <v>268.14999999999998</v>
     <v>3992064910000</v>
@@ -5020,11 +5020,11 @@
     <v>37.075600000000001</v>
     <v>268.81</v>
     <v>269</v>
-    <v>268.64999999999998</v>
+    <v>268.52999999999997</v>
     <v>14840390000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>41443517</v>
+    <v>41473172</v>
     <v>45206255</v>
     <v>1977</v>
   </rv>
@@ -5157,8 +5157,8 @@
     <v>1.2842</v>
     <v>2.2799999999999998</v>
     <v>1.0045E-2</v>
-    <v>-0.28000000000000003</v>
-    <v>-1.2210000000000001E-3</v>
+    <v>-0.2</v>
+    <v>-8.7239999999999996E-4</v>
     <v>USD</v>
     <v>Amazon.com, Inc. provides a range of products and services to customers. The products offered through its stores include merchandise and content it has purchased for resale and products offered by third-party sellers. The Company’s segments include North America, International and Amazon Web Services (AWS). It serves consumers through its online and physical stores and focuses on selection, price, and convenience. Customers access its offerings through its websites, mobile apps, Alexa, devices, streaming, and physically visiting its stores. It also manufactures and sells electronic devices, including Kindle, Fire tablet, Fire TV, Echo, Ring, Blink, and eero, and develops and produces media content. It serves developers and enterprises of all sizes, including start-ups, government agencies, and academic institutions, through AWS, which offers a set of on-demand technology services, including compute, storage, database, analytics, and machine learning, and other services.</v>
     <v>1546000</v>
@@ -5169,7 +5169,7 @@
     <v>231.48500000000001</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>45958.910078495312</v>
+    <v>45958.943784490628</v>
     <v>9</v>
     <v>226.21</v>
     <v>2444930617500</v>
@@ -5179,11 +5179,11 @@
     <v>34.982900000000001</v>
     <v>226.97</v>
     <v>229.25</v>
-    <v>228.97</v>
+    <v>229.05</v>
     <v>10664910000</v>
     <v>AMZN</v>
     <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
-    <v>46903995</v>
+    <v>46991794</v>
     <v>45445761</v>
     <v>1996</v>
   </rv>
@@ -5313,8 +5313,8 @@
     <v>1.2004999999999999</v>
     <v>10.92</v>
     <v>3.0162000000000001E-2</v>
-    <v>0.84</v>
-    <v>2.2520000000000001E-3</v>
+    <v>0.33</v>
+    <v>8.8480000000000004E-4</v>
     <v>USD</v>
     <v>Broadcom Inc. is a global technology firm that designs, develops, and supplies a range of semiconductors, enterprise software and security solutions. The Company operates through two segments: semiconductor solutions and infrastructure software. Its semiconductor solutions segment includes all of its product lines and intellectual property (IP) licensing. It provides a variety of radio frequency semiconductor devices, wireless connectivity solutions, custom touch controllers, and inductive charging solutions for mobile applications. Its infrastructure software segment includes its private and hybrid cloud, application development and delivery, software-defined edge, application networking and security, mainframe, distributed and cybersecurity solutions, and its FC SAN business. It provides a portfolio of software solutions that enable customers to plan, develop, automate, manage and secure applications across mainframe, distributed, mobile and cloud platforms.</v>
     <v>37000</v>
@@ -5325,7 +5325,7 @@
     <v>374.06</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45958.910013506247</v>
+    <v>45958.943683830468</v>
     <v>18</v>
     <v>362.53</v>
     <v>1761300474050</v>
@@ -5335,11 +5335,11 @@
     <v>92.81</v>
     <v>362.05</v>
     <v>372.97</v>
-    <v>373.81</v>
+    <v>373.3</v>
     <v>4722365000</v>
     <v>AVGO</v>
     <v>BROADCOM INC. (XNAS:AVGO)</v>
-    <v>20990453</v>
+    <v>21019816</v>
     <v>20556836</v>
     <v>2018</v>
   </rv>
@@ -5361,7 +5361,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1o3qh</v>
     <v>268435456</v>
@@ -5384,7 +5384,7 @@
     <v>84.22</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45958.908744096872</v>
+    <v>45958.932806700781</v>
     <v>22</v>
     <v>81.78</v>
     <v>258928500000</v>
@@ -5398,7 +5398,7 @@
     <v>3101404000</v>
     <v>AZN</v>
     <v>ASTRAZENECA PLC (XNAS:AZN)</v>
-    <v>3661505</v>
+    <v>3661534</v>
     <v>5720341</v>
     <v>1992</v>
   </rv>
@@ -5415,7 +5415,7 @@
     <v>2</v>
     <v>11</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1oldm</v>
     <v>268435456</v>
@@ -5426,8 +5426,8 @@
     <v>1.9781</v>
     <v>0.03</v>
     <v>8.7980000000000003E-3</v>
-    <v>0.01</v>
-    <v>2.9070000000000003E-3</v>
+    <v>0.02</v>
+    <v>5.8140000000000006E-3</v>
     <v>USD</v>
     <v>Ballard Power Systems Inc. is engaged in the design, development, manufacture, sale and service of proton exchange membrane (PEM) fuel cell products for a variety of applications, focusing on power products for bus, truck, rail, marine, stationary and emerging market (material handling, off-road and other) applications, as well as the delivery of services, including technology solutions, after sales services and training. The Company operates through fuel cell products and services segment. Embedded in each Ballard fuel cell product lies a stack of unit cells designed with its PEM fuel cell technology that includes membrane electrode assemblies, catalysts, plates, and other key components, and draw on intellectual property from its patent portfolio, together with its experience and know-how, in key areas of PEM fuel cell stack design, operation, production processes and systems integration.</v>
     <v>887</v>
@@ -5438,7 +5438,7 @@
     <v>3.5598999999999998</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45958.904144617969</v>
+    <v>45958.931424652343</v>
     <v>25</v>
     <v>3.3712</v>
     <v>1433756000</v>
@@ -5448,11 +5448,11 @@
     <v>0</v>
     <v>3.41</v>
     <v>3.44</v>
-    <v>3.45</v>
+    <v>3.46</v>
     <v>300577700</v>
     <v>BLDP</v>
     <v>BALLARD POWER SYSTEMS INC. (XNAS:BLDP)</v>
-    <v>5762180</v>
+    <v>5776523</v>
     <v>9521175</v>
     <v>2016</v>
   </rv>
@@ -5534,8 +5534,8 @@
     <v>1.3512</v>
     <v>0.4</v>
     <v>3.9610000000000001E-3</v>
-    <v>-0.13370000000000001</v>
-    <v>-1.3189999999999999E-3</v>
+    <v>0.06</v>
+    <v>5.9180000000000007E-4</v>
     <v>USD</v>
     <v>Citigroup Inc. is a global diversified financial services holding company. The Company’s segments include Services, Markets, Banking, Wealth and U.S. Personal Banking (USPB). The Services segment includes Treasury and Trade Solutions (TTS) and securities services. TTS provides an integrated suite of tailored cash management, trade and working capital solutions to multinational corporations, financial institutions and public sector organizations. The Markets segment provides corporate, institutional and public sector clients around the world with a full range of sales and trading services across equities, foreign exchange, rates, spread products and commodities. The Banking segment includes investment banking, which supports client capital-raising needs to help strengthen and grow their businesses. The Wealth segment includes Private Bank, Wealth at Work and Citigold and provides financial services to a range of client segments. USPB segment includes branded cards and retail services.</v>
     <v>227000</v>
@@ -5546,7 +5546,7 @@
     <v>101.52679999999999</v>
     <v>Investment Banking &amp; Investment Services</v>
     <v>Stock</v>
-    <v>45958.907661214842</v>
+    <v>45958.94136456016</v>
     <v>31</v>
     <v>100.13</v>
     <v>181417127000</v>
@@ -5556,11 +5556,11 @@
     <v>14.253</v>
     <v>100.99</v>
     <v>101.39</v>
-    <v>101.2563</v>
+    <v>101.45</v>
     <v>1789300000</v>
     <v>C</v>
     <v>CITIGROUP INC. (XNYS:C)</v>
-    <v>8754147</v>
+    <v>8759120</v>
     <v>13943431</v>
     <v>1988</v>
   </rv>
@@ -5588,8 +5588,8 @@
     <v>0.94769999999999999</v>
     <v>1.23</v>
     <v>1.7229000000000001E-2</v>
-    <v>-3.8800000000000001E-2</v>
-    <v>-5.3430000000000003E-4</v>
+    <v>-0.02</v>
+    <v>-2.7539999999999997E-4</v>
     <v>USD</v>
     <v>Cisco Systems, Inc. designs and sells a range of technologies that power the Internet. The Company is integrating its product portfolios across networking, security, collaboration, applications and cloud. The Company's segments include the Americas; Europe, Middle East, and Africa (EMEA), and Asia Pacific, Japan, and China (APJC). Its Networking product category represents its core networking technologies of switching, routing, wireless, fifth generation (5G), silicon, optics solutions and compute products. Its Security product category consists of its cloud and application security, industrial security, network security, and user and device security offerings. Its Collaboration product category consists of its meetings, collaboration devices, calling, contact center and platform as a service (CPaaS) offering. Its Observability product category consists of its full stack observability offerings.</v>
     <v>86200</v>
@@ -5600,7 +5600,7 @@
     <v>72.680000000000007</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45958.908908298436</v>
+    <v>45958.943276284372</v>
     <v>34</v>
     <v>71.03</v>
     <v>287081166140</v>
@@ -5610,11 +5610,11 @@
     <v>30.6996</v>
     <v>71.39</v>
     <v>72.62</v>
-    <v>72.581199999999995</v>
+    <v>72.599999999999994</v>
     <v>3953197000</v>
     <v>CSCO</v>
     <v>CISCO SYSTEMS, INC. (XNAS:CSCO)</v>
-    <v>19871185</v>
+    <v>19873218</v>
     <v>17271734</v>
     <v>2021</v>
   </rv>
@@ -5642,8 +5642,8 @@
     <v>0.61099999999999999</v>
     <v>-0.26</v>
     <v>-3.1530000000000004E-3</v>
-    <v>0.18</v>
-    <v>2.1900000000000001E-3</v>
+    <v>0.15010000000000001</v>
+    <v>1.8260000000000001E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company's segments include Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness and Corporate/Other. The Health Care Benefits segment offers a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, PDPs and Medicaid health care management services. The Health Services segment provides a full range of PBM solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services including pharmacy patient care programs, diagnostic testing and vaccination administration, and sells an assortment of health and wellness products and general merchandise.</v>
     <v>300000</v>
@@ -5654,7 +5654,7 @@
     <v>83.74</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45958.908717395316</v>
+    <v>45958.94380388828</v>
     <v>37</v>
     <v>81.61</v>
     <v>104243713940</v>
@@ -5664,11 +5664,11 @@
     <v>22.9376</v>
     <v>82.45</v>
     <v>82.19</v>
-    <v>82.38</v>
+    <v>82.350099999999998</v>
     <v>1268326000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>9831426</v>
+    <v>9841755</v>
     <v>6990736</v>
     <v>1996</v>
   </rv>
@@ -5696,8 +5696,8 @@
     <v>2.1855000000000002</v>
     <v>0.125</v>
     <v>4.0716999999999996E-2</v>
-    <v>0.01</v>
-    <v>3.1350000000000002E-3</v>
+    <v>-2.9899999999999999E-2</v>
+    <v>-9.3729999999999994E-3</v>
     <v>USD</v>
     <v>3D Systems Corporation provides comprehensive three-dimensional (3D) printing and digital manufacturing solutions, including 3D printers for plastics and metals, materials, software, and services, including maintenance, advanced manufacturing and applications engineering. The Company’s segments include Healthcare Solutions and Industrial Solutions. The Healthcare Solutions segment serves industry verticals, including dental, medical devices, personalized health services and regenerative medicine. The Industrial Solutions segment serves industry verticals, including aerospace, defense, transportation and general manufacturing. The Company architects solutions specific to customers’ needs through a combination of materials, hardware platforms, software, professional services and advanced manufacturing. It markets its products and services through subsidiaries in North America and South America, Europe and the Middle East and Asia Pacific and Oceania.</v>
     <v>1833</v>
@@ -5708,7 +5708,7 @@
     <v>3.4</v>
     <v>Electronic Equipment &amp; Parts</v>
     <v>Stock</v>
-    <v>45958.904932650003</v>
+    <v>45958.94197274297</v>
     <v>40</v>
     <v>3.04</v>
     <v>409767057</v>
@@ -5717,11 +5717,11 @@
     <v>3.24</v>
     <v>3.07</v>
     <v>3.1949999999999998</v>
-    <v>3.2</v>
+    <v>3.1600999999999999</v>
     <v>128252600</v>
     <v>DDD</v>
     <v>3D SYSTEMS CORPORATION (XNYS:DDD)</v>
-    <v>5964314</v>
+    <v>6002660</v>
     <v>5078937</v>
     <v>1993</v>
   </rv>
@@ -5769,8 +5769,8 @@
     <v>1.5483</v>
     <v>-0.67500000000000004</v>
     <v>-6.0089999999999996E-3</v>
-    <v>-0.1</v>
-    <v>-8.9569999999999993E-4</v>
+    <v>-0.05</v>
+    <v>-4.4779999999999999E-4</v>
     <v>USD</v>
     <v>The Walt Disney Company is a diversified worldwide entertainment company. The Company's segments include Entertainment, Sports and Experiences. The Entertainment segment generally encompasses its non-sports focused global film and episodic content production and distribution activities. The lines of business within the Entertainment segment along with their business activities include Linear Networks, Direct-to-Consumer, and Content Sales/Licensing. The Sports segment encompasses its sports-focused global television and direct-to-consumer (DTC) video streaming content production and distribution activities. The lines of business within the Sports segment include ESPN and Star. The Experiences segment includes Parks and Experiences and Consumer Products. Parks and Experiences consists of Walt Disney World Resort in Florida, Disneyland Resort in California, Disney Cruise Line, and others. Consumer Products includes licensing of its trade names, characters, visual, literary and other IP.</v>
     <v>233000</v>
@@ -5782,21 +5782,21 @@
     <v>46</v>
     <v>Media &amp; Publishing</v>
     <v>Stock</v>
-    <v>45958.909113911715</v>
+    <v>45958.940083390626</v>
     <v>47</v>
     <v>111.4623</v>
     <v>200766300110</v>
     <v>THE WALT DISNEY COMPANY</v>
     <v>THE WALT DISNEY COMPANY</v>
     <v>111.91</v>
-    <v>17.506699999999999</v>
+    <v>17.6127</v>
     <v>112.34</v>
     <v>111.66500000000001</v>
-    <v>111.55</v>
+    <v>111.6</v>
     <v>1797934000</v>
     <v>DIS</v>
     <v>THE WALT DISNEY COMPANY (XNYS:DIS)</v>
-    <v>6836444</v>
+    <v>6837700</v>
     <v>7852782</v>
     <v>2018</v>
   </rv>
@@ -5929,8 +5929,8 @@
     <v>1.1479999999999999</v>
     <v>-7.0000000000000007E-2</v>
     <v>-5.2119999999999996E-3</v>
-    <v>0.1</v>
-    <v>7.4850000000000003E-3</v>
+    <v>-0.1</v>
+    <v>-7.4850000000000003E-3</v>
     <v>USD</v>
     <v>DXC Technology Company is a global technology services provider. The Company helps global companies run their mission-critical systems and operations while modernizing information technology (IT), optimizing data architectures, and ensuring security and scalability across public, private and hybrid clouds. The Company’s segments include Global Business Services (GBS) and Global Infrastructure Services (GIS). The GBS segment provides technology solutions that help its customers address key business challenges and accelerate transformations tailored to each customer’s industry and specific objectives. GBS offerings include consulting and engineering services and insurance software and business process services. The GIS segment provides a portfolio of technology offerings that deliver predictable outcomes and measurable results while reducing business risk and operational costs for customers. GIS offerings include cloud IT outsourcing (ITO) and security and modern workplace.</v>
     <v>120000</v>
@@ -5941,21 +5941,21 @@
     <v>13.559100000000001</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.887189200781</v>
+    <v>45958.926149108593</v>
     <v>56</v>
     <v>13.27</v>
     <v>2391422632</v>
     <v>DXC TECHNOLOGY COMPANY</v>
     <v>DXC TECHNOLOGY COMPANY</v>
     <v>13.31</v>
-    <v>6.5233999999999996</v>
+    <v>6.5575999999999999</v>
     <v>13.43</v>
     <v>13.36</v>
-    <v>13.46</v>
+    <v>13.26</v>
     <v>178998700</v>
     <v>DXC</v>
     <v>DXC TECHNOLOGY COMPANY (XNYS:DXC)</v>
-    <v>2201982</v>
+    <v>2201983</v>
     <v>1714625</v>
     <v>2017</v>
   </rv>
@@ -6085,8 +6085,8 @@
     <v>1.4171</v>
     <v>0.49</v>
     <v>7.0630000000000007E-3</v>
-    <v>-0.08</v>
-    <v>-1.145E-3</v>
+    <v>2.8799999999999999E-2</v>
+    <v>4.1219999999999999E-4</v>
     <v>USD</v>
     <v>General Motors Company designs, builds and sells trucks, crossovers, cars and automobile parts and provides software-enabled services and subscriptions worldwide. The Company's segments include GMNA, GMI, Cruise and GM Financial. Its GM North America (GMNA) and GM International (GMI) develop, manufacture and/or markets vehicles under the Buick, Cadillac, Chevrolet and GMC brands. The Company provides automotive financing services through its General Motors Financial Company, Inc. (GM Financial) segment. Its Cruise segment is engaged in the development and commercialization of autonomous vehicle technology. Its software-enabled services and subscriptions, including OnStar, its advanced driver-assistance systems (ADAS), including Super Cruise driver assistance technology, and its end-to-end software platform. The Company is also focused on investing in electric vehicles (EVs) and AVs, software-enabled services and subscriptions and new business opportunities.</v>
     <v>162000</v>
@@ -6097,21 +6097,21 @@
     <v>70.19</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45958.900397753903</v>
+    <v>45958.941027372653</v>
     <v>65</v>
     <v>68.66</v>
     <v>65179019031</v>
     <v>GENERAL MOTORS COMPANY</v>
     <v>GENERAL MOTORS COMPANY</v>
     <v>69.459999999999994</v>
-    <v>13.438599999999999</v>
+    <v>13.3444</v>
     <v>69.38</v>
     <v>69.87</v>
-    <v>69.790000000000006</v>
+    <v>69.898799999999994</v>
     <v>932861300</v>
     <v>GM</v>
     <v>GENERAL MOTORS COMPANY (XNYS:GM)</v>
-    <v>13069583</v>
+    <v>13070283</v>
     <v>10365613</v>
     <v>2009</v>
   </rv>
@@ -6139,8 +6139,8 @@
     <v>1.4371</v>
     <v>0.09</v>
     <v>3.7219999999999996E-3</v>
-    <v>0.04</v>
-    <v>1.6489999999999999E-3</v>
+    <v>0.05</v>
+    <v>2.062E-3</v>
     <v>USD</v>
     <v>Hewlett Packard Enterprise Company is the global edge-to-cloud company. It delivers open and intelligent technology solutions as a service. Its offering includes cloud services, compute, high performance computing &amp; artificial intelligence, intelligent edge, software, and storage. Its segments include Server, Hybrid Cloud, Intelligent Edge, Financial Services, and Corporate Investments and Other. Its Server segment offerings consist of general-purpose servers for multi-workload computing, workload-optimized servers, and integrated systems. Its Hybrid Cloud segment offers a range of cloud-native and hybrid solutions across storage, private cloud and the infrastructure software-as-a-service space. Its Intelligent Edge segment offers wired and wireless local area networks, campus, branch, and data center switching, and others. Its Financial Services segment provides flexible investment solutions, such as leasing, financing, IT consumption, utility programs, and asset management services.</v>
     <v>61000</v>
@@ -6151,7 +6151,7 @@
     <v>24.697500000000002</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45958.90992578672</v>
+    <v>45958.94344538125</v>
     <v>68</v>
     <v>23.69</v>
     <v>32023051500</v>
@@ -6161,11 +6161,11 @@
     <v>29.1112</v>
     <v>24.18</v>
     <v>24.27</v>
-    <v>24.29</v>
+    <v>24.3</v>
     <v>1319450000</v>
     <v>HPE</v>
     <v>HEWLETT PACKARD ENTERPRISE COMPANY (XNYS:HPE)</v>
-    <v>38276997</v>
+    <v>38281692</v>
     <v>35125390</v>
     <v>2015</v>
   </rv>
@@ -6198,7 +6198,7 @@
     <v>16</v>
     <v>17</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-US</v>
     <v>a1uu5r</v>
     <v>268435456</v>
@@ -6207,10 +6207,10 @@
     <v>39.795000000000002</v>
     <v>21.21</v>
     <v>1.2952999999999999</v>
-    <v>0.15</v>
-    <v>5.372E-3</v>
-    <v>-0.12</v>
-    <v>-4.2750000000000002E-3</v>
+    <v>0.14499999999999999</v>
+    <v>5.1929999999999997E-3</v>
+    <v>0.12</v>
+    <v>4.2750000000000002E-3</v>
     <v>USD</v>
     <v>HP Inc. is a global provider of personal computing and other digital access devices, imaging and printing products, and related technologies, solutions, and services. The Company delivers a range of devices, services and subscriptions for personal computing, printing, three-dimensional (3D) printing, hybrid work, gaming, and more. It operates through three segments: Personal Systems, Printing and Corporate Investments. The Personal Systems segment offers commercial and consumer desktops and notebooks, detachables and convertibles, workstations, thin clients, commercial mobility devices, retail point-of-sale (POS) systems, displays, hybrid systems, software, solutions, and services. Printing segment offers consumer and commercial printer hardware, supplies, services, and solutions. Printing segment is also focused on graphics and 3D printing and personalization in the commercial and industrial markets. Corporate Investments include certain business incubation and investment projects.</v>
     <v>58000</v>
@@ -6222,21 +6222,21 @@
     <v>73</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45958.899425647658</v>
+    <v>45958.94359293906</v>
     <v>74</v>
     <v>27.513000000000002</v>
-    <v>26237079526</v>
+    <v>26232406017</v>
     <v>HP INC.</v>
     <v>HP INC.</v>
     <v>27.8</v>
-    <v>10.2255</v>
+    <v>10.170999999999999</v>
     <v>27.92</v>
-    <v>28.07</v>
-    <v>27.95</v>
+    <v>28.065000000000001</v>
+    <v>28.19</v>
     <v>934701800</v>
     <v>HPQ</v>
     <v>HP INC. (XNYS:HPQ)</v>
-    <v>7420499</v>
+    <v>7421042</v>
     <v>12115691</v>
     <v>1998</v>
   </rv>
@@ -6315,8 +6315,8 @@
     <v>0.55100000000000005</v>
     <v>-0.34</v>
     <v>-4.9979999999999998E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.21</v>
+    <v>3.1019999999999997E-3</v>
     <v>USD</v>
     <v>The Kroger Co. is a food and drug retailer. The Company operates supermarkets, multi-department stores and fulfillment centers throughout the United States. It operates approximately 2,731 supermarkets, 2,273 pharmacies and 1,702 fuel centers in over 35 states and the District of Columbia while also operating online through a digital ecosystem to offer customers an omnichannel shopping experience. The Company also manufactures and processes food for sale in its supermarkets and online. It offers Pickup and Harris Teeter ExpressLane personalized, order online, pick-up at the store services at approximately 2,412 of its supermarkets and provides delivery, which allows it to offer digital solutions to substantially all of its customers. Its delivery solutions include orders delivered to customers at retail store locations, customer fulfillment centers and orders placed through third-party platforms. The Company also offers customer-facing apps and interfaces.</v>
     <v>409000</v>
@@ -6327,7 +6327,7 @@
     <v>68.23</v>
     <v>Food &amp; Drug Retailing</v>
     <v>Stock</v>
-    <v>45958.898698969533</v>
+    <v>45958.932910844531</v>
     <v>80</v>
     <v>67.38</v>
     <v>44856687358</v>
@@ -6337,11 +6337,11 @@
     <v>17.148900000000001</v>
     <v>68.03</v>
     <v>67.69</v>
-    <v>67.69</v>
+    <v>67.900000000000006</v>
     <v>662678200</v>
     <v>KR</v>
     <v>THE KROGER CO. (XNYS:KR)</v>
-    <v>4366255</v>
+    <v>4366732</v>
     <v>6120650</v>
     <v>1902</v>
   </rv>
@@ -6423,8 +6423,8 @@
     <v>1.4581</v>
     <v>0.70499999999999996</v>
     <v>7.5320999999999999E-2</v>
-    <v>0.31990000000000002</v>
-    <v>3.1830999999999998E-2</v>
+    <v>0.32</v>
+    <v>3.1841000000000001E-2</v>
     <v>USD</v>
     <v>Lumen Technologies, Inc. is a networking company, which connects people, data, and applications quickly and securely. The Company is engaged in providing an array of integrated products and services to its domestic and global business customers and its domestic mass market customers. It operates through two segments: Business segment and Mass Markets segment. The Company conducts its operations under four brands: Lumen, which is its flagship brand for serving the enterprise and wholesale markets, including its Private Connectivity Fabric (PCF) network architecture, Lumen Digital products, and its priority services including Edge, Network-as-a-Service and cybersecurity; Quantum Fiber, which provides fiber-based broadband services to residential and small business customers; CenturyLink, which is engaged in providing primarily mass-marketed copper-based communications services, and Black Lotus Labs, which is its cyberthreat research and intelligence arm.</v>
     <v>24000</v>
@@ -6435,7 +6435,7 @@
     <v>10.1</v>
     <v>Telecommunications Services</v>
     <v>Stock</v>
-    <v>45958.909650671092</v>
+    <v>45958.943745995311</v>
     <v>86</v>
     <v>9.25</v>
     <v>10328109165</v>
@@ -6444,11 +6444,11 @@
     <v>9.3800000000000008</v>
     <v>9.36</v>
     <v>10.065</v>
-    <v>10.369899999999999</v>
+    <v>10.37</v>
     <v>1026141000</v>
     <v>LUMN</v>
     <v>LUMEN TECHNOLOGIES, INC. (XNYS:LUMN)</v>
-    <v>44204753</v>
+    <v>44297742</v>
     <v>14902618</v>
     <v>1968</v>
   </rv>
@@ -6476,8 +6476,8 @@
     <v>2.0148999999999999</v>
     <v>-1.31</v>
     <v>-4.9137000000000007E-2</v>
-    <v>0.13</v>
-    <v>5.1280000000000006E-3</v>
+    <v>0.11</v>
+    <v>4.339E-3</v>
     <v>USD</v>
     <v>Moderna, Inc. is a biotechnology company. The Company is advancing a new class of medicines made of messenger ribonucleic acid (mRNA). It is developing therapeutics and vaccines for infectious diseases, immuno-oncology, rare diseases and autoimmune diseases. mRNA medicines are designed to direct the body’s cells to produce intracellular, membrane or secreted proteins that have a therapeutic or preventive benefit with the potential to address a spectrum of diseases. The Company’s diverse development pipeline consists of 44 therapeutic and vaccine programs, 11 of which are in late-stage development. Its commercial products include Spikevax (its COVID vaccine) and mRESVIA (its respiratory syncytial virus (RSV) vaccine). Additionally, it has achieved four positive Phase III data readouts for its COVID vaccine (mRNA-1283), its RSV vaccine for high-risk adults aged 18 to 59 (mRNA-1345), its seasonal flu+COVID vaccine (mRNA-1083), and its seasonal flu vaccine (mRNA-1010).</v>
     <v>5800</v>
@@ -6488,7 +6488,7 @@
     <v>26.9</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45958.909992337503</v>
+    <v>45958.943806099218</v>
     <v>89</v>
     <v>25.2</v>
     <v>10412880000</v>
@@ -6498,11 +6498,11 @@
     <v>0</v>
     <v>26.66</v>
     <v>25.35</v>
-    <v>25.48</v>
+    <v>25.46</v>
     <v>390580800</v>
     <v>MRNA</v>
     <v>MODERNA, INC. (XNAS:MRNA)</v>
-    <v>8795295</v>
+    <v>8806254</v>
     <v>8988701</v>
     <v>2016</v>
   </rv>
@@ -6546,8 +6546,8 @@
     <v>1.0184</v>
     <v>10.55</v>
     <v>1.9849000000000002E-2</v>
-    <v>1.7857000000000001</v>
-    <v>3.2940000000000001E-3</v>
+    <v>2.0699999999999998</v>
+    <v>3.8190000000000003E-3</v>
     <v>USD</v>
     <v>Microsoft Corporation is a technology company. The Company develops and supports software, services, devices, and solutions. The Company’s segments include Productivity and Business Processes, Intelligent Cloud, and More Personal Computing. The Productivity and Business Processes segment consists of products and services in its portfolio of productivity, communication, and information services. This segment primarily comprises: Office Commercial, Office Consumer, LinkedIn, and Dynamics business solutions. The Intelligent Cloud segment consists of server products and cloud services, including Azure and other cloud services, SQL Server, Windows Server, Visual Studio, System Center, and related Client Access Licenses (CALs), and Nuance and GitHub; and Enterprise Services, including enterprise support services, industry solutions and Nuance professional services. The More Personal Computing segment primarily comprises Windows, Devices, Gaming, and search and news advertising.</v>
     <v>228000</v>
@@ -6559,7 +6559,7 @@
     <v>94</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.910000555472</v>
+    <v>45958.943671145309</v>
     <v>95</v>
     <v>540.77</v>
     <v>4029253470090</v>
@@ -6569,11 +6569,11 @@
     <v>38.964700000000001</v>
     <v>531.52</v>
     <v>542.07000000000005</v>
-    <v>543.85569999999996</v>
+    <v>544.14</v>
     <v>7433087000</v>
     <v>MSFT</v>
     <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
-    <v>29888043</v>
+    <v>29922694</v>
     <v>17203470</v>
     <v>1993</v>
   </rv>
@@ -6601,8 +6601,8 @@
     <v>0.69359999999999999</v>
     <v>-2.48</v>
     <v>-2.8826999999999998E-2</v>
-    <v>-0.02</v>
-    <v>-2.3929999999999999E-4</v>
+    <v>0.11</v>
+    <v>1.3159999999999999E-3</v>
     <v>USD</v>
     <v>NextEra Energy, Inc. is an electric power and energy infrastructure company. It operates through its wholly owned subsidiaries, NextEra Energy Resources, LLC and NextEra Energy Transmission, LLC (collectively, NEER) and Florida Power &amp; Light Company (FPL). Its segments include NEER and FPL. FPL segment is a rate-regulated electric utility engaged in the generation, transmission, distribution and sale of electric energy in Florida. FPL has approximately 35,052 megawatts of net generating capacity, over 91,000 circuit miles of transmission and distribution lines and 921 substations. The NEER segment owns, develops, constructs, manages and operates electric generation facilities in wholesale energy markets in the United States and Canada and includes assets and investments in other businesses with a clean energy focus, such as battery storage, natural gas pipelines, and renewable fuels. It owns, develops, constructs and operates rate-regulated transmission facilities in North America.</v>
     <v>16800</v>
@@ -6613,7 +6613,7 @@
     <v>87.53</v>
     <v>Electrical Utilities &amp; IPPs</v>
     <v>Stock</v>
-    <v>45958.909818402346</v>
+    <v>45958.942795242969</v>
     <v>98</v>
     <v>82.91</v>
     <v>172053846600</v>
@@ -6623,11 +6623,11 @@
     <v>31.247699999999998</v>
     <v>86.03</v>
     <v>83.55</v>
-    <v>83.55</v>
+    <v>83.68</v>
     <v>2059292000</v>
     <v>NEE</v>
     <v>NEXTERA ENERGY, INC. (XNYS:NEE)</v>
-    <v>13988213</v>
+    <v>13992118</v>
     <v>10251883</v>
     <v>1984</v>
   </rv>
@@ -6655,8 +6655,8 @@
     <v>0.34449999999999997</v>
     <v>0.7</v>
     <v>8.9020000000000002E-3</v>
-    <v>-0.21099999999999999</v>
-    <v>-2.6590000000000003E-3</v>
+    <v>-0.35</v>
+    <v>-4.411E-3</v>
     <v>USD</v>
     <v>Newmont Corporation is a gold company and a producer of copper, zinc, lead, and silver with operations and/or assets in the Africa, Australia, Latin America &amp; Caribbean, North America, and Papua New Guinea regions. The Company's operations include Brucejack, Red Chris, Penasquito, Merian, Cerro Negro, Yanacocha, Boddington, Tanami, Cadia, Lihir, Ahafo, and NGM. The Brucejack operation includes four mining leases and six core mineral claims which cover 8,169 acres (3,306 hectares) and 337 mineral claims covering 298,795 acres (120,918 hectares). The Red Chris operation includes five mining leases which cover 12,703 acres and 199 mineral claims, encompassing an area of 164,903 acres (66,734 hectares). Penasquito includes 20 mining concessions for operations comprising 113,231 acres (45,823 hectares) and 60 mining concessions for exploration of 107,456 acres (43,486 hectares). The Merian operation includes one right of exploitation encompassing an area of 41,687 acres (16,870 hectares).</v>
     <v>22200</v>
@@ -6667,21 +6667,21 @@
     <v>79.86</v>
     <v>Metals &amp; Mining</v>
     <v>Stock</v>
-    <v>45958.908327580466</v>
+    <v>45958.943397615622</v>
     <v>101</v>
     <v>76.046800000000005</v>
     <v>86569893790</v>
     <v>NEWMONT CORPORATION</v>
     <v>NEWMONT CORPORATION</v>
     <v>76.739999999999995</v>
-    <v>12.3279</v>
+    <v>12.218999999999999</v>
     <v>78.63</v>
     <v>79.33</v>
-    <v>79.129000000000005</v>
+    <v>78.989999999999995</v>
     <v>1091263000</v>
     <v>NEM</v>
     <v>NEWMONT CORPORATION (XNYS:NEM)</v>
-    <v>13301476</v>
+    <v>13324419</v>
     <v>12647951</v>
     <v>2001</v>
   </rv>
@@ -6709,8 +6709,8 @@
     <v>1.5746</v>
     <v>7.94</v>
     <v>7.254E-3</v>
-    <v>-0.52470000000000006</v>
-    <v>-4.7590000000000002E-4</v>
+    <v>-0.51</v>
+    <v>-4.6260000000000002E-4</v>
     <v>USD</v>
     <v>Netflix, Inc. is a provider of entertainment services. The Company acquires, licenses and produces content, including original programming. It provides paid memberships in over 190 countries offering television (TV) series, films and games across a variety of genres and languages. It allows members to play, pause and resume watching as much as they want, anytime, anywhere, and can change their plans at any time. The Company offers members the ability to receive streaming content through a host of Internet-connected devices, including TVs, digital video players, TV set-top boxes and mobile devices. It is engaged in scaling its streaming service, such as introducing games and advertising on its service, as well as offering live programming. It is developing technology and utilizing third-party cloud computing, technology and other services. The Company is also engaged in scaling its own studio operations to produce original content.</v>
     <v>14000</v>
@@ -6721,21 +6721,21 @@
     <v>1116.9799</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.910047198435</v>
+    <v>45958.943193796091</v>
     <v>104</v>
     <v>1093.0083</v>
     <v>467164860750</v>
     <v>NETFLIX, INC.</v>
     <v>NETFLIX, INC.</v>
     <v>1094</v>
-    <v>46.056899999999999</v>
+    <v>45.725099999999998</v>
     <v>1094.56</v>
     <v>1102.5</v>
-    <v>1101.9753000000001</v>
+    <v>1101.99</v>
     <v>423732300</v>
     <v>NFLX</v>
     <v>NETFLIX, INC. (XNAS:NFLX)</v>
-    <v>4011831</v>
+    <v>4015473</v>
     <v>3989398</v>
     <v>1997</v>
   </rv>
@@ -6775,7 +6775,7 @@
     <v>4.3827999999999996</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.905736041408</v>
+    <v>45958.941056053125</v>
     <v>107</v>
     <v>4.09</v>
     <v>59334512</v>
@@ -6788,7 +6788,7 @@
     <v>14366710</v>
     <v>NOTE</v>
     <v>FISCALNOTE HOLDINGS, INC. (XNYS:NOTE)</v>
-    <v>166174</v>
+    <v>167009</v>
     <v>249748</v>
     <v>2022</v>
   </rv>
@@ -6816,8 +6816,8 @@
     <v>0.9022</v>
     <v>0.51</v>
     <v>1.4684999999999998E-2</v>
-    <v>-0.01</v>
-    <v>-2.8380000000000001E-4</v>
+    <v>-0.09</v>
+    <v>-2.5540000000000003E-3</v>
     <v>USD</v>
     <v>Pan American Silver Corp. is a producer of silver and gold in the Americas, operating mines in Canada, Mexico, Peru, Brazil, Bolivia, Chile and Argentina. It owns a 100% interest in the Escobal mine in Guatemala, and it holds interests in exploration and development projects. Its segments include Silver, Gold and Other. Silver segment includes operations of La Colorada, Huaron, San Vicente, Cerro Moro, La Colorada Skarn, Navidad and Escobal. Gold segment includes operations in Dolores, Shahuindo, Timmins, Jacobina, El Penon and Minera Florida. La Colorada mine produces silver-rich lead and zinc concentrates from a flotation plant treating sulfide ore. Huaron mine produces silver-rich zinc, lead and copper concentrates using floatation technology. It owns 44% joint venture interest in the Juanicipio silver mine in Zacatecas, Mexico, operated by Fresnillo plc, along with 100% ownership of the Larder exploration project and a 100% earn-in interest in the Deer Trail exploration project.</v>
     <v>9000</v>
@@ -6828,7 +6828,7 @@
     <v>35.25</v>
     <v>Metals &amp; Mining</v>
     <v>Stock</v>
-    <v>45958.909128020314</v>
+    <v>45958.941953633592</v>
     <v>110</v>
     <v>33.9</v>
     <v>20503810000</v>
@@ -6838,11 +6838,11 @@
     <v>24.112400000000001</v>
     <v>34.729999999999997</v>
     <v>35.24</v>
-    <v>35.229999999999997</v>
+    <v>35.15</v>
     <v>421976000</v>
     <v>PAAS</v>
     <v>Pan American Silver Corp. (XNYS:PAAS)</v>
-    <v>4950764</v>
+    <v>4955807</v>
     <v>6641142</v>
     <v>1979</v>
   </rv>
@@ -6936,7 +6936,7 @@
     <v>7.58</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45958.909776029686</v>
+    <v>45958.942199074074</v>
     <v>116</v>
     <v>7.02</v>
     <v>737922766</v>
@@ -6950,7 +6950,7 @@
     <v>104373800</v>
     <v>POET</v>
     <v>POET Technologies Inc. (XNAS:POET)</v>
-    <v>11982812</v>
+    <v>12042192</v>
     <v>16032623</v>
     <v>2010</v>
   </rv>
@@ -7146,7 +7146,7 @@
     <v>235.05</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.8125</v>
+    <v>45958.929780092592</v>
     <v>128</v>
     <v>232.75</v>
     <v>289374200000</v>
@@ -7241,8 +7241,8 @@
     <v>1.6188</v>
     <v>-0.38</v>
     <v>-3.1905999999999997E-2</v>
-    <v>-0.01</v>
-    <v>-8.6729999999999999E-4</v>
+    <v>-0.02</v>
+    <v>-1.7349999999999998E-3</v>
     <v>USD</v>
     <v>Stratasys Ltd. provides polymer-based 3D printing solutions for industries such as aerospace, automotive, consumer products and healthcare. The Company's solutions consist of 3D printing systems, consumables, software, paid parts, and professional services and encompass everything from prototyping and design all the way through production. Its printers include F3300, FDM Fortus 450mc, PolyJet J3 DentaJet, P3 DLP Origin One Dental, SLA Neo, PolyJet J5 Digital Anatomy, and Powder Bed Fusion SAF H350. The Company's technologies include FDM Technology, PolyJet Technology, P3 DLP Technology, SAF Technology, Stereolithography Technology and 3DFashion Technology. Its FDM 3D printing technology has the ability to use a variety of production grade thermoplastic materials featuring surface resolution, chemical and heat resistance, color, and mechanical properties necessary for production of functional prototypes and parts for a variety of industries with specific demands and requirements.</v>
     <v>1779</v>
@@ -7253,7 +7253,7 @@
     <v>12.01</v>
     <v>Electronic Equipment &amp; Parts</v>
     <v>Stock</v>
-    <v>45958.907723460157</v>
+    <v>45958.942481747654</v>
     <v>134</v>
     <v>11.5273</v>
     <v>981125518</v>
@@ -7263,11 +7263,11 @@
     <v>0</v>
     <v>11.91</v>
     <v>11.53</v>
-    <v>11.52</v>
+    <v>11.51</v>
     <v>85093280</v>
     <v>SSYS</v>
     <v>STRATASYS LTD (XNAS:SSYS)</v>
-    <v>768463</v>
+    <v>769725</v>
     <v>1133226</v>
     <v>1998</v>
   </rv>
@@ -7295,8 +7295,8 @@
     <v>2.0646</v>
     <v>8.1300000000000008</v>
     <v>1.797E-2</v>
-    <v>-0.54</v>
-    <v>-1.173E-3</v>
+    <v>-0.87</v>
+    <v>-1.8890000000000001E-3</v>
     <v>USD</v>
     <v>Tesla, Inc. designs, develops, manufactures, sells and leases high-performance fully electric vehicles and energy generation and storage systems, and offers services related to its products. Its segments include automotive, and energy generation and storage. The automotive segment includes the design, development, manufacturing, sales and leasing of high-performance fully electric vehicles, and sales of automotive regulatory credits. It also includes sales of used vehicles, non-warranty maintenance services and collisions, part sales, paid supercharging, insurance services revenue and retail merchandise sales. The energy generation and storage segment include the design, manufacture, installation, sales and leasing of solar energy generation and energy storage products and related services and sales of solar energy systems incentives. Its consumer vehicles include the Model 3, Y, S, X and Cybertruck. Its lithium-ion battery energy storage products include Powerwall and Megapack.</v>
     <v>125665</v>
@@ -7307,7 +7307,7 @@
     <v>467</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45958.910039560156</v>
+    <v>45958.943851689066</v>
     <v>137</v>
     <v>451.6</v>
     <v>1531705940450</v>
@@ -7317,11 +7317,11 @@
     <v>319.31639999999999</v>
     <v>452.42</v>
     <v>460.55</v>
-    <v>460.01</v>
+    <v>459.68</v>
     <v>3325819000</v>
     <v>TSLA</v>
     <v>TESLA, INC. (XNAS:TSLA)</v>
-    <v>79864797</v>
+    <v>79959008</v>
     <v>90284890</v>
     <v>2024</v>
   </rv>
@@ -7349,8 +7349,8 @@
     <v>1.3134999999999999</v>
     <v>3.27</v>
     <v>1.0964E-2</v>
-    <v>0.77</v>
-    <v>2.5540000000000003E-3</v>
+    <v>0.17</v>
+    <v>5.6380000000000004E-4</v>
     <v>USD</v>
     <v>Taiwan Semiconductor Manufacturing Co Ltd is a Taiwan-based company mainly engaged in the provision of integrated circuit manufacturing services. The integrated circuit manufacturing services include process technology, special process technology, design ecosystem support, mask technology, 3DFabricTM advanced packaging and silicon stacking technology services. The Company has completed the transfer and mass production of 5nm technology, and is engaged in the research and development of 3nm process technology and 2nm process technology. The product application range covers the entire electronic application industry, including personal computers and peripheral products, information application products, wired and wireless communication system products, servers and data centers.</v>
     <v>52045</v>
@@ -7361,7 +7361,7 @@
     <v>302.13</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45958.909872395314</v>
+    <v>45958.943793957813</v>
     <v>140</v>
     <v>296.08</v>
     <v>1244779000000</v>
@@ -7371,11 +7371,11 @@
     <v>29.677900000000001</v>
     <v>298.25</v>
     <v>301.52</v>
-    <v>302.3</v>
+    <v>301.7</v>
     <v>5186523000</v>
     <v>TSM</v>
     <v>Taiwan Semiconductor Manufacturing Co., Ltd. (XNYS:TSM)</v>
-    <v>11750610</v>
+    <v>11766814</v>
     <v>14075572</v>
     <v>1987</v>
   </rv>
@@ -7618,7 +7618,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1y7rw</v>
     <v>268435456</v>
@@ -7629,8 +7629,8 @@
     <v>0.90059999999999996</v>
     <v>-0.13</v>
     <v>-1.2476000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>6.4000000000000001E-2</v>
+    <v>6.2199999999999998E-3</v>
     <v>USD</v>
     <v>Viatris Inc. is a global healthcare company. The Company's segments include Developed Markets, Greater China, JANZ, and Emerging Markets. The Developed Markets segment comprises its operations primarily in North America and Europe. The Greater China segment includes its operations in China, Taiwan and Hong Kong. The JANZ segment reflects its operations in Japan, Australia, and New Zealand. The Emerging Markets segment encompasses its presence in more than 125 countries with developing markets and emerging economies, including in Asia, Africa, Eastern Europe, Latin America, and the Middle East, as well as the Company’s Antiretroviral medicines (ARV) franchise. Its pipeline and research and development capabilities include expertise in formulation, device development, toxicology, analytical, clinical, bioanalytical, medical affairs, product safety and risk management across a range of therapeutic areas. It produces oral solid doses, injectables, and products with complex dosage forms.</v>
     <v>32000</v>
@@ -7641,7 +7641,7 @@
     <v>10.46</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45958.90942290469</v>
+    <v>45958.925457928126</v>
     <v>158</v>
     <v>10.27</v>
     <v>12051610000</v>
@@ -7651,11 +7651,11 @@
     <v>0</v>
     <v>10.42</v>
     <v>10.29</v>
-    <v>10.29</v>
+    <v>10.353999999999999</v>
     <v>1156585000</v>
     <v>VTRS</v>
     <v>VIATRIS INC. (XNAS:VTRS)</v>
-    <v>7206114</v>
+    <v>7206296</v>
     <v>7204986</v>
     <v>2019</v>
   </rv>
@@ -7734,8 +7734,8 @@
     <v>0.4657</v>
     <v>-0.9</v>
     <v>-7.7629999999999999E-3</v>
-    <v>0.11</v>
-    <v>9.563000000000001E-4</v>
+    <v>0.06</v>
+    <v>5.2159999999999999E-4</v>
     <v>USD</v>
     <v>Exxon Mobil Corporation is an energy provider and chemical manufacturer. The Company’s principal business involves exploration for, and production of, crude oil and natural gas; the manufacture, trade, transport and sale of crude oil, natural gas, petroleum products, petrochemicals and a wide variety of specialty products; and pursuit of lower-emission and other new business opportunities, including carbon capture and storage, hydrogen, lower-emission fuels, Proxxima systems, carbon materials, and lithium. Its Upstream segment explores for and produces crude oil and natural gas. The Energy Products, Chemical Products, and Specialty Products segments manufacture and sell petroleum products and petrochemicals. Energy Products segment includes fuels, aromatics, and catalysts and licensing. Chemical Products segment consists of olefins, polyolefins, and intermediates. Specialty Products segment includes finished lubricants, basestocks and waxes, synthetics, and elastomers and resins.</v>
     <v>61000</v>
@@ -7746,7 +7746,7 @@
     <v>116.18</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45958.908892303123</v>
+    <v>45958.941021376566</v>
     <v>164</v>
     <v>114.99</v>
     <v>490443934880</v>
@@ -7756,11 +7756,11 @@
     <v>16.323499999999999</v>
     <v>115.94</v>
     <v>115.04</v>
-    <v>115.14</v>
+    <v>115.09</v>
     <v>4263247000</v>
     <v>XOM</v>
     <v>EXXON MOBIL CORPORATION (XNYS:XOM)</v>
-    <v>9526062</v>
+    <v>9526590</v>
     <v>13644757</v>
     <v>1882</v>
   </rv>
@@ -7987,8 +7987,8 @@
     <v>3.5066000000000002</v>
     <v>-0.1</v>
     <v>-5.4945000000000001E-2</v>
-    <v>0.01</v>
-    <v>5.8140000000000006E-3</v>
+    <v>1E-4</v>
+    <v>5.8139999999999996E-5</v>
     <v>USD</v>
     <v>Blink Charging Co., through its wholly owned subsidiaries, is a manufacturer, owner, operator and provider of electric vehicle (EV) charging equipment and networked EV charging services. It offers residential and commercial EV charging equipment and services, enabling EV drivers to recharge at various location types. Its principal line of products and services is its nationwide Blink EV charging networks (the Blink Networks) and Blink EV charging equipment, also known as electric vehicle supply equipment (EVSE), and other EV-related services. The Blink Networks is a proprietary, cloud-based system that operates, maintains and manages Blink charging stations and handles the associated charging data, back-end operations and payment processing. The Blink Networks provide property owners, managers, parking companies, state and municipal entities, and other types of commercial customers with cloud-based services that enable the remote monitoring and management of EV charging stations.</v>
     <v>542</v>
@@ -7999,7 +7999,7 @@
     <v>1.86</v>
     <v>Electrical Utilities &amp; IPPs</v>
     <v>Stock</v>
-    <v>45958.908117753905</v>
+    <v>45958.940159478909</v>
     <v>178</v>
     <v>1.72</v>
     <v>180108596</v>
@@ -8009,11 +8009,11 @@
     <v>0</v>
     <v>1.82</v>
     <v>1.72</v>
-    <v>1.73</v>
+    <v>1.7201</v>
     <v>104714300</v>
     <v>BLNK</v>
     <v>BLINK CHARGING CO. (XNAS:BLNK)</v>
-    <v>3360064</v>
+    <v>3391431</v>
     <v>6418809</v>
     <v>2006</v>
   </rv>
@@ -8108,8 +8108,8 @@
     <v>1.6107</v>
     <v>-0.125</v>
     <v>-9.4269999999999996E-3</v>
-    <v>-0.01</v>
-    <v>-7.6160000000000008E-4</v>
+    <v>-0.02</v>
+    <v>-1.5229999999999998E-3</v>
     <v>USD</v>
     <v>Ford Motor Company is an automobile company. The Company develops and delivers Ford trucks, sport utility vehicles, commercial vans and cars, and Lincoln luxury vehicles, along with connected services. The Company’s segments include Ford Blue, Ford Model e, Ford Pro, and Ford Credit. The Ford Blue segment primarily includes the sale of Ford and Lincoln internal combustion engine (ICE) and hybrid vehicles, service parts, accessories, and digital services for retail customers. The Ford Model e segment primarily includes the sale of its electric vehicles, service parts, accessories, and digital services for retail customers. The Ford Pro segment primarily includes the sale of Ford and Lincoln vehicles, service parts, accessories, and services for commercial, government, and rental customers. The Ford Credit segment consists of the Ford Credit business on a consolidated basis, which is primarily vehicle-related financing and leasing activities. Its vehicle brands are Ford and Lincoln.</v>
     <v>171000</v>
@@ -8121,7 +8121,7 @@
     <v>186</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45958.909672256254</v>
+    <v>45958.943636180469</v>
     <v>187</v>
     <v>13.04</v>
     <v>52336394365</v>
@@ -8131,11 +8131,11 @@
     <v>11.279500000000001</v>
     <v>13.26</v>
     <v>13.135</v>
-    <v>13.12</v>
+    <v>13.11</v>
     <v>3984499000</v>
     <v>F</v>
     <v>FORD MOTOR COMPANY (XNYS:F)</v>
-    <v>96684145</v>
+    <v>96698107</v>
     <v>134400438</v>
     <v>1919</v>
   </rv>
@@ -8163,8 +8163,8 @@
     <v>1.7033</v>
     <v>-0.27</v>
     <v>-1.418E-3</v>
-    <v>0.8</v>
-    <v>4.2069999999999998E-3</v>
+    <v>1.85</v>
+    <v>9.7289999999999998E-3</v>
     <v>USD</v>
     <v>Generac Holdings Inc. is a global designer, manufacturer, and provider of energy technology solutions. The Company provides power generation equipment, energy storage systems, energy management devices &amp; solutions, and other power products serving the residential, light commercial, and industrial markets. The Company operates through two segments: Domestic and International. The Domestic segment includes the legacy Generac business and the acquisitions that are based in the United States and Canada. The International segment includes acquisitions not based in the United States and Canada. It designs and manufactures stationary, portable, and mobile power generators with single-engine outputs ranging between 800W and 3,250kW. Its residential automatic standby generators range in output from 7.5kW to 150kW, which predominantly operate on natural gas and liquid propane, and are permanently installed with an automatic transfer switch.</v>
     <v>9239</v>
@@ -8175,7 +8175,7 @@
     <v>191.505</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45958.909938946097</v>
+    <v>45958.943650161717</v>
     <v>190</v>
     <v>187.19</v>
     <v>11156645133</v>
@@ -8185,11 +8185,11 @@
     <v>31.5732</v>
     <v>190.41</v>
     <v>190.14</v>
-    <v>190.95</v>
+    <v>192</v>
     <v>58675950</v>
     <v>GNRC</v>
     <v>GENERAC HOLDINGS INC. (XNYS:GNRC)</v>
-    <v>1580869</v>
+    <v>1581906</v>
     <v>1032758</v>
     <v>2006</v>
   </rv>
@@ -8217,8 +8217,8 @@
     <v>1.3987000000000001</v>
     <v>2.29</v>
     <v>2.8990000000000001E-3</v>
-    <v>-1.65</v>
-    <v>-2.0830000000000002E-3</v>
+    <v>-1.03</v>
+    <v>-1.2999999999999999E-3</v>
     <v>USD</v>
     <v>The Goldman Sachs Group, Inc. is a global financial institution that delivers a range of financial services to a large and diversified client base that includes corporations, financial institutions, governments and individuals. Its segments include Global Banking &amp; Markets, Asset &amp; Wealth Management and Platform Solutions. The Global Banking &amp; Markets segment offers a range of services, including financing, advisory services, risk distribution, and hedging for its institutional and corporate clients. It facilitates client transactions and makes markets in fixed income, equity, currency and commodity products. The Asset &amp; Wealth Management segment manages assets and offers investment products across all asset classes to a diverse set of clients. It also provides investing and wealth advisory solutions. The Platform Solutions segment includes consumer platforms, such as partnerships offering credit cards and point-of-sale financing, and transaction banking and other platform businesses.</v>
     <v>48300</v>
@@ -8229,7 +8229,7 @@
     <v>798.36</v>
     <v>Investment Banking &amp; Investment Services</v>
     <v>Stock</v>
-    <v>45958.907151620311</v>
+    <v>45958.943829351563</v>
     <v>193</v>
     <v>787.35</v>
     <v>239839873108</v>
@@ -8239,11 +8239,11 @@
     <v>16.047799999999999</v>
     <v>789.99</v>
     <v>792.28</v>
-    <v>790.44</v>
+    <v>791.06</v>
     <v>302721100</v>
     <v>GS</v>
     <v>THE GOLDMAN SACHS GROUP, INC. (XNYS:GS)</v>
-    <v>1241106</v>
+    <v>1241487</v>
     <v>2071797</v>
     <v>1998</v>
   </rv>
@@ -8271,8 +8271,8 @@
     <v>2.0825999999999998</v>
     <v>-0.26</v>
     <v>-0.11206899999999999</v>
-    <v>0.01</v>
-    <v>4.8539999999999998E-3</v>
+    <v>0.03</v>
+    <v>1.4563E-2</v>
     <v>USD</v>
     <v>Luminar Technologies, Inc. is a global automotive technology company, which is engaged in vehicle safety and autonomy. It enables safety and autonomous capabilities for passenger and commercial vehicles and other adjacent markets. Its Autonomy Solutions segment is engaged in the design, manufacturing, and sale of LiDAR sensors, catering mainly to the original equipment manufacturers in the automobile, commercial vehicle, robo-taxi, and adjacent industries. Its Advanced Technologies and Services segment provides advanced semiconductors and related components, as well as design, test, and consulting services to the Autonomy Solutions segment and to various third-party customers, including government agencies and defense contractors, in markets generally unrelated to autonomous vehicles. Its products include Iris lidar, Core Sensor Software, Driving Functions Software, and others. EM4 manufactures and sells packaged photonic components and sub-systems for aerospace and industrial markets.</v>
     <v>580</v>
@@ -8283,7 +8283,7 @@
     <v>2.2949999999999999</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45958.91002387656</v>
+    <v>45958.94355054375</v>
     <v>196</v>
     <v>2.0499999999999998</v>
     <v>141654787</v>
@@ -8293,11 +8293,11 @@
     <v>0</v>
     <v>2.3199999999999998</v>
     <v>2.06</v>
-    <v>2.0699999999999998</v>
+    <v>2.09</v>
     <v>68764460</v>
     <v>LAZR</v>
     <v>LUMINAR TECHNOLOGIES, INC. (XNAS:LAZR)</v>
-    <v>6259469</v>
+    <v>6278163</v>
     <v>7584653</v>
     <v>2018</v>
   </rv>
@@ -8325,8 +8325,8 @@
     <v>1.2329000000000001</v>
     <v>-1.1599999999999999</v>
     <v>-3.5969000000000001E-2</v>
-    <v>0.14000000000000001</v>
-    <v>4.5030000000000001E-3</v>
+    <v>0.1598</v>
+    <v>5.1400000000000005E-3</v>
     <v>USD</v>
     <v>Southwest Airlines Co. (Southwest) operates Southwest Airlines, a passenger airline that provides scheduled air transportation in the United States and near-international markets. The Company's fare products include four categories: Wanna Get Away, Wanna Get Away Plus, Anytime, and Business Select to provide customers options when choosing a fare. It also offers ancillary services, such as EarlyBird Check-In, Upgraded Boarding, and transportation of pets and unaccompanied minors, in accordance with Southwest’s respective policies. Its Rapid Rewards loyalty program enables program members to earn points for every dollar spent on Southwest base fares, also including purchases paid with LUV Vouchers, gift cards, or flight credit, with no portion of the purchase price paid with Rapid Rewards points. It operates over 803 Boeing 737 aircraft in its fleet and serves 117 destinations in 42 states, the District of Columbia, the Commonwealth of Puerto Rico, and ten near-international countries.</v>
     <v>72223</v>
@@ -8337,7 +8337,7 @@
     <v>32.174999999999997</v>
     <v>Passenger Transportation Services</v>
     <v>Stock</v>
-    <v>45958.908607094534</v>
+    <v>45958.936456353906</v>
     <v>199</v>
     <v>31.024999999999999</v>
     <v>16078352059</v>
@@ -8347,11 +8347,11 @@
     <v>48.199100000000001</v>
     <v>32.25</v>
     <v>31.09</v>
-    <v>31.23</v>
+    <v>31.2498</v>
     <v>517155100</v>
     <v>LUV</v>
     <v>SOUTHWEST AIRLINES CO. (XNYS:LUV)</v>
-    <v>11372613</v>
+    <v>11375037</v>
     <v>9863868</v>
     <v>1967</v>
   </rv>
@@ -8379,8 +8379,8 @@
     <v>0.92490000000000006</v>
     <v>-6.16</v>
     <v>-1.0762000000000001E-2</v>
-    <v>1.08</v>
-    <v>1.908E-3</v>
+    <v>2.0699999999999998</v>
+    <v>3.6580000000000002E-3</v>
     <v>USD</v>
     <v>Mastercard Incorporated is a technology company in the global payments industry. The Company connects consumers, financial institutions, merchants, governments, digital partners, businesses and other organizations worldwide by enabling electronic payments and making those payment transactions secure, simple, smart and accessible. It provides a range of payment solutions and services using its brands, including Mastercard, Maestro and Cirrus. It operates a payments network that provides choice and flexibility for consumers, merchants and its customers. Through its proprietary global payments network, it switches (authorizes, clears and settles) payment transactions. Its additional payments capabilities include automated clearing house (ACH) transactions (both batch and real-time account-based payments). It offers security solutions, consumer acquisition and engagement, business and market insights, gateway, processing and open banking, among other services and solutions.</v>
     <v>35300</v>
@@ -8391,21 +8391,21 @@
     <v>573.99</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45958.907810601566</v>
+    <v>45958.937443437499</v>
     <v>202</v>
     <v>565.45000000000005</v>
     <v>511851481160</v>
     <v>MASTERCARD INCORPORATED.</v>
     <v>MASTERCARD INCORPORATED.</v>
     <v>573.08000000000004</v>
-    <v>38.183999999999997</v>
+    <v>38.599400000000003</v>
     <v>572.36</v>
     <v>566.20000000000005</v>
-    <v>567.01</v>
+    <v>568</v>
     <v>904011800</v>
     <v>MA</v>
     <v>MASTERCARD INCORPORATED. (XNYS:MA)</v>
-    <v>2915551</v>
+    <v>2915979</v>
     <v>2584390</v>
     <v>2001</v>
   </rv>
@@ -8422,7 +8422,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-US</v>
     <v>a1yuvh</v>
     <v>268435456</v>
@@ -8445,21 +8445,21 @@
     <v>8.75</v>
     <v>Biotechnology &amp; Medical Research</v>
     <v>Stock</v>
-    <v>45958.896075346878</v>
+    <v>45958.938877638284</v>
     <v>205</v>
     <v>8.4</v>
     <v>1383832032</v>
     <v>NOVAVAX, INC.</v>
     <v>NOVAVAX, INC.</v>
     <v>8.75</v>
-    <v>3.7250999999999999</v>
+    <v>3.8037000000000001</v>
     <v>8.6999999999999993</v>
     <v>8.52</v>
     <v>8.5</v>
     <v>162421600</v>
     <v>NVAX</v>
     <v>NOVAVAX, INC. (XNAS:NVAX)</v>
-    <v>2092861</v>
+    <v>2100770</v>
     <v>4420432</v>
     <v>1987</v>
   </rv>
@@ -8503,8 +8503,8 @@
     <v>0.60219999999999996</v>
     <v>-5.75</v>
     <v>-4.4524999999999995E-2</v>
-    <v>0.52</v>
-    <v>4.2129999999999997E-3</v>
+    <v>0.51</v>
+    <v>4.1320000000000003E-3</v>
     <v>USD</v>
     <v>Novartis AG is a Switzerland-based pharmaceutical company. The Company develops, manufactures, and markets branded and generic prescription drugs, active pharmaceutical ingredients (APIs), biosimilars and ophthalmic products. The Company uses science and digital technologies for treatments in the disease areas of immunology, dermatology, cancer, ophthalmology, neuroscience, respiratory, cardiovascular, renal and metabolism. The business activities of the Company are divided into two segments: Innovative Medicines, which includes innovative patent-protected prescription medicines for blood pressure, cancer and other ailments, and Sandoz, which includes generic pharmaceuticals and biosimilars.</v>
     <v>75883</v>
@@ -8516,7 +8516,7 @@
     <v>210</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45958.904235138281</v>
+    <v>45958.934662800784</v>
     <v>211</v>
     <v>123.06</v>
     <v>273972100000</v>
@@ -8526,11 +8526,11 @@
     <v>17.624600000000001</v>
     <v>129.13999999999999</v>
     <v>123.39</v>
-    <v>123.95</v>
+    <v>123.94</v>
     <v>2112422000</v>
     <v>NVS</v>
     <v>Novartis Inc. (XNYS:NVS)</v>
-    <v>4630509</v>
+    <v>4630798</v>
     <v>1567375</v>
     <v>1996</v>
   </rv>
@@ -8558,8 +8558,8 @@
     <v>0.90400000000000003</v>
     <v>-1.45</v>
     <v>-3.4279000000000004E-2</v>
-    <v>0.14000000000000001</v>
-    <v>3.4289999999999998E-3</v>
+    <v>0.2011</v>
+    <v>4.9249999999999997E-3</v>
     <v>USD</v>
     <v>Occidental Petroleum Corporation is an international energy company with assets primarily in the United States, the Middle East and North Africa. The Company is an oil and gas producer in the United States, including a producer in the Permian and DJ basins, and the offshore Gulf of Mexico. It operates through three segments: oil and gas, chemical and midstream and marketing. The oil and gas segment explores for, develops, and produces oil (which includes condensate), natural gas liquids (NGL) and natural gas. The chemical segment primarily manufactures and markets basic chemicals and vinyls. The midstream and marketing segment purchases, markets, gathers, processes, transports, and stores oil (which includes condensate), NGL, natural gas, carbon dioxide (CO2) and power. The midstream and marketing segment provides flow assurance and maximizes the value of its oil and gas. It also optimizes its transportation and storage capacity and invests in entities that conduct similar activities.</v>
     <v>13323</v>
@@ -8570,7 +8570,7 @@
     <v>42.11</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45958.910058263282</v>
+    <v>45958.943697661722</v>
     <v>214</v>
     <v>40.81</v>
     <v>40214365830</v>
@@ -8580,11 +8580,11 @@
     <v>24.062000000000001</v>
     <v>42.3</v>
     <v>40.85</v>
-    <v>40.97</v>
+    <v>41.031100000000002</v>
     <v>984439800</v>
     <v>OXY</v>
     <v>OCCIDENTAL PETROLEUM CORPORATION (XNYS:OXY)</v>
-    <v>13283484</v>
+    <v>13291787</v>
     <v>12094450</v>
     <v>1986</v>
   </rv>
@@ -8612,8 +8612,8 @@
     <v>0.50390000000000001</v>
     <v>-0.245</v>
     <v>-9.8910000000000005E-3</v>
-    <v>-2.9999999999999997E-4</v>
-    <v>-1.224E-5</v>
+    <v>0.04</v>
+    <v>1.6329999999999999E-3</v>
     <v>USD</v>
     <v>Pfizer Inc. is a research-based, global biopharmaceutical company. The Company is engaged in the discovery, development, manufacture, marketing, sale and distribution of biopharmaceutical products worldwide. Its Biopharma segment includes the Pfizer U.S. Commercial Division, and the Pfizer International Commercial Division. Its product categories include oncology, primary care and specialty care. Its oncology products include Ibrance, Xtandi, Padcev, Adcetris, Inlyta, Lorbrena, Bosulif, Tukysa, Braftovi, Mektovi, Orgovyx, Elrexfio, Tivdak and Talzenna. Its primary care products include Eliquis, Nurtec ODT/Vydura, Zavzpret, the Prevnar family, Comirnaty, Abrysvo, FSME/IMMUN-TicoVac, Nimenrix, Trumenba, and Paxlovid. Its specialty care products include Xeljanz, Enbrel (outside the United States and Canada), Inflectra, Abrilada, Cibinqo, Litfulo, Eucrisa, Velsipity, the Vyndaqel family, Genotropin, BeneFIX, Xyntha, Somavert, Ngenla, Hympavzi, Sulperazon, Zavicefta, Octagam and others.</v>
     <v>81000</v>
@@ -8624,7 +8624,7 @@
     <v>24.78</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45958.910012685155</v>
+    <v>45958.943426921091</v>
     <v>217</v>
     <v>24.38</v>
     <v>139438113750</v>
@@ -8634,11 +8634,11 @@
     <v>17.784600000000001</v>
     <v>24.77</v>
     <v>24.524999999999999</v>
-    <v>24.499700000000001</v>
+    <v>24.54</v>
     <v>5685550000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>50063446</v>
+    <v>50094470</v>
     <v>55089150</v>
     <v>1942</v>
   </rv>
@@ -8666,8 +8666,8 @@
     <v>2.6541000000000001</v>
     <v>-0.105</v>
     <v>-2.7202E-2</v>
-    <v>1E-4</v>
-    <v>2.667E-5</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Transocean Ltd. is an international provider of offshore contract drilling services for oil and gas wells. The Company's primary business is to contract its drilling rigs, related equipment and work crews on a dayrate basis to drill oil and gas wells. As of February 9, 2017, it owned or had partial ownership interests in and operated 56 mobile offshore drilling units. As of February 9, 2017, its fleet consisted of 30 floaters, seven harsh environment floaters, three deepwater floaters, six midwater floaters and 10 high-specification jackups. As February 9, 2017, it also had four ultra-deepwater drillships and five high-specification jackups under construction or under contract to be constructed. Its contract drilling services operations are spread across oil and gas exploration and development areas throughout the world. The Company's drilling fleet can be characterized as floaters, including drillships and semisubmersibles, and jackups.</v>
     <v>5800</v>
@@ -8678,7 +8678,7 @@
     <v>3.83</v>
     <v>Oil &amp; Gas Related Equipment and Services</v>
     <v>Stock</v>
-    <v>45958.90961271953</v>
+    <v>45958.936144490624</v>
     <v>220</v>
     <v>3.7250000000000001</v>
     <v>4134224960</v>
@@ -8687,11 +8687,11 @@
     <v>3.78</v>
     <v>3.86</v>
     <v>3.7549999999999999</v>
-    <v>3.7501000000000002</v>
+    <v>3.75</v>
     <v>1100992000</v>
     <v>RIG</v>
     <v>Transocean Ltd (XNYS:RIG)</v>
-    <v>53712232</v>
+    <v>53723268</v>
     <v>64431958</v>
     <v>2008</v>
   </rv>
@@ -8719,8 +8719,8 @@
     <v>0.49919999999999998</v>
     <v>-0.39</v>
     <v>-1.0439E-2</v>
-    <v>-0.02</v>
-    <v>-5.4100000000000003E-4</v>
+    <v>-7.0000000000000007E-2</v>
+    <v>-1.8929999999999999E-3</v>
     <v>USD</v>
     <v>Range Resources Corporation is an independent natural gas and natural gas liquids (NGLs) producer. The Company is engaged in the exploration, development and acquisition of natural gas and oil properties in the Appalachian region of the United States. Its principal area of operations is the Marcellus Shale in Pennsylvania. Its properties consist of interests in developed and undeveloped natural gas and oil leases. It owns approximately 1,431 net producing wells in Pennsylvania. It holds a portfolio of drilling opportunities and unbooked resource potential within the Marcellus, Utica/Point Pleasant and Upper Devonian formations. Its exploration and production operations are limited to the onshore United States. It has approximately 871,000 gross (763,000 net) acres under lease. Its subsidiaries include Range Resources-Appalachia, LLC, Range Resources-Pine Mountain, LLC, Range Production Company, LLC, Range Resources-Midcontinent, LLC and Range Resources-Louisiana, Inc.</v>
     <v>565</v>
@@ -8731,21 +8731,21 @@
     <v>37.32</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45958.891160474217</v>
+    <v>45958.92058277734</v>
     <v>223</v>
     <v>36.67</v>
     <v>8805924967</v>
     <v>RANGE RESOURCES CORPORATION</v>
     <v>RANGE RESOURCES CORPORATION</v>
     <v>36.97</v>
-    <v>33.154000000000003</v>
+    <v>33.502499999999998</v>
     <v>37.36</v>
     <v>36.97</v>
-    <v>36.950000000000003</v>
+    <v>36.9</v>
     <v>238191100</v>
     <v>RRC</v>
     <v>RANGE RESOURCES CORPORATION (XNYS:RRC)</v>
-    <v>2553001</v>
+    <v>2553012</v>
     <v>3010799</v>
     <v>1980</v>
   </rv>
@@ -8773,8 +8773,8 @@
     <v>2.7433999999999998</v>
     <v>0.04</v>
     <v>4.9910000000000004E-4</v>
-    <v>-0.17899999999999999</v>
-    <v>-2.232E-3</v>
+    <v>0.02</v>
+    <v>2.4939999999999999E-4</v>
     <v>USD</v>
     <v>Block, Inc. builds technology to increase access to the global economy. The Company operates through two segments: Square and Cash App. The Square includes managed payment services, software solutions, hardware, and financial services offered to sellers, excluding those that involve Cash App. The Cash App segment includes the financial tools available to individuals within the mobile Cash App, including peer-to-peer payments, bitcoin and stock investments. The Cash App also includes Cash App Card, which is linked to customer stored balances that customers can use to pay for purchases or withdraw funds from an ATM. Cash App also includes the BNPL platform. Its Afterpay business is transforming the way customers manage their spending over time. Its TIDAL business is a music platform that empowers artists to thrive as entrepreneurs. Its Bitkey business is a simple self-custody wallet built for bitcoin. Proto business is a suite of bitcoin mining products and services.</v>
     <v>11372</v>
@@ -8785,7 +8785,7 @@
     <v>81.7</v>
     <v>Professional &amp; Commercial Services</v>
     <v>Stock</v>
-    <v>45958.909989293752</v>
+    <v>45958.939988853905</v>
     <v>226</v>
     <v>79.77</v>
     <v>48882540960</v>
@@ -8795,11 +8795,11 @@
     <v>47.354399999999998</v>
     <v>80.150000000000006</v>
     <v>80.19</v>
-    <v>80.001000000000005</v>
+    <v>80.2</v>
     <v>609584000</v>
     <v>XYZ</v>
     <v>BLOCK, INC. (XNYS:XYZ)</v>
-    <v>3949441</v>
+    <v>3950889</v>
     <v>5718050</v>
     <v>2009</v>
   </rv>
@@ -8976,18 +8976,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.1918</v>
     <v>1.0176000000000001</v>
-    <v>2.0000000000000001E-4</v>
-    <v>1.717E-4</v>
+    <v>1E-4</v>
+    <v>8.5839999999999991E-5</v>
     <v>USD</v>
     <v>EUR</v>
-    <v>1.1653</v>
+    <v>1.1657999999999999</v>
     <v>Currency Pair</v>
-    <v>45958.91002314815</v>
+    <v>45958.943715277775</v>
     <v>1.1652</v>
     <v>Euro/US Dollar FX Spot Rate</v>
     <v>1.165</v>
     <v>1.165</v>
-    <v>1.1652</v>
+    <v>1.1651</v>
     <v>EURUSD</v>
     <v>EUR/USD</v>
   </rv>
@@ -9012,9 +9012,9 @@
     <v>5.4109999999999998E-4</v>
     <v>CHF</v>
     <v>EUR</v>
-    <v>0.92490000000000006</v>
+    <v>0.92520000000000002</v>
     <v>Currency Pair</v>
-    <v>45958.91002314815</v>
+    <v>45958.943831018521</v>
     <v>0.92459999999999998</v>
     <v>Euro/Swiss Franc FX Cross Rate</v>
     <v>0.9244</v>
@@ -9038,20 +9038,20 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>0.87780000000000002</v>
+    <v>0.87829999999999997</v>
     <v>0.82189999999999996</v>
-    <v>-4.0000000000000002E-4</v>
-    <v>-4.5570000000000002E-4</v>
+    <v>2.0000000000000001E-4</v>
+    <v>2.2790000000000001E-4</v>
     <v>GBP</v>
     <v>EUR</v>
-    <v>0.87780000000000002</v>
+    <v>0.87829999999999997</v>
     <v>Currency Pair</v>
-    <v>45958.910046296296</v>
+    <v>45958.943738425929</v>
     <v>0.87760000000000005</v>
     <v>Euro/UK Pound Sterling FX Cross Rate</v>
     <v>0.87760000000000005</v>
     <v>0.87770000000000004</v>
-    <v>0.87729999999999997</v>
+    <v>0.87790000000000001</v>
     <v>EURGBP</v>
     <v>EUR/GBP</v>
   </rv>
@@ -9072,18 +9072,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.8554999999999999</v>
     <v>1.5899000000000001</v>
-    <v>5.0000000000000001E-4</v>
-    <v>2.8269999999999999E-4</v>
+    <v>8.9999999999999998E-4</v>
+    <v>5.0889999999999996E-4</v>
     <v>AUD</v>
     <v>EUR</v>
-    <v>1.77</v>
+    <v>1.7704</v>
     <v>Currency Pair</v>
-    <v>45958.91002314815</v>
+    <v>45958.943715277775</v>
     <v>1.7696000000000001</v>
     <v>Euro/Australian Dollar FX Cross Rate</v>
     <v>1.7685999999999999</v>
     <v>1.7684</v>
-    <v>1.7688999999999999</v>
+    <v>1.7693000000000001</v>
     <v>EURAUD</v>
     <v>EUR/AUD</v>
   </rv>
@@ -9108,10 +9108,10 @@
     <v>-6.1550000000000005E-5</v>
     <v>CAD</v>
     <v>EUR</v>
-    <v>1.6251</v>
+    <v>1.6256999999999999</v>
     <v>Currency Pair</v>
-    <v>45958.91002314815</v>
-    <v>1.6249</v>
+    <v>45958.943807870368</v>
+    <v>1.6248</v>
     <v>Euro/Canadian Dollar FX Cross Rate</v>
     <v>1.6247</v>
     <v>1.6246</v>
@@ -9136,18 +9136,18 @@
     <v>Powered by Refinitiv</v>
     <v>158.87</v>
     <v>139.86000000000001</v>
-    <v>-0.04</v>
-    <v>-2.63E-4</v>
+    <v>0.05</v>
+    <v>3.2870000000000002E-4</v>
     <v>JPY</v>
     <v>USD</v>
-    <v>152.11000000000001</v>
+    <v>152.16</v>
     <v>Currency Pair</v>
-    <v>45958.909861111111</v>
+    <v>45958.943796296298</v>
     <v>152.06</v>
     <v>US Dollar/Japanese Yen FX Spot Rate</v>
     <v>152.1</v>
     <v>152.1</v>
-    <v>152.06</v>
+    <v>152.15</v>
     <v>USDJPY</v>
     <v>USD/JPY</v>
   </rv>
@@ -9168,18 +9168,18 @@
     <v>Powered by Refinitiv</v>
     <v>0.92</v>
     <v>0.78269999999999995</v>
-    <v>2.9999999999999997E-4</v>
-    <v>3.7830000000000003E-4</v>
+    <v>4.0000000000000002E-4</v>
+    <v>5.0440000000000001E-4</v>
     <v>CHF</v>
     <v>USD</v>
     <v>0.79379999999999995</v>
     <v>Currency Pair</v>
-    <v>45958.909942129627</v>
-    <v>0.79349999999999998</v>
+    <v>45958.943831018521</v>
+    <v>0.79339999999999999</v>
     <v>US Dollar/Swiss Franc FX Spot Rate</v>
     <v>0.79349999999999998</v>
     <v>0.79310000000000003</v>
-    <v>0.79339999999999999</v>
+    <v>0.79349999999999998</v>
     <v>USDCHF</v>
     <v>USD/CHF</v>
   </rv>
@@ -9200,18 +9200,18 @@
     <v>Powered by Refinitiv</v>
     <v>0.82650000000000001</v>
     <v>0.72509999999999997</v>
-    <v>-2.8400000000000002E-4</v>
-    <v>-3.7699999999999995E-4</v>
+    <v>5.7000000000000003E-5</v>
+    <v>7.5660000000000004E-5</v>
     <v>GBP</v>
     <v>USD</v>
-    <v>0.75339999999999996</v>
+    <v>0.75349999999999995</v>
     <v>Currency Pair</v>
-    <v>45958.91002314815</v>
+    <v>45958.943738425929</v>
     <v>0.75319999999999998</v>
     <v>US Dollar/UK Pound Sterling FX Cross Rate</v>
     <v>0.75329999999999997</v>
     <v>0.75339999999999996</v>
-    <v>0.75309999999999999</v>
+    <v>0.75349999999999995</v>
     <v>USDGBP</v>
     <v>USD/GBP</v>
   </rv>
@@ -9321,8 +9321,8 @@
     <v>1.8829</v>
     <v>-7.5</v>
     <v>-7.0759999999999998E-3</v>
-    <v>1.22</v>
-    <v>1.1590000000000001E-3</v>
+    <v>0.75</v>
+    <v>7.1260000000000008E-4</v>
     <v>USD</v>
     <v>ASML Holding N.V. is a holding company based in the Netherlands. The Company operates through its subsidiaries in the Netherlands, the United States, Italy, France, Germany, the United Kingdom, Ireland, Belgium, South Korea, Taiwan, Singapore, China, Hong Kong, Japan, Malaysia and Israel. The Company operates through one business segment which is engage in development, production, marketing, sales, upgrading and servicing of advanced semiconductor equipment systems, consisting of lithography, metrology and inspection systems. The Company offers TWINSCAN systems, equipped with lithography system with a mercury lamp as light source (i-line), Krypton Fluoride (KrF) and Argon Fluoride (ArF) light sources for processing wafers for manufacturing environments for which imaging at a small resolution is required. TWINSCAN systems also include immersion lithography systems (TWINSCAN immersion systems).</v>
     <v>43461</v>
@@ -9333,7 +9333,7 @@
     <v>1060.6400000000001</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45958.906627846874</v>
+    <v>45958.942684964844</v>
     <v>263</v>
     <v>1051.73</v>
     <v>409752000000</v>
@@ -9343,11 +9343,11 @@
     <v>37.136400000000002</v>
     <v>1059.98</v>
     <v>1052.48</v>
-    <v>1053.7</v>
+    <v>1053.23</v>
     <v>388147700</v>
     <v>ASML</v>
     <v>ASML Holding NV (XNAS:ASML)</v>
-    <v>855980</v>
+    <v>856184</v>
     <v>1627328</v>
     <v>1994</v>
   </rv>
@@ -9370,8 +9370,8 @@
     <v>0.6</v>
     <v>-1.7500000000000002E-2</v>
     <v>-2.4527E-2</v>
-    <v>-1.24E-2</v>
-    <v>-1.7464999999999998E-2</v>
+    <v>0.01</v>
+    <v>1.4085E-2</v>
     <v>USD</v>
     <v>Big Tree Cloud Holdings Ltd is a China-based company principally engaged in the development, production and sales of personal care products and other consumer goods. The Company delivers products that cater to the needs of modern, health-conscious, and independent consumers. It focuses on the development and production of feminine hygiene products, including sterilized feminine pads, menstrual pants, and other feminine hygiene products. Its body and oral care products include shampoo and conditioner, body wash, facial mask and cream, and others. Its accessories include earrings, bracelets, pendants and other jewelry accessories. It distributes its products through its flagship stores on e-commerce platforms. The Company also engages in licensing business by authorizing its customers and third-party commercial stores to use its logo, trademark and brand name.</v>
     <v>50</v>
@@ -9382,20 +9382,20 @@
     <v>0.78920000000000001</v>
     <v>Personal &amp; Household Products &amp; Services</v>
     <v>Stock</v>
-    <v>45958.905568541406</v>
+    <v>45958.941635404684</v>
     <v>0.68</v>
     <v>67970780</v>
     <v>Big Tree Cloud Holdings Limited</v>
     <v>Big Tree Cloud Holdings Limited</v>
     <v>0.70540000000000003</v>
-    <v>62.142899999999997</v>
+    <v>63.743299999999998</v>
     <v>0.71350000000000002</v>
     <v>0.69599999999999995</v>
-    <v>0.6976</v>
+    <v>0.72</v>
     <v>95037440</v>
     <v>DSY</v>
     <v>Big Tree Cloud Holdings Limited (XNAS:DSY)</v>
-    <v>856076</v>
+    <v>860343</v>
     <v>263706</v>
   </rv>
   <rv s="2">
@@ -9411,7 +9411,7 @@
     <v>2</v>
     <v>11</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1v3sm</v>
     <v>268435456</v>
@@ -9420,10 +9420,10 @@
     <v>14.67</v>
     <v>4.8899999999999997</v>
     <v>1.4450000000000001</v>
-    <v>7.4999999999999997E-2</v>
-    <v>6.5100000000000002E-3</v>
-    <v>-3.8E-3</v>
-    <v>-3.279E-4</v>
+    <v>7.0000000000000007E-2</v>
+    <v>6.0760000000000007E-3</v>
+    <v>-0.2</v>
+    <v>-1.7256000000000001E-2</v>
     <v>USD</v>
     <v>IAMGOLD Corporation is a Canada-based intermediate gold producer and developer. Its principal activities are the exploration, development, and operation of gold mining properties in North America and West Africa. Its projects include Essakane, Westwood and Cote Gold. The Essakane project is in north-eastern Burkina Faso, West Africa. It straddles the boundary of the Oudalan and Seno provinces in the Sahel region of Burkina Faso and is approximately 330 kilometers (km) northeast of the capital, Ouagadougou. The Westwood Project is located on the Doyon property, 2.5 km east of the former Doyon Gold Mine in Bousquet Township. The Cote Gold Project is in the Chester and Yeo Townships, District of Sudbury, in northeastern Ontario. It owns a 100% interest in the Nelligan Gold Project, located 60Km southwest of Chibougamau. It holds claims of Nelligan, as well as other earlier stage exploration properties in Northern Quebec. It also owns Rich Lake and Lac a l’Eau Jaune (gold) properties.</v>
     <v>4341</v>
@@ -9434,7 +9434,7 @@
     <v>11.71</v>
     <v>Metals &amp; Mining</v>
     <v>Stock</v>
-    <v>45958.901330300781</v>
+    <v>45958.924252175784</v>
     <v>268</v>
     <v>11.24</v>
     <v>9276791000</v>
@@ -9443,12 +9443,12 @@
     <v>11.24</v>
     <v>8.3327000000000009</v>
     <v>11.52</v>
-    <v>11.595000000000001</v>
-    <v>11.5862</v>
+    <v>11.59</v>
+    <v>11.39</v>
     <v>575332100</v>
     <v>IAG</v>
     <v>IAMGOLD CORPORATION (XNYS:IAG)</v>
-    <v>13964664</v>
+    <v>13971074</v>
     <v>15404111</v>
     <v>2017</v>
   </rv>
@@ -12340,7 +12340,7 @@
     <row r="1" spans="1:32" s="1" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="91">
         <f ca="1">MAX(E3:E96)</f>
-        <v>45958.910078495312</v>
+        <v>45958.943851689066</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>45958.952081944444</v>
+        <v>45958.985589814816</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
@@ -12479,7 +12479,7 @@
       </c>
       <c r="B3" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C3" s="16" t="e" vm="1">
         <v>#VALUE!</v>
@@ -12490,7 +12490,7 @@
       </c>
       <c r="E3" s="18" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909980022654</v>
+        <v>45958.9436489</v>
       </c>
       <c r="F3" s="19" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -12534,7 +12534,7 @@
       </c>
       <c r="P3" s="23" cm="1">
         <f t="array" aca="1" ref="P3" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>41443517</v>
+        <v>41473172</v>
       </c>
       <c r="Q3" s="23" cm="1">
         <f t="array" aca="1" ref="Q3" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -12553,7 +12553,7 @@
       </c>
       <c r="V3" s="114">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.91676510252840016</v>
+        <v>0.91742109581959397</v>
       </c>
       <c r="W3" s="24"/>
       <c r="X3" s="108">
@@ -12597,7 +12597,7 @@
       </c>
       <c r="B4" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C4" s="25" t="e" vm="2">
         <v>#VALUE!</v>
@@ -12715,7 +12715,7 @@
       </c>
       <c r="B5" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1398609369656903E-2</v>
+        <v>1.1390818999886093E-2</v>
       </c>
       <c r="C5" s="25" t="e" vm="3">
         <v>#VALUE!</v>
@@ -12831,7 +12831,7 @@
       </c>
       <c r="B6" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C6" t="e" vm="4">
         <v>#VALUE!</v>
@@ -12842,7 +12842,7 @@
       </c>
       <c r="E6" s="18" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910078495312</v>
+        <v>45958.943784490628</v>
       </c>
       <c r="F6" s="19" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -12886,7 +12886,7 @@
       </c>
       <c r="P6" s="23" cm="1">
         <f t="array" aca="1" ref="P6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>46903995</v>
+        <v>46991794</v>
       </c>
       <c r="Q6" s="23" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -12905,7 +12905,7 @@
       </c>
       <c r="V6" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0320873491369196</v>
+        <v>1.0340193005019764</v>
       </c>
       <c r="W6" s="24"/>
       <c r="X6" s="108">
@@ -13189,7 +13189,7 @@
       </c>
       <c r="E9" s="18" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910013506247</v>
+        <v>45958.943683830468</v>
       </c>
       <c r="F9" s="19" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13233,7 +13233,7 @@
       </c>
       <c r="P9" s="23" cm="1">
         <f t="array" aca="1" ref="P9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>20990453</v>
+        <v>21019816</v>
       </c>
       <c r="Q9" s="23" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13251,7 +13251,7 @@
       </c>
       <c r="V9" s="107">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0210935671228782</v>
+        <v>1.0225219484165753</v>
       </c>
       <c r="W9" s="107"/>
       <c r="X9" s="108">
@@ -13302,7 +13302,7 @@
       </c>
       <c r="E10" s="18" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908744096872</v>
+        <v>45958.932806700781</v>
       </c>
       <c r="F10" s="19" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13346,7 +13346,7 @@
       </c>
       <c r="P10" s="23" cm="1">
         <f t="array" aca="1" ref="P10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>3661505</v>
+        <v>3661534</v>
       </c>
       <c r="Q10" s="23" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13362,7 +13362,7 @@
       </c>
       <c r="V10" s="107">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.64008509282925619</v>
+        <v>0.64009016245709827</v>
       </c>
       <c r="W10" s="107"/>
       <c r="X10" s="108">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="B11" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C11" t="e" vm="10">
         <v>#VALUE!</v>
@@ -13414,7 +13414,7 @@
       </c>
       <c r="E11" s="30" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.904144617969</v>
+        <v>45958.931424652343</v>
       </c>
       <c r="F11" s="19" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13458,7 +13458,7 @@
       </c>
       <c r="P11" s="34" cm="1">
         <f t="array" aca="1" ref="P11" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>5762180</v>
+        <v>5776523</v>
       </c>
       <c r="Q11" s="34" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13478,7 +13478,7 @@
       </c>
       <c r="V11" s="93">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.60519631242992589</v>
+        <v>0.60670274414659953</v>
       </c>
       <c r="W11" s="93"/>
       <c r="X11" s="108">
@@ -13522,7 +13522,7 @@
       </c>
       <c r="B12" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C12" t="e" vm="11">
         <v>#VALUE!</v>
@@ -13640,7 +13640,7 @@
       </c>
       <c r="B13" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C13" t="e" vm="12">
         <v>#VALUE!</v>
@@ -13651,7 +13651,7 @@
       </c>
       <c r="E13" s="18" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.907661214842</v>
+        <v>45958.94136456016</v>
       </c>
       <c r="F13" s="19" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13695,7 +13695,7 @@
       </c>
       <c r="P13" s="23" cm="1">
         <f t="array" aca="1" ref="P13" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8754147</v>
+        <v>8759120</v>
       </c>
       <c r="Q13" s="23" cm="1">
         <f t="array" aca="1" ref="Q13" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13714,7 +13714,7 @@
       </c>
       <c r="V13" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.62783306346909884</v>
+        <v>0.62818971887191899</v>
       </c>
       <c r="W13" s="24"/>
       <c r="X13" s="108">
@@ -13758,7 +13758,7 @@
       </c>
       <c r="B14" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C14" t="e" vm="13">
         <v>#VALUE!</v>
@@ -13769,7 +13769,7 @@
       </c>
       <c r="E14" s="18" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908908298436</v>
+        <v>45958.943276284372</v>
       </c>
       <c r="F14" s="19" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13813,7 +13813,7 @@
       </c>
       <c r="P14" s="23" cm="1">
         <f t="array" aca="1" ref="P14" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>19871185</v>
+        <v>19873218</v>
       </c>
       <c r="Q14" s="23" cm="1">
         <f t="array" aca="1" ref="Q14" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13832,7 +13832,7 @@
       </c>
       <c r="V14" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.1505031863042818</v>
+        <v>1.1506208930730406</v>
       </c>
       <c r="W14" s="24"/>
       <c r="X14" s="108">
@@ -13876,7 +13876,7 @@
       </c>
       <c r="B15" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C15" t="e" vm="14">
         <v>#VALUE!</v>
@@ -13887,7 +13887,7 @@
       </c>
       <c r="E15" s="18" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908717395316</v>
+        <v>45958.94380388828</v>
       </c>
       <c r="F15" s="19" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13931,7 +13931,7 @@
       </c>
       <c r="P15" s="23" cm="1">
         <f t="array" aca="1" ref="P15" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>9831426</v>
+        <v>9841755</v>
       </c>
       <c r="Q15" s="23" cm="1">
         <f t="array" aca="1" ref="Q15" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13950,7 +13950,7 @@
       </c>
       <c r="V15" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.4063506331808266</v>
+        <v>1.4078281600106197</v>
       </c>
       <c r="W15" s="24"/>
       <c r="X15" s="108">
@@ -13994,7 +13994,7 @@
       </c>
       <c r="B16" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C16" t="e" vm="15">
         <v>#VALUE!</v>
@@ -14005,7 +14005,7 @@
       </c>
       <c r="E16" s="18" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.904932650003</v>
+        <v>45958.94197274297</v>
       </c>
       <c r="F16" s="19" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14049,7 +14049,7 @@
       </c>
       <c r="P16" s="23" cm="1">
         <f t="array" aca="1" ref="P16" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>5964314</v>
+        <v>6002660</v>
       </c>
       <c r="Q16" s="23" cm="1">
         <f t="array" aca="1" ref="Q16" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14068,7 +14068,7 @@
       </c>
       <c r="V16" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.1743232885149</v>
+        <v>1.1818732935651692</v>
       </c>
       <c r="W16" s="24"/>
       <c r="X16" s="108">
@@ -14112,7 +14112,7 @@
       </c>
       <c r="B17" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C17" t="e" vm="16">
         <v>#VALUE!</v>
@@ -14123,7 +14123,7 @@
       </c>
       <c r="E17" s="18" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909113911715</v>
+        <v>45958.940083390626</v>
       </c>
       <c r="F17" s="19" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14147,7 +14147,7 @@
       </c>
       <c r="K17" s="20" cm="1">
         <f t="array" aca="1" ref="K17" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>17.506699999999999</v>
+        <v>17.6127</v>
       </c>
       <c r="L17" s="21" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -14167,7 +14167,7 @@
       </c>
       <c r="P17" s="23" cm="1">
         <f t="array" aca="1" ref="P17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>6836444</v>
+        <v>6837700</v>
       </c>
       <c r="Q17" s="23" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14186,7 +14186,7 @@
       </c>
       <c r="V17" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.87057605826826723</v>
+        <v>0.87073600158517073</v>
       </c>
       <c r="W17" s="24"/>
       <c r="X17" s="108">
@@ -14230,7 +14230,7 @@
       </c>
       <c r="B18" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C18" t="e" vm="17">
         <v>#VALUE!</v>
@@ -14463,7 +14463,7 @@
       </c>
       <c r="B20" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C20" t="e" vm="19">
         <v>#VALUE!</v>
@@ -14474,7 +14474,7 @@
       </c>
       <c r="E20" s="18" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.887189200781</v>
+        <v>45958.926149108593</v>
       </c>
       <c r="F20" s="19" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14498,7 +14498,7 @@
       </c>
       <c r="K20" s="20" cm="1">
         <f t="array" aca="1" ref="K20" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>6.5233999999999996</v>
+        <v>6.5575999999999999</v>
       </c>
       <c r="L20" s="21" cm="1">
         <f t="array" aca="1" ref="L20" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -14518,7 +14518,7 @@
       </c>
       <c r="P20" s="23" cm="1">
         <f t="array" aca="1" ref="P20" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2201982</v>
+        <v>2201983</v>
       </c>
       <c r="Q20" s="23" cm="1">
         <f t="array" aca="1" ref="Q20" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14537,7 +14537,7 @@
       </c>
       <c r="V20" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.2842353284245827</v>
+        <v>1.2842359116424875</v>
       </c>
       <c r="W20" s="24"/>
       <c r="X20" s="108">
@@ -14581,7 +14581,7 @@
       </c>
       <c r="B21" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C21" t="e" vm="20">
         <v>#VALUE!</v>
@@ -14814,7 +14814,7 @@
       </c>
       <c r="B23" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C23" t="e" vm="22">
         <v>#VALUE!</v>
@@ -14825,7 +14825,7 @@
       </c>
       <c r="E23" s="18" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.900397753903</v>
+        <v>45958.941027372653</v>
       </c>
       <c r="F23" s="19" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14849,7 +14849,7 @@
       </c>
       <c r="K23" s="20" cm="1">
         <f t="array" aca="1" ref="K23" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>13.438599999999999</v>
+        <v>13.3444</v>
       </c>
       <c r="L23" s="21" cm="1">
         <f t="array" aca="1" ref="L23" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -14869,7 +14869,7 @@
       </c>
       <c r="P23" s="23" cm="1">
         <f t="array" aca="1" ref="P23" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>13069583</v>
+        <v>13070283</v>
       </c>
       <c r="Q23" s="23" cm="1">
         <f t="array" aca="1" ref="Q23" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14888,7 +14888,7 @@
       </c>
       <c r="V23" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.2608596327105788</v>
+        <v>1.2609271636901744</v>
       </c>
       <c r="W23" s="24"/>
       <c r="X23" s="108">
@@ -14932,7 +14932,7 @@
       </c>
       <c r="B24" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C24" t="e" vm="23">
         <v>#VALUE!</v>
@@ -14943,7 +14943,7 @@
       </c>
       <c r="E24" s="18" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.90992578672</v>
+        <v>45958.94344538125</v>
       </c>
       <c r="F24" s="19" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14987,7 +14987,7 @@
       </c>
       <c r="P24" s="23" cm="1">
         <f t="array" aca="1" ref="P24" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>38276997</v>
+        <v>38281692</v>
       </c>
       <c r="Q24" s="23" cm="1">
         <f t="array" aca="1" ref="Q24" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15006,7 +15006,7 @@
       </c>
       <c r="V24" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0897244699631805</v>
+        <v>1.089858133959509</v>
       </c>
       <c r="W24" s="24"/>
       <c r="X24" s="108">
@@ -15050,7 +15050,7 @@
       </c>
       <c r="B25" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C25" t="e" vm="24">
         <v>#VALUE!</v>
@@ -15061,7 +15061,7 @@
       </c>
       <c r="E25" s="18" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.899425647658</v>
+        <v>45958.94359293906</v>
       </c>
       <c r="F25" s="19" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15073,7 +15073,7 @@
       </c>
       <c r="H25" s="19" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>28.07</v>
+        <v>28.065000000000001</v>
       </c>
       <c r="I25" s="19" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Low")</f>
@@ -15085,15 +15085,15 @@
       </c>
       <c r="K25" s="20" cm="1">
         <f t="array" aca="1" ref="K25" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>10.2255</v>
+        <v>10.170999999999999</v>
       </c>
       <c r="L25" s="21" cm="1">
         <f t="array" aca="1" ref="L25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>0.15</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="M25" s="22" cm="1">
         <f t="array" aca="1" ref="M25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>5.372E-3</v>
+        <v>5.1929999999999997E-3</v>
       </c>
       <c r="N25" s="19" cm="1">
         <f t="array" aca="1" ref="N25" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -15105,7 +15105,7 @@
       </c>
       <c r="P25" s="23" cm="1">
         <f t="array" aca="1" ref="P25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7420499</v>
+        <v>7421042</v>
       </c>
       <c r="Q25" s="23" cm="1">
         <f t="array" aca="1" ref="Q25" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15124,7 +15124,7 @@
       </c>
       <c r="V25" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.61247014305663627</v>
+        <v>0.61251496097086</v>
       </c>
       <c r="W25" s="24"/>
       <c r="X25" s="108">
@@ -15168,7 +15168,7 @@
       </c>
       <c r="B26" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C26" t="e" vm="25">
         <v>#VALUE!</v>
@@ -15286,7 +15286,7 @@
       </c>
       <c r="B27" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1398609369656903E-2</v>
+        <v>1.1390818999886093E-2</v>
       </c>
       <c r="C27" t="e" vm="26">
         <v>#VALUE!</v>
@@ -15297,7 +15297,7 @@
       </c>
       <c r="E27" s="18" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.898698969533</v>
+        <v>45958.932910844531</v>
       </c>
       <c r="F27" s="26" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15341,7 +15341,7 @@
       </c>
       <c r="P27" s="23" cm="1">
         <f t="array" aca="1" ref="P27" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>4366255</v>
+        <v>4366732</v>
       </c>
       <c r="Q27" s="23" cm="1">
         <f t="array" aca="1" ref="Q27" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15360,7 +15360,7 @@
       </c>
       <c r="V27" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.71336459362976157</v>
+        <v>0.71344252652904516</v>
       </c>
       <c r="W27" s="24"/>
       <c r="X27" s="108">
@@ -15402,7 +15402,7 @@
       </c>
       <c r="B28" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C28" t="e" vm="27">
         <v>#VALUE!</v>
@@ -15520,7 +15520,7 @@
       </c>
       <c r="B29" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C29" t="e" vm="28">
         <v>#VALUE!</v>
@@ -15531,7 +15531,7 @@
       </c>
       <c r="E29" s="18" cm="1">
         <f t="array" aca="1" ref="E29" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909650671092</v>
+        <v>45958.943745995311</v>
       </c>
       <c r="F29" s="19" cm="1">
         <f t="array" aca="1" ref="F29" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15575,7 +15575,7 @@
       </c>
       <c r="P29" s="23" cm="1">
         <f t="array" aca="1" ref="P29" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>44204753</v>
+        <v>44297742</v>
       </c>
       <c r="Q29" s="23" cm="1">
         <f t="array" aca="1" ref="Q29" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15594,7 +15594,7 @@
       </c>
       <c r="V29" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.9662407638711534</v>
+        <v>2.9724805399963952</v>
       </c>
       <c r="W29" s="24"/>
       <c r="X29" s="108">
@@ -15638,7 +15638,7 @@
       </c>
       <c r="B30" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C30" t="e" vm="29">
         <v>#VALUE!</v>
@@ -15649,7 +15649,7 @@
       </c>
       <c r="E30" s="18" cm="1">
         <f t="array" aca="1" ref="E30" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909992337503</v>
+        <v>45958.943806099218</v>
       </c>
       <c r="F30" s="19" cm="1">
         <f t="array" aca="1" ref="F30" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15693,7 +15693,7 @@
       </c>
       <c r="P30" s="23" cm="1">
         <f t="array" aca="1" ref="P30" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8795295</v>
+        <v>8806254</v>
       </c>
       <c r="Q30" s="23" cm="1">
         <f t="array" aca="1" ref="Q30" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15712,7 +15712,7 @@
       </c>
       <c r="V30" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.97848343158816831</v>
+        <v>0.97970262888931336</v>
       </c>
       <c r="W30" s="24"/>
       <c r="X30" s="108">
@@ -15756,7 +15756,7 @@
       </c>
       <c r="B31" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C31" t="e" vm="30">
         <v>#VALUE!</v>
@@ -15767,7 +15767,7 @@
       </c>
       <c r="E31" s="18" cm="1">
         <f t="array" aca="1" ref="E31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910000555472</v>
+        <v>45958.943671145309</v>
       </c>
       <c r="F31" s="19" cm="1">
         <f t="array" aca="1" ref="F31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15811,7 +15811,7 @@
       </c>
       <c r="P31" s="23" cm="1">
         <f t="array" aca="1" ref="P31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>29888043</v>
+        <v>29922694</v>
       </c>
       <c r="Q31" s="23" cm="1">
         <f t="array" aca="1" ref="Q31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15830,7 +15830,7 @@
       </c>
       <c r="V31" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.7373264230995258</v>
+        <v>1.7393406097723307</v>
       </c>
       <c r="W31" s="24"/>
       <c r="X31" s="108">
@@ -15874,7 +15874,7 @@
       </c>
       <c r="B32" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C32" t="e" vm="31">
         <v>#VALUE!</v>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="E32" s="18" cm="1">
         <f t="array" aca="1" ref="E32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909818402346</v>
+        <v>45958.942795242969</v>
       </c>
       <c r="F32" s="19" cm="1">
         <f t="array" aca="1" ref="F32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15929,7 +15929,7 @@
       </c>
       <c r="P32" s="23" cm="1">
         <f t="array" aca="1" ref="P32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>13988213</v>
+        <v>13992118</v>
       </c>
       <c r="Q32" s="23" cm="1">
         <f t="array" aca="1" ref="Q32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15948,7 +15948,7 @@
       </c>
       <c r="V32" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3644530473084797</v>
+        <v>1.3648339529430837</v>
       </c>
       <c r="W32" s="24"/>
       <c r="X32" s="108">
@@ -15992,7 +15992,7 @@
       </c>
       <c r="B33" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C33" t="e" vm="32">
         <v>#VALUE!</v>
@@ -16003,7 +16003,7 @@
       </c>
       <c r="E33" s="18" cm="1">
         <f t="array" aca="1" ref="E33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908327580466</v>
+        <v>45958.943397615622</v>
       </c>
       <c r="F33" s="19" cm="1">
         <f t="array" aca="1" ref="F33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16027,7 +16027,7 @@
       </c>
       <c r="K33" s="20" cm="1">
         <f t="array" aca="1" ref="K33" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>12.3279</v>
+        <v>12.218999999999999</v>
       </c>
       <c r="L33" s="21" cm="1">
         <f t="array" aca="1" ref="L33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -16047,7 +16047,7 @@
       </c>
       <c r="P33" s="23" cm="1">
         <f t="array" aca="1" ref="P33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>13301476</v>
+        <v>13324419</v>
       </c>
       <c r="Q33" s="23" cm="1">
         <f t="array" aca="1" ref="Q33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16066,7 +16066,7 @@
       </c>
       <c r="V33" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0516704247193873</v>
+        <v>1.0534843944287893</v>
       </c>
       <c r="W33" s="24"/>
       <c r="X33" s="108">
@@ -16110,7 +16110,7 @@
       </c>
       <c r="B34" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C34" t="e" vm="33">
         <v>#VALUE!</v>
@@ -16121,7 +16121,7 @@
       </c>
       <c r="E34" s="18" cm="1">
         <f t="array" aca="1" ref="E34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910047198435</v>
+        <v>45958.943193796091</v>
       </c>
       <c r="F34" s="19" cm="1">
         <f t="array" aca="1" ref="F34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16145,7 +16145,7 @@
       </c>
       <c r="K34" s="20" cm="1">
         <f t="array" aca="1" ref="K34" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>46.056899999999999</v>
+        <v>45.725099999999998</v>
       </c>
       <c r="L34" s="21" cm="1">
         <f t="array" aca="1" ref="L34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -16165,7 +16165,7 @@
       </c>
       <c r="P34" s="23" cm="1">
         <f t="array" aca="1" ref="P34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>4011831</v>
+        <v>4015473</v>
       </c>
       <c r="Q34" s="23" cm="1">
         <f t="array" aca="1" ref="Q34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16184,7 +16184,7 @@
       </c>
       <c r="V34" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0056231541701279</v>
+        <v>1.0065360738637759</v>
       </c>
       <c r="W34" s="24"/>
       <c r="X34" s="108">
@@ -16228,7 +16228,7 @@
       </c>
       <c r="B35" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C35" t="e" vm="34">
         <v>#VALUE!</v>
@@ -16239,7 +16239,7 @@
       </c>
       <c r="E35" s="18" cm="1">
         <f t="array" aca="1" ref="E35" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.905736041408</v>
+        <v>45958.941056053125</v>
       </c>
       <c r="F35" s="19" cm="1">
         <f t="array" aca="1" ref="F35" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16283,7 +16283,7 @@
       </c>
       <c r="P35" s="23" cm="1">
         <f t="array" aca="1" ref="P35" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>166174</v>
+        <v>167009</v>
       </c>
       <c r="Q35" s="23" cm="1">
         <f t="array" aca="1" ref="Q35" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16302,7 +16302,7 @@
       </c>
       <c r="V35" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.66536668962314016</v>
+        <v>0.66871005974021813</v>
       </c>
       <c r="W35" s="24"/>
       <c r="X35" s="108">
@@ -16346,7 +16346,7 @@
       </c>
       <c r="B36" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C36" t="e" vm="35">
         <v>#VALUE!</v>
@@ -16357,7 +16357,7 @@
       </c>
       <c r="E36" s="18" cm="1">
         <f t="array" aca="1" ref="E36" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909128020314</v>
+        <v>45958.941953633592</v>
       </c>
       <c r="F36" s="19" cm="1">
         <f t="array" aca="1" ref="F36" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16401,7 +16401,7 @@
       </c>
       <c r="P36" s="23" cm="1">
         <f t="array" aca="1" ref="P36" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>4950764</v>
+        <v>4955807</v>
       </c>
       <c r="Q36" s="23" cm="1">
         <f t="array" aca="1" ref="Q36" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16420,7 +16420,7 @@
       </c>
       <c r="V36" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.74546877630383446</v>
+        <v>0.74622813365532614</v>
       </c>
       <c r="W36" s="24"/>
       <c r="X36" s="108">
@@ -16464,7 +16464,7 @@
       </c>
       <c r="B37" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C37" t="e" vm="36">
         <v>#VALUE!</v>
@@ -16582,7 +16582,7 @@
       </c>
       <c r="B38" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C38" t="e" vm="37">
         <v>#VALUE!</v>
@@ -16593,7 +16593,7 @@
       </c>
       <c r="E38" s="18" cm="1">
         <f t="array" aca="1" ref="E38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909776029686</v>
+        <v>45958.942199074074</v>
       </c>
       <c r="F38" s="19" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16637,7 +16637,7 @@
       </c>
       <c r="P38" s="23" cm="1">
         <f t="array" aca="1" ref="P38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>11982812</v>
+        <v>12042192</v>
       </c>
       <c r="Q38" s="23" cm="1">
         <f t="array" aca="1" ref="Q38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16656,7 +16656,7 @@
       </c>
       <c r="V38" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.74740184435198154</v>
+        <v>0.75110554274244457</v>
       </c>
       <c r="W38" s="24"/>
       <c r="X38" s="108">
@@ -16818,7 +16818,7 @@
       </c>
       <c r="B40" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C40" t="e" vm="39">
         <v>#VALUE!</v>
@@ -16936,7 +16936,7 @@
       </c>
       <c r="B41" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C41" t="e" vm="40">
         <v>#VALUE!</v>
@@ -17064,7 +17064,7 @@
       </c>
       <c r="E42" s="18" cm="1">
         <f t="array" aca="1" ref="E42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.8125</v>
+        <v>45958.929780092592</v>
       </c>
       <c r="F42" s="28" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17284,7 +17284,7 @@
       </c>
       <c r="B44" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C44" t="e" vm="43">
         <v>#VALUE!</v>
@@ -17295,7 +17295,7 @@
       </c>
       <c r="E44" s="18" cm="1">
         <f t="array" aca="1" ref="E44" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.907723460157</v>
+        <v>45958.942481747654</v>
       </c>
       <c r="F44" s="19" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17339,7 +17339,7 @@
       </c>
       <c r="P44" s="23" cm="1">
         <f t="array" aca="1" ref="P44" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>768463</v>
+        <v>769725</v>
       </c>
       <c r="Q44" s="23" cm="1">
         <f t="array" aca="1" ref="Q44" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17358,7 +17358,7 @@
       </c>
       <c r="V44" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.67811981017025735</v>
+        <v>0.67923344504979588</v>
       </c>
       <c r="W44" s="24"/>
       <c r="X44" s="108">
@@ -17402,7 +17402,7 @@
       </c>
       <c r="B45" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C45" t="e" vm="44">
         <v>#VALUE!</v>
@@ -17413,7 +17413,7 @@
       </c>
       <c r="E45" s="18" cm="1">
         <f t="array" aca="1" ref="E45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910039560156</v>
+        <v>45958.943851689066</v>
       </c>
       <c r="F45" s="19" cm="1">
         <f t="array" aca="1" ref="F45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17457,7 +17457,7 @@
       </c>
       <c r="P45" s="23" cm="1">
         <f t="array" aca="1" ref="P45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>79864797</v>
+        <v>79959008</v>
       </c>
       <c r="Q45" s="23" cm="1">
         <f t="array" aca="1" ref="Q45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17476,7 +17476,7 @@
       </c>
       <c r="V45" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.88458652383582681</v>
+        <v>0.88563000962841065</v>
       </c>
       <c r="W45" s="24"/>
       <c r="X45" s="108">
@@ -17521,7 +17521,7 @@
       </c>
       <c r="B46" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C46" t="e" vm="45">
         <v>#VALUE!</v>
@@ -17532,7 +17532,7 @@
       </c>
       <c r="E46" s="18" cm="1">
         <f t="array" aca="1" ref="E46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909872395314</v>
+        <v>45958.943793957813</v>
       </c>
       <c r="F46" s="19" cm="1">
         <f t="array" aca="1" ref="F46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17576,7 +17576,7 @@
       </c>
       <c r="P46" s="23" cm="1">
         <f t="array" aca="1" ref="P46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>11750610</v>
+        <v>11766814</v>
       </c>
       <c r="Q46" s="23" cm="1">
         <f t="array" aca="1" ref="Q46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17595,7 +17595,7 @@
       </c>
       <c r="V46" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.83482291163726774</v>
+        <v>0.83597412595381559</v>
       </c>
       <c r="W46" s="24"/>
       <c r="X46" s="108">
@@ -17639,7 +17639,7 @@
       </c>
       <c r="B47" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C47" t="e" vm="46">
         <v>#VALUE!</v>
@@ -17872,7 +17872,7 @@
       </c>
       <c r="B49" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C49" t="e" vm="48">
         <v>#VALUE!</v>
@@ -18106,7 +18106,7 @@
       </c>
       <c r="B51" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C51" t="e" vm="50">
         <v>#VALUE!</v>
@@ -18117,7 +18117,7 @@
       </c>
       <c r="E51" s="18" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.90942290469</v>
+        <v>45958.925457928126</v>
       </c>
       <c r="F51" s="19" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18161,7 +18161,7 @@
       </c>
       <c r="P51" s="23" cm="1">
         <f t="array" aca="1" ref="P51" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7206114</v>
+        <v>7206296</v>
       </c>
       <c r="Q51" s="23" cm="1">
         <f t="array" aca="1" ref="Q51" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18180,7 +18180,7 @@
       </c>
       <c r="V51" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0001565582500784</v>
+        <v>1.0001818185351088</v>
       </c>
       <c r="W51" s="24"/>
       <c r="X51" s="108">
@@ -18224,7 +18224,7 @@
       </c>
       <c r="B52" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C52" t="e" vm="51">
         <v>#VALUE!</v>
@@ -18342,7 +18342,7 @@
       </c>
       <c r="B53" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C53" t="e" vm="52">
         <v>#VALUE!</v>
@@ -18353,7 +18353,7 @@
       </c>
       <c r="E53" s="18" cm="1">
         <f t="array" aca="1" ref="E53" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908892303123</v>
+        <v>45958.941021376566</v>
       </c>
       <c r="F53" s="19" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18397,7 +18397,7 @@
       </c>
       <c r="P53" s="23" cm="1">
         <f t="array" aca="1" ref="P53" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>9526062</v>
+        <v>9526590</v>
       </c>
       <c r="Q53" s="23" cm="1">
         <f t="array" aca="1" ref="Q53" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18416,7 +18416,7 @@
       </c>
       <c r="V53" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.69814816049857098</v>
+        <v>0.69818685668055502</v>
       </c>
       <c r="W53" s="24"/>
       <c r="X53" s="108">
@@ -18460,7 +18460,7 @@
       </c>
       <c r="B54" s="15">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C54" t="e" vm="53">
         <v>#VALUE!</v>
@@ -18698,7 +18698,7 @@
       </c>
       <c r="B56" s="58">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C56" t="e" vm="15">
         <v>#VALUE!</v>
@@ -18709,7 +18709,7 @@
       </c>
       <c r="E56" s="62" cm="1">
         <f t="array" aca="1" ref="E56" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.904932650003</v>
+        <v>45958.94197274297</v>
       </c>
       <c r="F56" s="61" cm="1">
         <f t="array" aca="1" ref="F56" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18753,7 +18753,7 @@
       </c>
       <c r="P56" s="66" cm="1">
         <f t="array" aca="1" ref="P56" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>5964314</v>
+        <v>6002660</v>
       </c>
       <c r="Q56" s="66" cm="1">
         <f t="array" aca="1" ref="Q56" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18775,7 +18775,7 @@
       </c>
       <c r="V56" s="94">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.1743232885149</v>
+        <v>1.1818732935651692</v>
       </c>
       <c r="W56" s="94"/>
       <c r="X56" s="108">
@@ -19184,7 +19184,7 @@
       </c>
       <c r="B60" s="58">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C60" t="e" vm="21">
         <v>#VALUE!</v>
@@ -19679,7 +19679,7 @@
       </c>
       <c r="E64" s="62" cm="1">
         <f t="array" aca="1" ref="E64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.8125</v>
+        <v>45958.929780092592</v>
       </c>
       <c r="F64" s="68" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -19909,7 +19909,7 @@
       </c>
       <c r="B66" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C66" t="e" vm="1">
         <v>#VALUE!</v>
@@ -19920,7 +19920,7 @@
       </c>
       <c r="E66" s="18" cm="1">
         <f t="array" aca="1" ref="E66" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909980022654</v>
+        <v>45958.9436489</v>
       </c>
       <c r="F66" s="19" cm="1">
         <f t="array" aca="1" ref="F66" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -19964,7 +19964,7 @@
       </c>
       <c r="P66" s="23" cm="1">
         <f t="array" aca="1" ref="P66" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>41443517</v>
+        <v>41473172</v>
       </c>
       <c r="Q66" s="23" cm="1">
         <f t="array" aca="1" ref="Q66" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19986,7 +19986,7 @@
       </c>
       <c r="V66" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.91676510252840016</v>
+        <v>0.91742109581959397</v>
       </c>
       <c r="W66" s="24"/>
       <c r="X66" s="108">
@@ -20030,7 +20030,7 @@
       </c>
       <c r="B67" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C67" t="e" vm="4">
         <v>#VALUE!</v>
@@ -20041,7 +20041,7 @@
       </c>
       <c r="E67" s="18" cm="1">
         <f t="array" aca="1" ref="E67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910078495312</v>
+        <v>45958.943784490628</v>
       </c>
       <c r="F67" s="19" cm="1">
         <f t="array" aca="1" ref="F67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20085,7 +20085,7 @@
       </c>
       <c r="P67" s="23" cm="1">
         <f t="array" aca="1" ref="P67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>46903995</v>
+        <v>46991794</v>
       </c>
       <c r="Q67" s="23" cm="1">
         <f t="array" aca="1" ref="Q67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20107,7 +20107,7 @@
       </c>
       <c r="V67" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0320873491369196</v>
+        <v>1.0340193005019764</v>
       </c>
       <c r="W67" s="24"/>
       <c r="X67" s="108">
@@ -20271,7 +20271,7 @@
       </c>
       <c r="B69" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C69" t="e" vm="15">
         <v>#VALUE!</v>
@@ -20282,7 +20282,7 @@
       </c>
       <c r="E69" s="18" cm="1">
         <f t="array" aca="1" ref="E69" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.904932650003</v>
+        <v>45958.94197274297</v>
       </c>
       <c r="F69" s="19" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20326,7 +20326,7 @@
       </c>
       <c r="P69" s="23" cm="1">
         <f t="array" aca="1" ref="P69" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>5964314</v>
+        <v>6002660</v>
       </c>
       <c r="Q69" s="23" cm="1">
         <f t="array" aca="1" ref="Q69" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20348,7 +20348,7 @@
       </c>
       <c r="V69" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.1743232885149</v>
+        <v>1.1818732935651692</v>
       </c>
       <c r="W69" s="24"/>
       <c r="X69" s="108">
@@ -20392,7 +20392,7 @@
       </c>
       <c r="B70" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C70" t="e" vm="16">
         <v>#VALUE!</v>
@@ -20403,7 +20403,7 @@
       </c>
       <c r="E70" s="18" cm="1">
         <f t="array" aca="1" ref="E70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909113911715</v>
+        <v>45958.940083390626</v>
       </c>
       <c r="F70" s="19" cm="1">
         <f t="array" aca="1" ref="F70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20427,7 +20427,7 @@
       </c>
       <c r="K70" s="20" cm="1">
         <f t="array" aca="1" ref="K70" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>17.506699999999999</v>
+        <v>17.6127</v>
       </c>
       <c r="L70" s="21" cm="1">
         <f t="array" aca="1" ref="L70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -20447,7 +20447,7 @@
       </c>
       <c r="P70" s="23" cm="1">
         <f t="array" aca="1" ref="P70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>6836444</v>
+        <v>6837700</v>
       </c>
       <c r="Q70" s="23" cm="1">
         <f t="array" aca="1" ref="Q70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20469,7 +20469,7 @@
       </c>
       <c r="V70" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.87057605826826723</v>
+        <v>0.87073600158517073</v>
       </c>
       <c r="W70" s="24"/>
       <c r="X70" s="108">
@@ -20513,7 +20513,7 @@
       </c>
       <c r="B71" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C71" t="e" vm="22">
         <v>#VALUE!</v>
@@ -20524,7 +20524,7 @@
       </c>
       <c r="E71" s="18" cm="1">
         <f t="array" aca="1" ref="E71" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.900397753903</v>
+        <v>45958.941027372653</v>
       </c>
       <c r="F71" s="19" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20548,7 +20548,7 @@
       </c>
       <c r="K71" s="20" cm="1">
         <f t="array" aca="1" ref="K71" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>13.438599999999999</v>
+        <v>13.3444</v>
       </c>
       <c r="L71" s="21" cm="1">
         <f t="array" aca="1" ref="L71" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -20568,7 +20568,7 @@
       </c>
       <c r="P71" s="23" cm="1">
         <f t="array" aca="1" ref="P71" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>13069583</v>
+        <v>13070283</v>
       </c>
       <c r="Q71" s="23" cm="1">
         <f t="array" aca="1" ref="Q71" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20590,7 +20590,7 @@
       </c>
       <c r="V71" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.2608596327105788</v>
+        <v>1.2609271636901744</v>
       </c>
       <c r="W71" s="24"/>
       <c r="X71" s="108">
@@ -20634,7 +20634,7 @@
       </c>
       <c r="B72" s="40">
         <f ca="1">D101/100</f>
-        <v>1.1398609369656903E-2</v>
+        <v>1.1390818999886093E-2</v>
       </c>
       <c r="C72" t="e" vm="25">
         <v>#VALUE!</v>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="B73" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C73" t="e" vm="29">
         <v>#VALUE!</v>
@@ -20766,7 +20766,7 @@
       </c>
       <c r="E73" s="18" cm="1">
         <f t="array" aca="1" ref="E73" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909992337503</v>
+        <v>45958.943806099218</v>
       </c>
       <c r="F73" s="19" cm="1">
         <f t="array" aca="1" ref="F73" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20810,7 +20810,7 @@
       </c>
       <c r="P73" s="23" cm="1">
         <f t="array" aca="1" ref="P73" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8795295</v>
+        <v>8806254</v>
       </c>
       <c r="Q73" s="23" cm="1">
         <f t="array" aca="1" ref="Q73" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20832,7 +20832,7 @@
       </c>
       <c r="V73" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.97848343158816831</v>
+        <v>0.97970262888931336</v>
       </c>
       <c r="W73" s="24"/>
       <c r="X73" s="108">
@@ -20876,7 +20876,7 @@
       </c>
       <c r="B74" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C74" t="e" vm="57">
         <v>#VALUE!</v>
@@ -20887,7 +20887,7 @@
       </c>
       <c r="E74" s="18" cm="1">
         <f t="array" aca="1" ref="E74" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908117753905</v>
+        <v>45958.940159478909</v>
       </c>
       <c r="F74" s="19" cm="1">
         <f t="array" aca="1" ref="F74" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20931,7 +20931,7 @@
       </c>
       <c r="P74" s="23" cm="1">
         <f t="array" aca="1" ref="P74" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>3360064</v>
+        <v>3391431</v>
       </c>
       <c r="Q74" s="23" cm="1">
         <f t="array" aca="1" ref="Q74" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20950,7 +20950,7 @@
       </c>
       <c r="V74" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.52347156614256629</v>
+        <v>0.52835829824504832</v>
       </c>
       <c r="W74" s="24"/>
       <c r="X74" s="108">
@@ -21109,7 +21109,7 @@
       </c>
       <c r="B76" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1398609369656903E-2</v>
+        <v>1.1390818999886093E-2</v>
       </c>
       <c r="C76" t="e" vm="58">
         <v>#VALUE!</v>
@@ -21225,7 +21225,7 @@
       </c>
       <c r="B77" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C77" t="e" vm="59">
         <v>#VALUE!</v>
@@ -21236,7 +21236,7 @@
       </c>
       <c r="E77" s="18" cm="1">
         <f t="array" aca="1" ref="E77" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909672256254</v>
+        <v>45958.943636180469</v>
       </c>
       <c r="F77" s="19" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21280,7 +21280,7 @@
       </c>
       <c r="P77" s="23" cm="1">
         <f t="array" aca="1" ref="P77" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>96684145</v>
+        <v>96698107</v>
       </c>
       <c r="Q77" s="23" cm="1">
         <f t="array" aca="1" ref="Q77" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21299,7 +21299,7 @@
       </c>
       <c r="V77" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.71937373448143083</v>
+        <v>0.71947761807145305</v>
       </c>
       <c r="W77" s="24"/>
       <c r="X77" s="108">
@@ -21458,7 +21458,7 @@
       </c>
       <c r="B79" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C79" t="e" vm="60">
         <v>#VALUE!</v>
@@ -21469,7 +21469,7 @@
       </c>
       <c r="E79" s="18" cm="1">
         <f t="array" aca="1" ref="E79" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909938946097</v>
+        <v>45958.943650161717</v>
       </c>
       <c r="F79" s="19" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21513,7 +21513,7 @@
       </c>
       <c r="P79" s="23" cm="1">
         <f t="array" aca="1" ref="P79" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>1580869</v>
+        <v>1581906</v>
       </c>
       <c r="Q79" s="23" cm="1">
         <f t="array" aca="1" ref="Q79" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21532,7 +21532,7 @@
       </c>
       <c r="V79" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.5307254942590616</v>
+        <v>1.5317296017072732</v>
       </c>
       <c r="W79" s="24"/>
       <c r="X79" s="108">
@@ -21576,7 +21576,7 @@
       </c>
       <c r="B80" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C80" t="e" vm="61">
         <v>#VALUE!</v>
@@ -21587,7 +21587,7 @@
       </c>
       <c r="E80" s="18" cm="1">
         <f t="array" aca="1" ref="E80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.907151620311</v>
+        <v>45958.943829351563</v>
       </c>
       <c r="F80" s="19" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21631,7 +21631,7 @@
       </c>
       <c r="P80" s="23" cm="1">
         <f t="array" aca="1" ref="P80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>1241106</v>
+        <v>1241487</v>
       </c>
       <c r="Q80" s="23" cm="1">
         <f t="array" aca="1" ref="Q80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21650,7 +21650,7 @@
       </c>
       <c r="V80" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.59904807276002425</v>
+        <v>0.59923197108597026</v>
       </c>
       <c r="W80" s="24"/>
       <c r="X80" s="108">
@@ -21694,7 +21694,7 @@
       </c>
       <c r="B81" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C81" t="e" vm="62">
         <v>#VALUE!</v>
@@ -21705,7 +21705,7 @@
       </c>
       <c r="E81" s="18" cm="1">
         <f t="array" aca="1" ref="E81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.91002387656</v>
+        <v>45958.94355054375</v>
       </c>
       <c r="F81" s="19" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21749,7 +21749,7 @@
       </c>
       <c r="P81" s="23" cm="1">
         <f t="array" aca="1" ref="P81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>6259469</v>
+        <v>6278163</v>
       </c>
       <c r="Q81" s="23" cm="1">
         <f t="array" aca="1" ref="Q81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21768,7 +21768,7 @@
       </c>
       <c r="V81" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.82528086650767019</v>
+        <v>0.82774558045041746</v>
       </c>
       <c r="W81" s="24"/>
       <c r="X81" s="108">
@@ -21812,7 +21812,7 @@
       </c>
       <c r="B82" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C82" t="e" vm="63">
         <v>#VALUE!</v>
@@ -21823,7 +21823,7 @@
       </c>
       <c r="E82" s="18" cm="1">
         <f t="array" aca="1" ref="E82" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.908607094534</v>
+        <v>45958.936456353906</v>
       </c>
       <c r="F82" s="19" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21867,7 +21867,7 @@
       </c>
       <c r="P82" s="23" cm="1">
         <f t="array" aca="1" ref="P82" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>11372613</v>
+        <v>11375037</v>
       </c>
       <c r="Q82" s="23" cm="1">
         <f t="array" aca="1" ref="Q82" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21886,7 +21886,7 @@
       </c>
       <c r="V82" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.152956730564521</v>
+        <v>1.1532024759455419</v>
       </c>
       <c r="W82" s="24"/>
       <c r="X82" s="108">
@@ -21930,7 +21930,7 @@
       </c>
       <c r="B83" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C83" t="e" vm="64">
         <v>#VALUE!</v>
@@ -21941,7 +21941,7 @@
       </c>
       <c r="E83" s="18" cm="1">
         <f t="array" aca="1" ref="E83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.907810601566</v>
+        <v>45958.937443437499</v>
       </c>
       <c r="F83" s="19" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21965,7 +21965,7 @@
       </c>
       <c r="K83" s="20" cm="1">
         <f t="array" aca="1" ref="K83" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>38.183999999999997</v>
+        <v>38.599400000000003</v>
       </c>
       <c r="L83" s="21" cm="1">
         <f t="array" aca="1" ref="L83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -21985,7 +21985,7 @@
       </c>
       <c r="P83" s="23" cm="1">
         <f t="array" aca="1" ref="P83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2915551</v>
+        <v>2915979</v>
       </c>
       <c r="Q83" s="23" cm="1">
         <f t="array" aca="1" ref="Q83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22004,7 +22004,7 @@
       </c>
       <c r="V83" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.1281389418779673</v>
+        <v>1.1283045515576209</v>
       </c>
       <c r="W83" s="24"/>
       <c r="X83" s="108">
@@ -22048,7 +22048,7 @@
       </c>
       <c r="B84" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C84" t="e" vm="65">
         <v>#VALUE!</v>
@@ -22059,7 +22059,7 @@
       </c>
       <c r="E84" s="18" cm="1">
         <f t="array" aca="1" ref="E84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.896075346878</v>
+        <v>45958.938877638284</v>
       </c>
       <c r="F84" s="19" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22083,7 +22083,7 @@
       </c>
       <c r="K84" s="20" cm="1">
         <f t="array" aca="1" ref="K84" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>3.7250999999999999</v>
+        <v>3.8037000000000001</v>
       </c>
       <c r="L84" s="21" cm="1">
         <f t="array" aca="1" ref="L84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -22103,7 +22103,7 @@
       </c>
       <c r="P84" s="23" cm="1">
         <f t="array" aca="1" ref="P84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2092861</v>
+        <v>2100770</v>
       </c>
       <c r="Q84" s="23" cm="1">
         <f t="array" aca="1" ref="Q84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22122,7 +22122,7 @@
       </c>
       <c r="V84" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.47345168978959523</v>
+        <v>0.47524088143421278</v>
       </c>
       <c r="W84" s="24"/>
       <c r="X84" s="108">
@@ -22166,7 +22166,7 @@
       </c>
       <c r="B85" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C85" t="e" vm="66">
         <v>#VALUE!</v>
@@ -22177,7 +22177,7 @@
       </c>
       <c r="E85" s="18" cm="1">
         <f t="array" aca="1" ref="E85" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.904235138281</v>
+        <v>45958.934662800784</v>
       </c>
       <c r="F85" s="19" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22221,7 +22221,7 @@
       </c>
       <c r="P85" s="23" cm="1">
         <f t="array" aca="1" ref="P85" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>4630509</v>
+        <v>4630798</v>
       </c>
       <c r="Q85" s="23" cm="1">
         <f t="array" aca="1" ref="Q85" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22240,7 +22240,7 @@
       </c>
       <c r="V85" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.954308318047691</v>
+        <v>2.9544927027673658</v>
       </c>
       <c r="W85" s="24"/>
       <c r="X85" s="108">
@@ -22399,7 +22399,7 @@
       </c>
       <c r="B87" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C87" t="e" vm="67">
         <v>#VALUE!</v>
@@ -22410,7 +22410,7 @@
       </c>
       <c r="E87" s="18" cm="1">
         <f t="array" aca="1" ref="E87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910058263282</v>
+        <v>45958.943697661722</v>
       </c>
       <c r="F87" s="19" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22454,7 +22454,7 @@
       </c>
       <c r="P87" s="23" cm="1">
         <f t="array" aca="1" ref="P87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>13283484</v>
+        <v>13291787</v>
       </c>
       <c r="Q87" s="23" cm="1">
         <f t="array" aca="1" ref="Q87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22473,7 +22473,7 @@
       </c>
       <c r="V87" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0983123664160008</v>
+        <v>1.0989988796514103</v>
       </c>
       <c r="W87" s="24"/>
       <c r="X87" s="108">
@@ -22517,7 +22517,7 @@
       </c>
       <c r="B88" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C88" t="e" vm="68">
         <v>#VALUE!</v>
@@ -22528,7 +22528,7 @@
       </c>
       <c r="E88" s="18" cm="1">
         <f t="array" aca="1" ref="E88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.910012685155</v>
+        <v>45958.943426921091</v>
       </c>
       <c r="F88" s="19" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22572,7 +22572,7 @@
       </c>
       <c r="P88" s="23" cm="1">
         <f t="array" aca="1" ref="P88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>50063446</v>
+        <v>50094470</v>
       </c>
       <c r="Q88" s="23" cm="1">
         <f t="array" aca="1" ref="Q88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22591,7 +22591,7 @@
       </c>
       <c r="V88" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.90877143684373418</v>
+        <v>0.90933459674001138</v>
       </c>
       <c r="W88" s="24"/>
       <c r="X88" s="108">
@@ -22635,7 +22635,7 @@
       </c>
       <c r="B89" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C89" t="e" vm="69">
         <v>#VALUE!</v>
@@ -22646,7 +22646,7 @@
       </c>
       <c r="E89" s="18" cm="1">
         <f t="array" aca="1" ref="E89" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.90961271953</v>
+        <v>45958.936144490624</v>
       </c>
       <c r="F89" s="19" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22690,7 +22690,7 @@
       </c>
       <c r="P89" s="23" cm="1">
         <f t="array" aca="1" ref="P89" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>53712232</v>
+        <v>53723268</v>
       </c>
       <c r="Q89" s="23" cm="1">
         <f t="array" aca="1" ref="Q89" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22709,7 +22709,7 @@
       </c>
       <c r="V89" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.8336271885451626</v>
+        <v>0.83379847000769403</v>
       </c>
       <c r="W89" s="24"/>
       <c r="X89" s="108">
@@ -22753,7 +22753,7 @@
       </c>
       <c r="B90" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C90" t="e" vm="70">
         <v>#VALUE!</v>
@@ -22764,7 +22764,7 @@
       </c>
       <c r="E90" s="18" cm="1">
         <f t="array" aca="1" ref="E90" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.891160474217</v>
+        <v>45958.92058277734</v>
       </c>
       <c r="F90" s="19" cm="1">
         <f t="array" aca="1" ref="F90" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22788,7 +22788,7 @@
       </c>
       <c r="K90" s="20" cm="1">
         <f t="array" aca="1" ref="K90" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>33.154000000000003</v>
+        <v>33.502499999999998</v>
       </c>
       <c r="L90" s="21" cm="1">
         <f t="array" aca="1" ref="L90" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
@@ -22808,7 +22808,7 @@
       </c>
       <c r="P90" s="23" cm="1">
         <f t="array" aca="1" ref="P90" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2553001</v>
+        <v>2553012</v>
       </c>
       <c r="Q90" s="23" cm="1">
         <f t="array" aca="1" ref="Q90" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22827,7 +22827,7 @@
       </c>
       <c r="V90" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.84794800317125119</v>
+        <v>0.84795165668648087</v>
       </c>
       <c r="W90" s="24"/>
       <c r="X90" s="108">
@@ -22871,7 +22871,7 @@
       </c>
       <c r="B91" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C91" t="e" vm="71">
         <v>#VALUE!</v>
@@ -22882,7 +22882,7 @@
       </c>
       <c r="E91" s="18" cm="1">
         <f t="array" aca="1" ref="E91" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45958.909989293752</v>
+        <v>45958.939988853905</v>
       </c>
       <c r="F91" s="19" cm="1">
         <f t="array" aca="1" ref="F91" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22926,7 +22926,7 @@
       </c>
       <c r="P91" s="23" cm="1">
         <f t="array" aca="1" ref="P91" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>3949441</v>
+        <v>3950889</v>
       </c>
       <c r="Q91" s="23" cm="1">
         <f t="array" aca="1" ref="Q91" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22945,7 +22945,7 @@
       </c>
       <c r="V91" s="24">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.69069717823383847</v>
+        <v>0.69095041141647939</v>
       </c>
       <c r="W91" s="24"/>
       <c r="X91" s="108">
@@ -22989,7 +22989,7 @@
       </c>
       <c r="B92" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C92" t="e" vm="72">
         <v>#VALUE!</v>
@@ -23107,7 +23107,7 @@
       </c>
       <c r="B93" s="40">
         <f ca="1">D99</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="C93" t="e" vm="73">
         <v>#VALUE!</v>
@@ -23593,7 +23593,7 @@
       <c r="K97"/>
       <c r="L97" s="21">
         <f ca="1">SUBTOTAL(101,RTData[Change])</f>
-        <v>0.17768829787234053</v>
+        <v>0.17763510638297889</v>
       </c>
       <c r="M97" s="44">
         <f ca="1">SUBTOTAL(104,RTData[Change%])</f>
@@ -23644,7 +23644,7 @@
       </c>
       <c r="B99" s="48" cm="1">
         <f t="array" aca="1" ref="B99" ca="1">_FV(A99,"Price")</f>
-        <v>1.1652</v>
+        <v>1.1651</v>
       </c>
       <c r="C99" s="49" cm="1">
         <f t="array" aca="1" ref="C99" ca="1">_FV(A99,"52 week high",TRUE)</f>
@@ -23652,7 +23652,7 @@
       </c>
       <c r="D99" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>0.85822176450394783</v>
+        <v>0.85829542528538316</v>
       </c>
       <c r="P99" s="50"/>
       <c r="R99"/>
@@ -23684,15 +23684,15 @@
       </c>
       <c r="B101" s="48" cm="1">
         <f t="array" aca="1" ref="B101" ca="1">_FV(A101,"Price")</f>
-        <v>0.87729999999999997</v>
+        <v>0.87790000000000001</v>
       </c>
       <c r="C101" s="53" cm="1">
         <f t="array" aca="1" ref="C101" ca="1">_FV(A101,"52 week high",TRUE)</f>
-        <v>0.87780000000000002</v>
+        <v>0.87829999999999997</v>
       </c>
       <c r="D101" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>1.1398609369656902</v>
+        <v>1.1390818999886092</v>
       </c>
       <c r="P101" s="50"/>
       <c r="R101"/>
@@ -23703,7 +23703,7 @@
       </c>
       <c r="B102" s="48" cm="1">
         <f t="array" aca="1" ref="B102" ca="1">_FV(A102,"Price")</f>
-        <v>1.7688999999999999</v>
+        <v>1.7693000000000001</v>
       </c>
       <c r="C102" s="49" cm="1">
         <f t="array" aca="1" ref="C102" ca="1">_FV(A102,"52 week high",TRUE)</f>
@@ -23711,7 +23711,7 @@
       </c>
       <c r="D102" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>0.56532308214144389</v>
+        <v>0.56519527496750122</v>
       </c>
       <c r="P102" s="50"/>
       <c r="R102"/>
@@ -23741,7 +23741,7 @@
       </c>
       <c r="B104" s="48" cm="1">
         <f t="array" aca="1" ref="B104" ca="1">_FV(A104,"Price")</f>
-        <v>152.06</v>
+        <v>152.15</v>
       </c>
       <c r="C104" s="54" cm="1">
         <f t="array" aca="1" ref="C104" ca="1">_FV(A104,"52 week high",TRUE)</f>
@@ -23749,7 +23749,7 @@
       </c>
       <c r="D104" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>6.576351440220965E-3</v>
+        <v>6.5724613867893522E-3</v>
       </c>
       <c r="J104"/>
       <c r="P104" s="50"/>
@@ -23761,7 +23761,7 @@
       </c>
       <c r="B105" s="48" cm="1">
         <f t="array" aca="1" ref="B105" ca="1">_FV(A105,"Price")</f>
-        <v>0.79339999999999999</v>
+        <v>0.79349999999999998</v>
       </c>
       <c r="C105" s="52" cm="1">
         <f t="array" aca="1" ref="C105" ca="1">_FV(A105,"52 week high",TRUE)</f>
@@ -23769,7 +23769,7 @@
       </c>
       <c r="D105" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>1.2603982858583311</v>
+        <v>1.260239445494644</v>
       </c>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.3">
@@ -23778,7 +23778,7 @@
       </c>
       <c r="B106" s="48" cm="1">
         <f t="array" aca="1" ref="B106" ca="1">_FV(A106,"Price")</f>
-        <v>0.75309999999999999</v>
+        <v>0.75349999999999995</v>
       </c>
       <c r="C106" s="53" cm="1">
         <f t="array" aca="1" ref="C106" ca="1">_FV(A106,"52 week high",TRUE)</f>
@@ -23786,7 +23786,7 @@
       </c>
       <c r="D106" s="19">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>1.3278449077147789</v>
+        <v>1.3271400132714002</v>
       </c>
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated MEDY and Speedy4
</commit_message>
<xml_diff>
--- a/MEDY.xlsx
+++ b/MEDY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4506D9-7DC8-F044-8200-3370B58F8AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD2B8C1-D143-474D-A9E8-4D714257D510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="1240" windowWidth="29880" windowHeight="18520" xr2:uid="{A82D0DB8-8028-8749-AD8E-3907692F5E1B}"/>
   </bookViews>
@@ -4088,7 +4088,7 @@
     <v>10690220000</v>
     <v>AMZN</v>
     <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
-    <v>73714</v>
+    <v>74470</v>
     <v>52729509</v>
     <v>1996</v>
   </rv>
@@ -4114,8 +4114,8 @@
     <v>1.53</v>
     <v>0.65</v>
     <v>0.96550000000000002</v>
-    <v>-2.1999999999999999E-2</v>
-    <v>-3.0556E-2</v>
+    <v>-5.3999999999999999E-2</v>
+    <v>-7.4999999999999997E-2</v>
     <v>EUR</v>
     <v>Dont Nod Entertainment SA is a France-based video game developer. The Company develops video games for consoles and personal computers (PC) based on original concepts and technologies. The Company specializes in narrative games in a number of genres, including adventure, action and role play. Its games are natively multi-screens (consoles, PCs, Smartphone, tablets, Mac and TV). Its game portfolio includes Remember me, which includes digitized personal and intimate memories; Life is Strange, which narrates the story of Max, a photography student who suddenly discovers an internal power to go back in time, and Vampyr, which depicts London in the early 20th century after it has been ravaged by the Spanish Flu.</v>
     <v>279</v>
@@ -4126,7 +4126,7 @@
     <v>0.72</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45975.432119490622</v>
+    <v>45975.435856481483</v>
     <v>12</v>
     <v>0.66200000000000003</v>
     <v>9026410</v>
@@ -4135,11 +4135,11 @@
     <v>0.72</v>
     <v>0</v>
     <v>0.72</v>
-    <v>0.69799999999999995</v>
+    <v>0.66600000000000004</v>
     <v>13081760</v>
     <v>ALDNE</v>
     <v>Dont Nod Entertainment SA (XPAR:ALDNE)</v>
-    <v>7681</v>
+    <v>10854</v>
     <v>5790</v>
     <v>2008</v>
   </rv>
@@ -4165,8 +4165,8 @@
     <v>938.6</v>
     <v>508.4</v>
     <v>2.1187999999999998</v>
-    <v>-23.8</v>
-    <v>-2.6998999999999999E-2</v>
+    <v>-22.1</v>
+    <v>-2.5071E-2</v>
     <v>EUR</v>
     <v>ASML Holding N.V. is a holding company based in the Netherlands. The Company operates through its subsidiaries in the Netherlands, the United States, Italy, France, Germany, the United Kingdom, Ireland, Belgium, South Korea, Taiwan, Singapore, China, Hong Kong, Japan, Malaysia and Israel. The Company operates through one business segment which is engage in development, production, marketing, sales, upgrading and servicing of advanced semiconductor equipment systems, consisting of lithography, metrology and inspection systems. The Company offers TWINSCAN systems, equipped with lithography system with a mercury lamp as light source (i-line), Krypton Fluoride (KrF) and Argon Fluoride (ArF) light sources for processing wafers for manufacturing environments for which imaging at a small resolution is required. TWINSCAN systems also include immersion lithography systems (TWINSCAN immersion systems).</v>
     <v>44000</v>
@@ -4177,20 +4177,20 @@
     <v>870</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45975.433807870373</v>
+    <v>45975.4372337963</v>
     <v>15</v>
     <v>854.1</v>
     <v>346150100000</v>
     <v>ASML Holding NV</v>
     <v>ASML Holding NV</v>
     <v>866.9</v>
-    <v>32.932600000000001</v>
+    <v>32.997900000000001</v>
     <v>881.5</v>
-    <v>857.7</v>
+    <v>859.4</v>
     <v>388147700</v>
     <v>ASML</v>
     <v>ASML Holding NV (XAMS:ASML)</v>
-    <v>153992</v>
+    <v>155625</v>
     <v>546390</v>
     <v>1994</v>
   </rv>
@@ -4241,7 +4241,7 @@
     <v>4722365000</v>
     <v>AVGO</v>
     <v>BROADCOM INC. (XNAS:AVGO)</v>
-    <v>35763</v>
+    <v>36270</v>
     <v>20679852</v>
     <v>2018</v>
   </rv>
@@ -4258,7 +4258,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-US</v>
     <v>a1o3qh</v>
     <v>268435456</v>
@@ -4292,7 +4292,7 @@
     <v>3101426000</v>
     <v>AZN</v>
     <v>ASTRAZENECA PLC (XNAS:AZN)</v>
-    <v>4563</v>
+    <v>4800</v>
     <v>5089321</v>
     <v>1992</v>
   </rv>
@@ -4669,7 +4669,7 @@
     <v>1797934000</v>
     <v>DIS</v>
     <v>THE WALT DISNEY COMPANY (XNYS:DIS)</v>
-    <v>7555</v>
+    <v>8260</v>
     <v>8219055</v>
     <v>2018</v>
   </rv>
@@ -4707,10 +4707,10 @@
     <v>24.04</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45975.433692129627</v>
+    <v>45975.437256944446</v>
     <v>49</v>
     <v>23.77</v>
-    <v>32235190000</v>
+    <v>32503480000</v>
     <v>Dassault Systemes SE</v>
     <v>Dassault Systemes SE</v>
     <v>24.01</v>
@@ -4720,7 +4720,7 @@
     <v>1341456000</v>
     <v>DSY</v>
     <v>Dassault Systemes SE (XPAR:DSY)</v>
-    <v>234662</v>
+    <v>236855</v>
     <v>1868320</v>
     <v>1981</v>
   </rv>
@@ -4848,8 +4848,8 @@
     <v>16.515000000000001</v>
     <v>7.3</v>
     <v>0.85529999999999995</v>
-    <v>-8.5000000000000006E-2</v>
-    <v>-5.5830000000000003E-3</v>
+    <v>-5.0000000000000001E-3</v>
+    <v>-3.2840000000000001E-4</v>
     <v>EUR</v>
     <v>E.ON SE is a Germany-based energy company. The Company’s core business is divided into two segments: Energy Networks and Customer Solutions. The Energy Networks segment includes power and gas distribution networks and related activities, divided into three regional markets: Germany, Sweden, and East-Central Europe/Turkey. Its main tasks are operating networks, maintenance, repairs, and network expansion, including customer connections and renewable energy integration. The Customer Solutions segment focuses on working with customers to support Europe's energy transition. It supplies power, gas, and heat, and offers solutions for energy efficiency, autonomy, and eMobility. The Company serves residential, Small and Medium enterprises (SME), commercial and industrial customers, sales partners, and public entities across locations. Energy Infrastructure Solutions also works on decarbonizing commercial customers, cities, and communities.</v>
     <v>78536</v>
@@ -4860,20 +4860,20 @@
     <v>15.225</v>
     <v>Multiline Utilities</v>
     <v>Stock</v>
-    <v>45975.433333333334</v>
+    <v>45975.436805555553</v>
     <v>58</v>
     <v>15.05</v>
     <v>40834790000</v>
     <v>E.ON SE</v>
     <v>E.ON SE</v>
     <v>15.225</v>
-    <v>12.5124</v>
+    <v>12.5785</v>
     <v>15.225</v>
-    <v>15.14</v>
+    <v>15.22</v>
     <v>2641319000</v>
     <v>EOAN</v>
     <v>E.ON SE (XFRA:EOAN)</v>
-    <v>8580</v>
+    <v>8610</v>
     <v>3872800</v>
     <v>2017</v>
   </rv>
@@ -5121,8 +5121,8 @@
     <v>429.3</v>
     <v>210</v>
     <v>2.2747999999999999</v>
-    <v>-8.1999999999999993</v>
-    <v>-2.0718E-2</v>
+    <v>-8.4</v>
+    <v>-2.1223000000000002E-2</v>
     <v>GBp</v>
     <v>International Consolidated Airlines Group, S.A. is a United Kingdom-based airline company that holds interests of airline and ancillary operations. The Company’s segments include British Airways, Iberia, Vueling, Aer Lingus, and IAG Loyalty. It operates various aircraft fleet services, including the Airbus A319ceo; Airbus A320ceo; Airbus A320neo; Airbus A321ceo; Airbus A321 LR; Airbus A321 XLR; Airbus A330-200; Boeing 737-8200; Boeing 777-200; Boeing 737-10; Boeing 777-300; Embraer E190, and others. The Company, through its subsidiaries, is engaged in providing airline operations, life insurance, air freight operations, cargo transport services and others. Its subsidiaries include AERL Holding Limited, British Airways Plc, IAG Cargo Limited, IAG GBS Limited, IAG Connect Limited, British Airways Avionic Engineering Limited and others. IAG Connect Limited provides an inflight eCommerce platform service. British Airways Avionic Engineering Limited provides aircraft maintenance services.</v>
     <v>74378</v>
@@ -5133,20 +5133,20 @@
     <v>392.7</v>
     <v>Passenger Transportation Services</v>
     <v>Stock</v>
-    <v>45975.433682233597</v>
+    <v>45975.437146122655</v>
     <v>76</v>
     <v>387</v>
     <v>17982000000</v>
     <v>International Consolidated Airlines Group SA</v>
     <v>International Consolidated Airlines Group SA</v>
     <v>391</v>
-    <v>6.9824999999999999</v>
+    <v>6.9789000000000003</v>
     <v>395.8</v>
-    <v>387.6</v>
+    <v>387.4</v>
     <v>4581400000</v>
     <v>IAG</v>
     <v>International Consolidated Airlines Group SA (XLON:IAG)</v>
-    <v>2337191</v>
+    <v>2389916</v>
     <v>19440160</v>
     <v>2009</v>
   </rv>
@@ -5417,7 +5417,7 @@
     <v>7432377000</v>
     <v>MSFT</v>
     <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
-    <v>30348</v>
+    <v>31936</v>
     <v>21942106</v>
     <v>1993</v>
   </rv>
@@ -5428,13 +5428,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1ye2w&amp;q=XNYS%3aNEE&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="8">
-    <v>19</v>
+  <rv s="1">
+    <v>0</v>
     <v>NEXTERA ENERGY, INC. (XNYS:NEE)</v>
     <v>2</v>
-    <v>20</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>21</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1ye2w</v>
     <v>268435456</v>
@@ -5465,11 +5465,10 @@
     <v>26.675000000000001</v>
     <v>85.89</v>
     <v>83.99</v>
-    <v>84</v>
     <v>2082610000</v>
     <v>NEE</v>
     <v>NEXTERA ENERGY, INC. (XNYS:NEE)</v>
-    <v>1291</v>
+    <v>1389</v>
     <v>9023713</v>
     <v>1984</v>
   </rv>
@@ -5520,7 +5519,7 @@
     <v>1091263000</v>
     <v>NEM</v>
     <v>NEWMONT CORPORATION (XNYS:NEM)</v>
-    <v>10701</v>
+    <v>10800</v>
     <v>12112852</v>
     <v>2001</v>
   </rv>
@@ -5571,7 +5570,7 @@
     <v>423732300</v>
     <v>NFLX</v>
     <v>NETFLIX, INC. (XNAS:NFLX)</v>
-    <v>6724</v>
+    <v>6736</v>
     <v>4512229</v>
     <v>1997</v>
   </rv>
@@ -5638,7 +5637,7 @@
     <v>2</v>
     <v>10</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1zfec</v>
     <v>268435456</v>
@@ -5774,7 +5773,7 @@
     <v>104373800</v>
     <v>POET</v>
     <v>POET Technologies Inc. (XNAS:POET)</v>
-    <v>49556</v>
+    <v>49844</v>
     <v>15414153</v>
     <v>2010</v>
   </rv>
@@ -5785,11 +5784,11 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a21g2w&amp;q=XNYS%3aPW&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="9">
-    <v>22</v>
+  <rv s="8">
+    <v>19</v>
     <v>POWER REIT (XNYS:PW)</v>
     <v>2</v>
-    <v>23</v>
+    <v>20</v>
     <v>Finance</v>
     <v>21</v>
     <v>en-US</v>
@@ -5914,7 +5913,7 @@
     <v>45.5</v>
     <v>Multiline Utilities</v>
     <v>Stock</v>
-    <v>45975.433333333334</v>
+    <v>45975.436805555553</v>
     <v>124</v>
     <v>45.13</v>
     <v>34856400000</v>
@@ -5953,8 +5952,8 @@
     <v>283.5</v>
     <v>209.7</v>
     <v>1.0482</v>
-    <v>-7.6</v>
-    <v>-3.4846000000000002E-2</v>
+    <v>-7.35</v>
+    <v>-3.3700000000000001E-2</v>
     <v>EUR</v>
     <v>SAP SE (SAP) is a Germany-based company. The Company provides business application software. It operates through three segments: Applications, Technology and Services, which engages in the sale of software licenses, subscriptions to its cloud-based applications and related services, primarily support services and various professional services, and support services, as well as implementation services for its software products and educational services on the use of its products; the SAP Business Network segment, which includes its cloud-based collaborative business networks and services related to the SAP Business Network, including cloud applications, professional services and educational services, as well as the Company markets and sells cloud offerings developed by SAP Ariba, SAP Fieldglass and Concur; and the Customer Experience segment, which comprises on-premise and cloud-based products that execute front office functions across the entire customer experience.</v>
     <v>110730</v>
@@ -5965,20 +5964,20 @@
     <v>214.2</v>
     <v>Software &amp; IT Services</v>
     <v>Stock</v>
-    <v>45975.43377314815</v>
+    <v>45975.437245370369</v>
     <v>127</v>
-    <v>210.4</v>
+    <v>210.35</v>
     <v>268305300000</v>
     <v>Sap Se</v>
     <v>Sap Se</v>
     <v>213.75</v>
-    <v>34.674199999999999</v>
+    <v>34.715400000000002</v>
     <v>218.1</v>
-    <v>210.5</v>
+    <v>210.75</v>
     <v>1228504000</v>
     <v>SAP</v>
     <v>Sap Se (XETR:SAP)</v>
-    <v>260937</v>
+    <v>263672</v>
     <v>1171450</v>
     <v>2014</v>
   </rv>
@@ -5993,7 +5992,7 @@
     <v>0</v>
     <v>Shin-Etsu Chemical Co., Ltd. (OTCM:SHECY)</v>
     <v>2</v>
-    <v>24</v>
+    <v>22</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -6131,7 +6130,7 @@
     <v>3325819000</v>
     <v>TSLA</v>
     <v>TESLA, INC. (XNAS:TSLA)</v>
-    <v>995766</v>
+    <v>1012731</v>
     <v>82861773</v>
     <v>2024</v>
   </rv>
@@ -6182,7 +6181,7 @@
     <v>5186523000</v>
     <v>TSM</v>
     <v>Taiwan Semiconductor Manufacturing Co., Ltd. (XNYS:TSM)</v>
-    <v>42049</v>
+    <v>42526</v>
     <v>14394948</v>
     <v>1987</v>
   </rv>
@@ -6197,7 +6196,7 @@
     <v>11</v>
     <v>Uniper SE (XFRA:UN0)</v>
     <v>2</v>
-    <v>25</v>
+    <v>23</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -6314,7 +6313,7 @@
     <v>13</v>
     <v>Volvo AB (OTCM:VLVLY)</v>
     <v>15</v>
-    <v>26</v>
+    <v>24</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -6366,7 +6365,7 @@
     <v>0</v>
     <v>Vontobel Holding Ltd (XSWX:VONN)</v>
     <v>2</v>
-    <v>27</v>
+    <v>25</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -6389,7 +6388,7 @@
     <v>60.1</v>
     <v>Investment Banking &amp; Investment Services</v>
     <v>Stock</v>
-    <v>45975.432430555556</v>
+    <v>45975.434641203705</v>
     <v>154</v>
     <v>59.8</v>
     <v>3435250000</v>
@@ -6563,10 +6562,10 @@
   <rv s="2">
     <v>164</v>
   </rv>
-  <rv s="10">
-    <v>28</v>
+  <rv s="9">
+    <v>26</v>
     <v>XPERI INC. (XNYS:XPER)</v>
-    <v>29</v>
+    <v>27</v>
     <v>3</v>
     <v>Finance</v>
     <v>5</v>
@@ -6613,13 +6612,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=ajezf2&amp;q=XMIL%3aENI&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="11">
-    <v>30</v>
+  <rv s="10">
+    <v>28</v>
     <v>Eni SpA (XMIL:ENI)</v>
     <v>2</v>
-    <v>31</v>
+    <v>29</v>
     <v>Finance</v>
-    <v>32</v>
+    <v>30</v>
     <v>en-US</v>
     <v>ajezf2</v>
     <v>268435456</v>
@@ -6628,8 +6627,8 @@
     <v>16.55</v>
     <v>11.01</v>
     <v>0.82950000000000002</v>
-    <v>-3.4000000000000002E-2</v>
-    <v>-2.0660000000000001E-3</v>
+    <v>-4.5999999999999999E-2</v>
+    <v>-2.7950000000000002E-3</v>
     <v>EUR</v>
     <v>Eni SpA (Eni) is an Italy-based company engaged in the exploration, development and production of hydrocarbons, in the supply and marketing of gas, liquefied natural gas (LNG) and power, in the refining and marketing of petroleum products, in the production and marketing of basic petrochemicals, plastics and elastomers and in commodity trading. The Company's segments include Exploration &amp; Production, Gas &amp; Power, and Refining &amp; Marketing. Its Exploration &amp; Production segment engages in oil and natural gas exploration and field development and production, as well as LNG operations in over 40 countries, including Italy, Libya, Egypt, Norway, the United Kingdom, Angola, Congo, Nigeria, the United States, Kazakhstan, Algeria, Australia, Venezuela, Iraq, Ghana and Mozambique. Its Gas &amp; Power segment engages in supply, trading and marketing of gas, LNG and electricity, international gas transport activities and commodity trading and derivatives.</v>
     <v>32356</v>
@@ -6640,20 +6639,20 @@
     <v>16.495999999999999</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45975.433831018519</v>
+    <v>45975.437175925923</v>
     <v>168</v>
     <v>16.338000000000001</v>
     <v>51701350000</v>
     <v>Eni SpA</v>
     <v>Eni SpA</v>
     <v>16.457999999999998</v>
-    <v>18.138000000000002</v>
+    <v>18.1248</v>
     <v>16.457999999999998</v>
-    <v>16.423999999999999</v>
+    <v>16.411999999999999</v>
     <v>3146765000</v>
     <v>ENI</v>
     <v>Eni SpA (XMIL:ENI)</v>
-    <v>2002696</v>
+    <v>2037548</v>
     <v>9296840</v>
   </rv>
   <rv s="2">
@@ -6663,11 +6662,11 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=ae8t4c&amp;q=XPAR%3aGLE&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="11">
-    <v>30</v>
+  <rv s="10">
+    <v>28</v>
     <v>Societe Generale SA (XPAR:GLE)</v>
     <v>2</v>
-    <v>31</v>
+    <v>29</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -6678,8 +6677,8 @@
     <v>59.9</v>
     <v>24.03</v>
     <v>1.3859999999999999</v>
-    <v>-1.26</v>
-    <v>-2.1297999999999997E-2</v>
+    <v>-1.28</v>
+    <v>-2.1636000000000002E-2</v>
     <v>EUR</v>
     <v>Societe Generale SA is a France-based financial services group. The Group offers a wide range of advisory services and tailored financial solutions to secure transactions, protect and manage assets and savings, and help its clients finance their projects. It operates through three segments: French Retail Banking, International Retail Banking &amp; Financial Services and Global Banking and Investor Solutions. French Retail Banking includes the domestic networks Societe Generale, Credit du Nord and Boursorama. International Retail Banking &amp; Financial Services consists of International Retail Banking (consumer finance activities), Financial Services to Corporates (operational vehicle leasing and fleet management, equipment and vendor finance) and Insurance Activities. Global Banking and Investor Solutions comprises Global Markets and Investors Services, Financing and Advisory, Asset and Wealth Management. The Group is active globally.</v>
     <v>119000</v>
@@ -6690,20 +6689,20 @@
     <v>58.84</v>
     <v>Banking Services</v>
     <v>Stock</v>
-    <v>45975.433796296296</v>
+    <v>45975.437175925923</v>
     <v>171</v>
     <v>57.48</v>
     <v>44832670000</v>
     <v>Societe Generale SA</v>
     <v>Societe Generale SA</v>
     <v>58.72</v>
-    <v>9.2719000000000005</v>
+    <v>9.2687000000000008</v>
     <v>59.16</v>
-    <v>57.9</v>
+    <v>57.88</v>
     <v>766894800</v>
     <v>GLE</v>
     <v>Societe Generale SA (XPAR:GLE)</v>
-    <v>429078</v>
+    <v>430071</v>
     <v>2149550</v>
   </rv>
   <rv s="2">
@@ -6728,8 +6727,8 @@
     <v>14.56</v>
     <v>9.3699999999999992</v>
     <v>0.2382</v>
-    <v>-0.28499999999999998</v>
-    <v>-1.9887999999999999E-2</v>
+    <v>-0.28999999999999998</v>
+    <v>-2.0236999999999998E-2</v>
     <v>EUR</v>
     <v>Orange SA is a France-based multi-service telecommunications operator. The Company operates seven segments: France, Spain, Europe, Africa &amp; Middle East, Enterprise, International Carriers &amp; Shared Services, Orange Bank. France includes all fixed and mobile communication services to consumers and companies as well as services for carriers. Spain covers fixed line and mobile telephony and fiber. Europe (Poland, Belgium, Luxembourg, Romania, Slovakia, and Moldova) provides high-speed fixed and mobile broadband. Africa &amp; Middle East primarily operates in the mobile markets but also provides telephony and fixed Internet services. Enterprise provides digital transformation support. International Carriers &amp; Shared Services includes international carrier and the activities of OCS and Orange Studio in content, among others. Orange Bank provides mobile financial services. Orange SA is the parent company of the Orange group.</v>
     <v>119270</v>
@@ -6740,20 +6739,20 @@
     <v>14.36</v>
     <v>Telecommunications Services</v>
     <v>Stock</v>
-    <v>45975.43375081016</v>
+    <v>45975.4372337963</v>
     <v>174</v>
-    <v>14.045</v>
+    <v>14.025</v>
     <v>37812700000</v>
     <v>Orange SA</v>
     <v>Orange SA</v>
     <v>14.35</v>
-    <v>44.362000000000002</v>
+    <v>44.346200000000003</v>
     <v>14.33</v>
-    <v>14.045</v>
+    <v>14.04</v>
     <v>2660057000</v>
     <v>ORA</v>
     <v>Orange SA (XPAR:ORA)</v>
-    <v>489474</v>
+    <v>500881</v>
     <v>3331760</v>
     <v>1991</v>
   </rv>
@@ -6842,7 +6841,7 @@
     <v>474.4</v>
     <v>Passenger Transportation Services</v>
     <v>Stock</v>
-    <v>45975.433195346872</v>
+    <v>45975.437199375003</v>
     <v>180</v>
     <v>468.9</v>
     <v>3590694000</v>
@@ -6855,7 +6854,7 @@
     <v>758010000</v>
     <v>EZJ</v>
     <v>EASYJET PLC (XLON:EZJ)</v>
-    <v>677099</v>
+    <v>683767</v>
     <v>3935350</v>
     <v>2000</v>
   </rv>
@@ -7025,7 +7024,7 @@
     <v>299928500</v>
     <v>GS</v>
     <v>THE GOLDMAN SACHS GROUP, INC. (XNYS:GS)</v>
-    <v>1775</v>
+    <v>1869</v>
     <v>2173298</v>
     <v>1998</v>
   </rv>
@@ -7076,7 +7075,7 @@
     <v>68764460</v>
     <v>LAZR</v>
     <v>LUMINAR TECHNOLOGIES, INC. (XNAS:LAZR)</v>
-    <v>47980</v>
+    <v>49873</v>
     <v>10548388</v>
     <v>2018</v>
   </rv>
@@ -7144,7 +7143,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-US</v>
     <v>a1x8w7</v>
     <v>268435456</v>
@@ -7178,7 +7177,7 @@
     <v>897995800</v>
     <v>MA</v>
     <v>MASTERCARD INCORPORATED. (XNYS:MA)</v>
-    <v>199</v>
+    <v>208</v>
     <v>2672917</v>
     <v>2001</v>
   </rv>
@@ -7229,7 +7228,7 @@
     <v>162499000</v>
     <v>NVAX</v>
     <v>NOVAVAX, INC. (XNAS:NVAX)</v>
-    <v>652</v>
+    <v>698</v>
     <v>4399043</v>
     <v>1987</v>
   </rv>
@@ -7314,7 +7313,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-US</v>
     <v>a1zez2</v>
     <v>268435456</v>
@@ -7348,7 +7347,7 @@
     <v>985210400</v>
     <v>OXY</v>
     <v>OCCIDENTAL PETROLEUM CORPORATION (XNYS:OXY)</v>
-    <v>7838</v>
+    <v>8177</v>
     <v>10334964</v>
     <v>1986</v>
   </rv>
@@ -7399,7 +7398,7 @@
     <v>5685708000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>81475</v>
+    <v>85298</v>
     <v>80023246</v>
     <v>1942</v>
   </rv>
@@ -7566,7 +7565,7 @@
     <v>0</v>
     <v>TENET HEALTHCARE CORPORATION (XNYS:THC)</v>
     <v>2</v>
-    <v>33</v>
+    <v>31</v>
     <v>Finance</v>
     <v>5</v>
     <v>en-US</v>
@@ -7665,11 +7664,11 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=bnyaur&amp;q=XSWX%3aLOCK&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="12">
+  <rv s="11">
+    <v>32</v>
+    <v>iShs Digtl Sec UCITS ETF USD A (XSWX:LOCK)</v>
+    <v>33</v>
     <v>34</v>
-    <v>iShs Digtl Sec UCITS ETF USD A (XSWX:LOCK)</v>
-    <v>35</v>
-    <v>36</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -7703,22 +7702,22 @@
   <rv s="2">
     <v>235</v>
   </rv>
-  <rv s="13">
+  <rv s="12">
     <v>12</v>
     <v>Volume average</v>
     <v>0</v>
   </rv>
-  <rv s="14">
+  <rv s="13">
     <v>12</v>
     <v>1</v>
   </rv>
-  <rv s="15">
+  <rv s="14">
+    <v>35</v>
+    <v>EUR/USD</v>
+    <v>36</v>
     <v>37</v>
-    <v>EUR/USD</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>39</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>av932w</v>
     <v>268435456</v>
@@ -7726,31 +7725,31 @@
     <v>Powered by Refinitiv</v>
     <v>1.1918</v>
     <v>1.0176000000000001</v>
-    <v>-1.8E-3</v>
-    <v>-1.5479999999999999E-3</v>
+    <v>-1.6999999999999999E-3</v>
+    <v>-1.462E-3</v>
     <v>USD</v>
     <v>EUR</v>
     <v>1.1648000000000001</v>
     <v>Currency Pair</v>
-    <v>45975.444178240738</v>
+    <v>45975.447638888887</v>
     <v>1.1613</v>
     <v>Euro/US Dollar FX Spot Rate</v>
     <v>1.1637999999999999</v>
     <v>1.1631</v>
-    <v>1.1613</v>
+    <v>1.1614</v>
     <v>EURUSD</v>
     <v>EUR/USD</v>
   </rv>
   <rv s="2">
     <v>239</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>EUR/CHF</v>
+    <v>36</v>
+    <v>39</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>41</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>av923m</v>
     <v>268435456</v>
@@ -7758,31 +7757,31 @@
     <v>Powered by Refinitiv</v>
     <v>0.96609999999999996</v>
     <v>0.91869999999999996</v>
-    <v>-2.3999999999999998E-3</v>
-    <v>-2.6029999999999998E-3</v>
+    <v>-2.3E-3</v>
+    <v>-2.4940000000000001E-3</v>
     <v>CHF</v>
     <v>EUR</v>
     <v>0.92290000000000005</v>
     <v>Currency Pair</v>
-    <v>45975.444189814814</v>
+    <v>45975.447627314818</v>
     <v>0.91869999999999996</v>
     <v>Euro/Swiss Franc FX Cross Rate</v>
     <v>0.92269999999999996</v>
     <v>0.92210000000000003</v>
-    <v>0.91969999999999996</v>
+    <v>0.91979999999999995</v>
     <v>EURCHF</v>
     <v>EUR/CHF</v>
   </rv>
   <rv s="2">
     <v>241</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>EUR/GBP</v>
+    <v>36</v>
+    <v>40</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>42</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>av92z2</v>
     <v>268435456</v>
@@ -7790,31 +7789,31 @@
     <v>Powered by Refinitiv</v>
     <v>0.88649999999999995</v>
     <v>0.82189999999999996</v>
-    <v>2E-3</v>
-    <v>2.2689999999999997E-3</v>
+    <v>2.2000000000000001E-3</v>
+    <v>2.496E-3</v>
     <v>GBP</v>
     <v>EUR</v>
     <v>0.88649999999999995</v>
     <v>Currency Pair</v>
-    <v>45975.444224537037</v>
+    <v>45975.447638888887</v>
     <v>0.88139999999999996</v>
     <v>Euro/UK Pound Sterling FX Cross Rate</v>
     <v>0.88139999999999996</v>
     <v>0.88149999999999995</v>
-    <v>0.88349999999999995</v>
+    <v>0.88370000000000004</v>
     <v>EURGBP</v>
     <v>EUR/GBP</v>
   </rv>
   <rv s="2">
     <v>243</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>EUR/AUD</v>
+    <v>36</v>
+    <v>41</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>43</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>av8sfr</v>
     <v>268435456</v>
@@ -7822,31 +7821,31 @@
     <v>Powered by Refinitiv</v>
     <v>1.8554999999999999</v>
     <v>1.5899000000000001</v>
-    <v>-1E-4</v>
-    <v>-5.6140000000000001E-5</v>
+    <v>-5.0000000000000001E-4</v>
+    <v>-2.8069999999999999E-4</v>
     <v>AUD</v>
     <v>EUR</v>
     <v>1.7841</v>
     <v>Currency Pair</v>
-    <v>45975.444178240738</v>
+    <v>45975.447638888887</v>
     <v>1.7763</v>
     <v>Euro/Australian Dollar FX Cross Rate</v>
     <v>1.7811999999999999</v>
     <v>1.7811999999999999</v>
-    <v>1.7810999999999999</v>
+    <v>1.7806999999999999</v>
     <v>EURAUD</v>
     <v>EUR/AUD</v>
   </rv>
   <rv s="2">
     <v>245</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>EUR/CAD</v>
+    <v>36</v>
+    <v>42</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>44</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>av8ttc</v>
     <v>268435456</v>
@@ -7854,31 +7853,31 @@
     <v>Powered by Refinitiv</v>
     <v>1.6468</v>
     <v>1.4484999999999999</v>
-    <v>-1.8E-3</v>
-    <v>-1.103E-3</v>
+    <v>-1.6999999999999999E-3</v>
+    <v>-1.042E-3</v>
     <v>CAD</v>
     <v>EUR</v>
     <v>1.6335999999999999</v>
     <v>Currency Pair</v>
-    <v>45975.444236111114</v>
+    <v>45975.447627314818</v>
     <v>1.6305000000000001</v>
     <v>Euro/Canadian Dollar FX Cross Rate</v>
     <v>1.6323000000000001</v>
     <v>1.6321000000000001</v>
-    <v>1.6303000000000001</v>
+    <v>1.6304000000000001</v>
     <v>EURCAD</v>
     <v>EUR/CAD</v>
   </rv>
   <rv s="2">
     <v>247</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>USD/JPY</v>
+    <v>36</v>
+    <v>43</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>45</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>avyomw</v>
     <v>268435456</v>
@@ -7886,31 +7885,31 @@
     <v>Powered by Refinitiv</v>
     <v>158.87</v>
     <v>139.86000000000001</v>
-    <v>0.16</v>
-    <v>1.0349999999999999E-3</v>
+    <v>0.14000000000000001</v>
+    <v>9.0590000000000006E-4</v>
     <v>JPY</v>
     <v>USD</v>
     <v>154.76</v>
     <v>Currency Pair</v>
-    <v>45975.444224537037</v>
+    <v>45975.447615740741</v>
     <v>154.32</v>
     <v>US Dollar/Japanese Yen FX Spot Rate</v>
     <v>154.53</v>
     <v>154.55000000000001</v>
-    <v>154.71</v>
+    <v>154.69</v>
     <v>USDJPY</v>
     <v>USD/JPY</v>
   </rv>
   <rv s="2">
     <v>249</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>USD/CHF</v>
+    <v>36</v>
+    <v>39</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>41</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>avyt7w</v>
     <v>268435456</v>
@@ -7924,7 +7923,7 @@
     <v>USD</v>
     <v>0.79349999999999998</v>
     <v>Currency Pair</v>
-    <v>45975.444189814814</v>
+    <v>45975.447638888887</v>
     <v>0.79020000000000001</v>
     <v>US Dollar/Swiss Franc FX Spot Rate</v>
     <v>0.7923</v>
@@ -7936,13 +7935,13 @@
   <rv s="2">
     <v>251</v>
   </rv>
-  <rv s="15">
-    <v>37</v>
+  <rv s="14">
+    <v>35</v>
     <v>USD/GBP</v>
+    <v>36</v>
+    <v>40</v>
+    <v>Finance</v>
     <v>38</v>
-    <v>42</v>
-    <v>Finance</v>
-    <v>40</v>
     <v>en-US</v>
     <v>avyu4c</v>
     <v>268435456</v>
@@ -7956,7 +7955,7 @@
     <v>USD</v>
     <v>0.76280000000000003</v>
     <v>Currency Pair</v>
-    <v>45975.444224537037</v>
+    <v>45975.447662037041</v>
     <v>0.75760000000000005</v>
     <v>US Dollar/UK Pound Sterling FX Cross Rate</v>
     <v>0.75780000000000003</v>
@@ -7972,13 +7971,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a6qja2&amp;q=DOW+JONES+INDU+AVERAGE+NDX&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="16">
+  <rv s="15">
+    <v>44</v>
+    <v>DOW JONES INDU AVERAGE NDX</v>
+    <v>33</v>
+    <v>45</v>
+    <v>Finance</v>
     <v>46</v>
-    <v>DOW JONES INDU AVERAGE NDX</v>
-    <v>35</v>
-    <v>47</v>
-    <v>Finance</v>
-    <v>48</v>
     <v>en-US</v>
     <v>a6qja2</v>
     <v>268435456</v>
@@ -8007,13 +8006,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=bxjpp2&amp;q=XLON%3aXNAS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="12">
+  <rv s="11">
+    <v>32</v>
+    <v>X NASDAQ 100 UCITS ETF 1C (XLON:XNAS)</v>
+    <v>33</v>
     <v>34</v>
-    <v>X NASDAQ 100 UCITS ETF 1C (XLON:XNAS)</v>
-    <v>35</v>
-    <v>36</v>
     <v>Finance</v>
-    <v>49</v>
+    <v>47</v>
     <v>en-US</v>
     <v>bxjpp2</v>
     <v>268435456</v>
@@ -8045,7 +8044,7 @@
   <rv s="2">
     <v>259</v>
   </rv>
-  <rv s="13">
+  <rv s="12">
     <v>12</v>
     <v>Instrument type</v>
     <v>0</v>
@@ -8094,18 +8093,18 @@
     <v>388147700</v>
     <v>ASML</v>
     <v>ASML Holding NV (XNAS:ASML)</v>
-    <v>6316</v>
+    <v>6401</v>
     <v>1495418</v>
     <v>1994</v>
   </rv>
   <rv s="2">
     <v>263</v>
   </rv>
-  <rv s="17">
-    <v>50</v>
+  <rv s="16">
+    <v>48</v>
     <v>Big Tree Cloud Holdings Limited (XNAS:DSY)</v>
-    <v>29</v>
-    <v>51</v>
+    <v>27</v>
+    <v>49</v>
     <v>Finance</v>
     <v>5</v>
     <v>en-US</v>
@@ -8155,7 +8154,7 @@
     <v>2</v>
     <v>10</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1v3sm</v>
     <v>268435456</v>
@@ -8189,7 +8188,7 @@
     <v>575332100</v>
     <v>IAG</v>
     <v>IAMGOLD CORPORATION (XNYS:IAG)</v>
-    <v>1369</v>
+    <v>2140</v>
     <v>12885981</v>
     <v>2017</v>
   </rv>
@@ -8200,11 +8199,11 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=bvct77&amp;q=XFRA%3aNQA&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="18">
-    <v>52</v>
+  <rv s="17">
+    <v>50</v>
     <v>Note AB (publ) (XFRA:NQA)</v>
     <v>2</v>
-    <v>53</v>
+    <v>51</v>
     <v>Finance</v>
     <v>9</v>
     <v>en-US</v>
@@ -8249,13 +8248,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1rjbh&amp;q=XNYS%3aE&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="11">
-    <v>30</v>
+  <rv s="10">
+    <v>28</v>
     <v>Eni SpA (XNYS:E)</v>
     <v>2</v>
-    <v>54</v>
+    <v>52</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-US</v>
     <v>a1rjbh</v>
     <v>268435456</v>
@@ -8299,13 +8298,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=aazgim&amp;q=XTSE%3aORA&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="19">
-    <v>55</v>
+  <rv s="18">
+    <v>53</v>
     <v>Aura Minerals Inc. (XTSE:ORA)</v>
     <v>2</v>
-    <v>56</v>
+    <v>54</v>
     <v>Finance</v>
-    <v>57</v>
+    <v>55</v>
     <v>en-US</v>
     <v>aazgim</v>
     <v>268435456</v>
@@ -8353,7 +8352,7 @@
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="20">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="19">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -8543,51 +8542,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Shares outstanding"/>
-    <k n="Ticker symbol" t="s"/>
-    <k n="UniqueName" t="s"/>
-    <k n="Volume"/>
-    <k n="Volume average"/>
-    <k n="Year incorporated"/>
-  </s>
-  <s t="_linkedentitycore">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="_Flags" t="spb"/>
-    <k n="_Format" t="spb"/>
-    <k n="_Icon" t="s"/>
-    <k n="_SubLabel" t="spb"/>
-    <k n="%EntityCulture" t="s"/>
-    <k n="%EntityId" t="s"/>
-    <k n="%EntityServiceId"/>
-    <k n="%IsRefreshable" t="b"/>
-    <k n="%ProviderInfo" t="s"/>
-    <k n="52 week high"/>
-    <k n="52 week low"/>
-    <k n="Beta"/>
-    <k n="Change"/>
-    <k n="Change (%)"/>
-    <k n="Currency" t="s"/>
-    <k n="Description" t="s"/>
-    <k n="Employees"/>
-    <k n="Exchange" t="s"/>
-    <k n="Exchange abbreviation" t="s"/>
-    <k n="ExchangeID" t="s"/>
-    <k n="Headquarters" t="s"/>
-    <k n="High"/>
-    <k n="Industry" t="s"/>
-    <k n="Instrument type" t="s"/>
-    <k n="Last trade time"/>
-    <k n="LearnMoreOnLink" t="r"/>
-    <k n="Low"/>
-    <k n="Market cap"/>
-    <k n="Name" t="s"/>
-    <k n="Official name" t="s"/>
-    <k n="Open"/>
-    <k n="P/E"/>
-    <k n="Previous close"/>
-    <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -8961,7 +8915,7 @@
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="14">
+  <spbArrays count="13">
     <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
@@ -9138,51 +9092,6 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
       <v t="s">%OutdatedReason</v>
-    </a>
-    <a count="43">
-      <v t="s">%EntityServiceId</v>
-      <v t="s">_Format</v>
-      <v t="s">%IsRefreshable</v>
-      <v t="s">%EntityCulture</v>
-      <v t="s">%EntityId</v>
-      <v t="s">_Icon</v>
-      <v t="s">_Display</v>
-      <v t="s">Name</v>
-      <v t="s">_SubLabel</v>
-      <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
-      <v t="s">Exchange</v>
-      <v t="s">Official name</v>
-      <v t="s">Last trade time</v>
-      <v t="s">Ticker symbol</v>
-      <v t="s">Exchange abbreviation</v>
-      <v t="s">Change</v>
-      <v t="s">Change (%)</v>
-      <v t="s">Currency</v>
-      <v t="s">Previous close</v>
-      <v t="s">Open</v>
-      <v t="s">High</v>
-      <v t="s">Low</v>
-      <v t="s">52 week high</v>
-      <v t="s">52 week low</v>
-      <v t="s">Volume</v>
-      <v t="s">Volume average</v>
-      <v t="s">Market cap</v>
-      <v t="s">Beta</v>
-      <v t="s">P/E</v>
-      <v t="s">Shares outstanding</v>
-      <v t="s">Description</v>
-      <v t="s">Employees</v>
-      <v t="s">Headquarters</v>
-      <v t="s">Industry</v>
-      <v t="s">Instrument type</v>
-      <v t="s">Year incorporated</v>
-      <v t="s">_Flags</v>
-      <v t="s">UniqueName</v>
-      <v t="s">_DisplayString</v>
-      <v t="s">LearnMoreOnLink</v>
-      <v t="s">ExchangeID</v>
-      <v t="s">%ProviderInfo</v>
     </a>
     <a count="42">
       <v t="s">%EntityServiceId</v>
@@ -9537,7 +9446,7 @@
       <v t="s">%OutdatedReason</v>
     </a>
   </spbArrays>
-  <spbData count="58">
+  <spbData count="56">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -9750,7 +9659,6 @@
     <spb s="11">
       <v>1</v>
       <v>2</v>
-      <v>2</v>
       <v>1</v>
       <v>3</v>
       <v>1</v>
@@ -9777,33 +9685,6 @@
       <v>Source: Nasdaq</v>
       <v>GMT</v>
       <v>Delayed 15 minutes</v>
-    </spb>
-    <spb s="0">
-      <v>5</v>
-      <v>Name</v>
-      <v>LearnMoreOnLink</v>
-    </spb>
-    <spb s="13">
-      <v>1</v>
-      <v>2</v>
-      <v>1</v>
-      <v>3</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>4</v>
-      <v>5</v>
-      <v>6</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>7</v>
-      <v>8</v>
-      <v>9</v>
-      <v>4</v>
-      <v>1</v>
     </spb>
     <spb s="3">
       <v>1</v>
@@ -9893,21 +9774,21 @@
       <v>9</v>
       <v>4</v>
     </spb>
-    <spb s="14">
-      <v>6</v>
+    <spb s="13">
+      <v>5</v>
       <v>Name</v>
     </spb>
-    <spb s="15">
+    <spb s="14">
       <v>1</v>
       <v>1</v>
       <v>1</v>
     </spb>
     <spb s="0">
-      <v>7</v>
+      <v>6</v>
       <v>Name</v>
       <v>LearnMoreOnLink</v>
     </spb>
-    <spb s="16">
+    <spb s="15">
       <v>12</v>
       <v>2</v>
       <v>2</v>
@@ -9958,16 +9839,16 @@
       <v>4</v>
     </spb>
     <spb s="0">
-      <v>8</v>
+      <v>7</v>
       <v>Name</v>
       <v>LearnMoreOnLink</v>
     </spb>
-    <spb s="17">
+    <spb s="16">
       <v>1</v>
       <v>1</v>
       <v>1</v>
     </spb>
-    <spb s="18">
+    <spb s="17">
       <v>1</v>
       <v>2</v>
       <v>1</v>
@@ -9985,15 +9866,15 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="14">
-      <v>9</v>
+    <spb s="13">
+      <v>8</v>
       <v>Name</v>
     </spb>
-    <spb s="19">
+    <spb s="18">
       <v>1</v>
       <v>1</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>1</v>
       <v>1</v>
       <v>3</v>
@@ -10007,10 +9888,10 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="21">
+    <spb s="20">
       <v>GMT</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>18</v>
       <v>18</v>
       <v>3</v>
@@ -10024,7 +9905,7 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>21</v>
       <v>21</v>
       <v>3</v>
@@ -10038,7 +9919,7 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>22</v>
       <v>22</v>
       <v>3</v>
@@ -10052,7 +9933,7 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>23</v>
       <v>23</v>
       <v>3</v>
@@ -10066,7 +9947,7 @@
       <v>7</v>
       <v>9</v>
     </spb>
-    <spb s="20">
+    <spb s="19">
       <v>24</v>
       <v>24</v>
       <v>3</v>
@@ -10081,11 +9962,11 @@
       <v>9</v>
     </spb>
     <spb s="0">
-      <v>10</v>
+      <v>9</v>
       <v>Name</v>
       <v>LearnMoreOnLink</v>
     </spb>
-    <spb s="22">
+    <spb s="21">
       <v>1</v>
       <v>1</v>
       <v>3</v>
@@ -10098,23 +9979,69 @@
       <v>1</v>
       <v>9</v>
     </spb>
-    <spb s="23">
+    <spb s="22">
       <v>from previous close</v>
       <v>from previous close</v>
     </spb>
-    <spb s="24">
+    <spb s="23">
       <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>LSE</v>
       <v>from previous close</v>
       <v>GMT</v>
     </spb>
-    <spb s="14">
+    <spb s="13">
+      <v>10</v>
+      <v>Name</v>
+    </spb>
+    <spb s="24">
+      <v>1</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="0">
       <v>11</v>
       <v>Name</v>
+      <v>LearnMoreOnLink</v>
     </spb>
     <spb s="25">
+      <v>12</v>
+      <v>2</v>
+      <v>2</v>
+      <v>12</v>
+      <v>3</v>
+      <v>12</v>
+      <v>12</v>
+      <v>12</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>17</v>
+      <v>12</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="15">
       <v>1</v>
+      <v>2</v>
       <v>2</v>
       <v>1</v>
       <v>3</v>
@@ -10139,52 +10066,6 @@
       <v>LearnMoreOnLink</v>
     </spb>
     <spb s="26">
-      <v>12</v>
-      <v>2</v>
-      <v>2</v>
-      <v>12</v>
-      <v>3</v>
-      <v>12</v>
-      <v>12</v>
-      <v>12</v>
-      <v>4</v>
-      <v>4</v>
-      <v>5</v>
-      <v>17</v>
-      <v>12</v>
-      <v>4</v>
-      <v>7</v>
-      <v>8</v>
-      <v>9</v>
-      <v>4</v>
-    </spb>
-    <spb s="16">
-      <v>1</v>
-      <v>2</v>
-      <v>2</v>
-      <v>1</v>
-      <v>3</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>4</v>
-      <v>5</v>
-      <v>6</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>7</v>
-      <v>9</v>
-      <v>4</v>
-    </spb>
-    <spb s="0">
-      <v>13</v>
-      <v>Name</v>
-      <v>LearnMoreOnLink</v>
-    </spb>
-    <spb s="27">
       <v>23</v>
       <v>2</v>
       <v>2</v>
@@ -10208,7 +10089,7 @@
       <v>23</v>
       <v>5</v>
     </spb>
-    <spb s="28">
+    <spb s="27">
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
@@ -10222,7 +10103,7 @@
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="29">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="28">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -10334,7 +10215,6 @@
   </s>
   <s>
     <k n="Low" t="i"/>
-    <k n="P/E" t="i"/>
     <k n="Beta" t="i"/>
     <k n="High" t="i"/>
     <k n="Name" t="i"/>
@@ -10362,28 +10242,6 @@
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
     <k n="Price (Extended hours)" t="s"/>
-  </s>
-  <s>
-    <k n="Low" t="i"/>
-    <k n="Beta" t="i"/>
-    <k n="High" t="i"/>
-    <k n="Name" t="i"/>
-    <k n="Open" t="i"/>
-    <k n="Price" t="i"/>
-    <k n="Change" t="i"/>
-    <k n="Volume" t="i"/>
-    <k n="Employees" t="i"/>
-    <k n="Change (%)" t="i"/>
-    <k n="Market cap" t="i"/>
-    <k n="52 week low" t="i"/>
-    <k n="52 week high" t="i"/>
-    <k n="Previous close" t="i"/>
-    <k n="Volume average" t="i"/>
-    <k n="Last trade time" t="i"/>
-    <k n="Year incorporated" t="i"/>
-    <k n="`%EntityServiceId" t="i"/>
-    <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -11151,7 +11009,7 @@
     <row r="1" spans="1:32" s="1" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="87">
         <f ca="1">MAX(E3:E96)</f>
-        <v>45975.433831018519</v>
+        <v>45975.437256944446</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -11163,7 +11021,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>45975.486575578703</v>
+        <v>45975.489911689816</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
@@ -11290,7 +11148,7 @@
       </c>
       <c r="B3" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C3" s="16" t="e" vm="1">
         <v>#VALUE!</v>
@@ -11408,7 +11266,7 @@
       </c>
       <c r="B4" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C4" s="24" t="e" vm="2">
         <v>#VALUE!</v>
@@ -11526,7 +11384,7 @@
       </c>
       <c r="B5" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1318619128466328E-2</v>
+        <v>1.1316057485572026E-2</v>
       </c>
       <c r="C5" s="24" t="e" vm="3">
         <v>#VALUE!</v>
@@ -11642,7 +11500,7 @@
       </c>
       <c r="B6" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C6" t="e" vm="4">
         <v>#VALUE!</v>
@@ -11697,7 +11555,7 @@
       </c>
       <c r="P6" s="22" cm="1">
         <f t="array" aca="1" ref="P6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>73714</v>
+        <v>74470</v>
       </c>
       <c r="Q6" s="22" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -11716,7 +11574,7 @@
       </c>
       <c r="V6" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3979648473495174E-3</v>
+        <v>1.4123021703084701E-3</v>
       </c>
       <c r="W6" s="23"/>
       <c r="X6" s="104">
@@ -11770,7 +11628,7 @@
       </c>
       <c r="E7" s="17" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.432119490622</v>
+        <v>45975.435856481483</v>
       </c>
       <c r="F7" s="27" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -11782,7 +11640,7 @@
       </c>
       <c r="H7" s="27" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>0.69799999999999995</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="I7" s="27" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -11798,11 +11656,11 @@
       </c>
       <c r="L7" s="20" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-2.1999999999999999E-2</v>
+        <v>-5.3999999999999999E-2</v>
       </c>
       <c r="M7" s="21" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-3.0556E-2</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="N7" s="27" cm="1">
         <f t="array" aca="1" ref="N7" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -11814,7 +11672,7 @@
       </c>
       <c r="P7" s="22" cm="1">
         <f t="array" aca="1" ref="P7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7681</v>
+        <v>10854</v>
       </c>
       <c r="Q7" s="22" cm="1">
         <f t="array" aca="1" ref="Q7" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -11833,7 +11691,7 @@
       </c>
       <c r="V7" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3265975820379965</v>
+        <v>1.8746113989637305</v>
       </c>
       <c r="W7" s="23"/>
       <c r="X7" s="104">
@@ -11885,7 +11743,7 @@
       </c>
       <c r="E8" s="17" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433807870373</v>
+        <v>45975.4372337963</v>
       </c>
       <c r="F8" s="27" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -11897,7 +11755,7 @@
       </c>
       <c r="H8" s="27" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>857.7</v>
+        <v>859.4</v>
       </c>
       <c r="I8" s="27" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -11909,15 +11767,15 @@
       </c>
       <c r="K8" s="19" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>32.932600000000001</v>
+        <v>32.997900000000001</v>
       </c>
       <c r="L8" s="20" cm="1">
         <f t="array" aca="1" ref="L8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-23.8</v>
+        <v>-22.1</v>
       </c>
       <c r="M8" s="21" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.6998999999999999E-2</v>
+        <v>-2.5071E-2</v>
       </c>
       <c r="N8" s="27" cm="1">
         <f t="array" aca="1" ref="N8" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -11929,7 +11787,7 @@
       </c>
       <c r="P8" s="22" cm="1">
         <f t="array" aca="1" ref="P8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>153992</v>
+        <v>155625</v>
       </c>
       <c r="Q8" s="22" cm="1">
         <f t="array" aca="1" ref="Q8" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -11948,7 +11806,7 @@
       </c>
       <c r="V8" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.28183531909441972</v>
+        <v>0.28482402679404822</v>
       </c>
       <c r="W8" s="23"/>
       <c r="X8" s="104">
@@ -12044,7 +11902,7 @@
       </c>
       <c r="P9" s="22" cm="1">
         <f t="array" aca="1" ref="P9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>35763</v>
+        <v>36270</v>
       </c>
       <c r="Q9" s="22" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -12062,7 +11920,7 @@
       </c>
       <c r="V9" s="103">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.7293644074435348E-3</v>
+        <v>1.7538810239067476E-3</v>
       </c>
       <c r="W9" s="103"/>
       <c r="X9" s="104">
@@ -12158,7 +12016,7 @@
       </c>
       <c r="P10" s="22" cm="1">
         <f t="array" aca="1" ref="P10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>4563</v>
+        <v>4800</v>
       </c>
       <c r="Q10" s="22" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -12174,7 +12032,7 @@
       </c>
       <c r="V10" s="103">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>8.9658325737362605E-4</v>
+        <v>9.4315135555411028E-4</v>
       </c>
       <c r="W10" s="103"/>
       <c r="X10" s="104">
@@ -12216,7 +12074,7 @@
       </c>
       <c r="B11" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C11" t="e" vm="9">
         <v>#VALUE!</v>
@@ -12335,7 +12193,7 @@
       </c>
       <c r="B12" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C12" t="e" vm="10">
         <v>#VALUE!</v>
@@ -12453,7 +12311,7 @@
       </c>
       <c r="B13" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C13" t="e" vm="11">
         <v>#VALUE!</v>
@@ -12571,7 +12429,7 @@
       </c>
       <c r="B14" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C14" t="e" vm="12">
         <v>#VALUE!</v>
@@ -12689,7 +12547,7 @@
       </c>
       <c r="B15" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C15" t="e" vm="13">
         <v>#VALUE!</v>
@@ -12807,7 +12665,7 @@
       </c>
       <c r="B16" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C16" t="e" vm="14">
         <v>#VALUE!</v>
@@ -12925,7 +12783,7 @@
       </c>
       <c r="B17" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C17" t="e" vm="15">
         <v>#VALUE!</v>
@@ -12980,7 +12838,7 @@
       </c>
       <c r="P17" s="22" cm="1">
         <f t="array" aca="1" ref="P17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7555</v>
+        <v>8260</v>
       </c>
       <c r="Q17" s="22" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -12999,7 +12857,7 @@
       </c>
       <c r="V17" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>9.1920543176800739E-4</v>
+        <v>1.0049817162678678E-3</v>
       </c>
       <c r="W17" s="23"/>
       <c r="X17" s="104">
@@ -13043,7 +12901,7 @@
       </c>
       <c r="B18" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C18" t="e" vm="16">
         <v>#VALUE!</v>
@@ -13054,7 +12912,7 @@
       </c>
       <c r="E18" s="17" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433692129627</v>
+        <v>45975.437256944446</v>
       </c>
       <c r="F18" s="18" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13098,7 +12956,7 @@
       </c>
       <c r="P18" s="22" cm="1">
         <f t="array" aca="1" ref="P18" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>234662</v>
+        <v>236855</v>
       </c>
       <c r="Q18" s="22" cm="1">
         <f t="array" aca="1" ref="Q18" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13117,7 +12975,7 @@
       </c>
       <c r="V18" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.12560053952213754</v>
+        <v>0.12677432131540636</v>
       </c>
       <c r="W18" s="23"/>
       <c r="X18" s="104">
@@ -13276,7 +13134,7 @@
       </c>
       <c r="B20" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C20" t="e" vm="18">
         <v>#VALUE!</v>
@@ -13394,7 +13252,7 @@
       </c>
       <c r="B21" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C21" t="e" vm="19">
         <v>#VALUE!</v>
@@ -13405,7 +13263,7 @@
       </c>
       <c r="E21" s="17" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433333333334</v>
+        <v>45975.436805555553</v>
       </c>
       <c r="F21" s="18" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -13417,7 +13275,7 @@
       </c>
       <c r="H21" s="18" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>15.14</v>
+        <v>15.22</v>
       </c>
       <c r="I21" s="18" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -13429,15 +13287,15 @@
       </c>
       <c r="K21" s="19" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>12.5124</v>
+        <v>12.5785</v>
       </c>
       <c r="L21" s="20" cm="1">
         <f t="array" aca="1" ref="L21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-8.5000000000000006E-2</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="M21" s="21" cm="1">
         <f t="array" aca="1" ref="M21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-5.5830000000000003E-3</v>
+        <v>-3.2840000000000001E-4</v>
       </c>
       <c r="N21" s="18" cm="1">
         <f t="array" aca="1" ref="N21" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -13449,7 +13307,7 @@
       </c>
       <c r="P21" s="22" cm="1">
         <f t="array" aca="1" ref="P21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8580</v>
+        <v>8610</v>
       </c>
       <c r="Q21" s="22" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -13468,7 +13326,7 @@
       </c>
       <c r="V21" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.2154513530262343E-3</v>
+        <v>2.2231976864284238E-3</v>
       </c>
       <c r="W21" s="23"/>
       <c r="X21" s="104">
@@ -13627,7 +13485,7 @@
       </c>
       <c r="B23" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C23" t="e" vm="21">
         <v>#VALUE!</v>
@@ -13745,7 +13603,7 @@
       </c>
       <c r="B24" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C24" t="e" vm="22">
         <v>#VALUE!</v>
@@ -13863,7 +13721,7 @@
       </c>
       <c r="B25" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C25" t="e" vm="23">
         <v>#VALUE!</v>
@@ -13981,7 +13839,7 @@
       </c>
       <c r="B26" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C26" t="e" vm="24">
         <v>#VALUE!</v>
@@ -13992,7 +13850,7 @@
       </c>
       <c r="E26" s="17" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433682233597</v>
+        <v>45975.437146122655</v>
       </c>
       <c r="F26" s="18" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -14004,7 +13862,7 @@
       </c>
       <c r="H26" s="18" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>387.6</v>
+        <v>387.4</v>
       </c>
       <c r="I26" s="18" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -14016,15 +13874,15 @@
       </c>
       <c r="K26" s="19" cm="1">
         <f t="array" aca="1" ref="K26" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>6.9824999999999999</v>
+        <v>6.9789000000000003</v>
       </c>
       <c r="L26" s="20" cm="1">
         <f t="array" aca="1" ref="L26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-8.1999999999999993</v>
+        <v>-8.4</v>
       </c>
       <c r="M26" s="21" cm="1">
         <f t="array" aca="1" ref="M26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.0718E-2</v>
+        <v>-2.1223000000000002E-2</v>
       </c>
       <c r="N26" s="18" cm="1">
         <f t="array" aca="1" ref="N26" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -14036,7 +13894,7 @@
       </c>
       <c r="P26" s="22" cm="1">
         <f t="array" aca="1" ref="P26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2337191</v>
+        <v>2389916</v>
       </c>
       <c r="Q26" s="22" cm="1">
         <f t="array" aca="1" ref="Q26" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14055,7 +13913,7 @@
       </c>
       <c r="V26" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.12022488498037054</v>
+        <v>0.12293705401601633</v>
       </c>
       <c r="W26" s="23"/>
       <c r="X26" s="104">
@@ -14099,7 +13957,7 @@
       </c>
       <c r="B27" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1318619128466328E-2</v>
+        <v>1.1316057485572026E-2</v>
       </c>
       <c r="C27" t="e" vm="25">
         <v>#VALUE!</v>
@@ -14215,7 +14073,7 @@
       </c>
       <c r="B28" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C28" t="e" vm="26">
         <v>#VALUE!</v>
@@ -14333,7 +14191,7 @@
       </c>
       <c r="B29" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C29" t="e" vm="27">
         <v>#VALUE!</v>
@@ -14451,7 +14309,7 @@
       </c>
       <c r="B30" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C30" t="e" vm="28">
         <v>#VALUE!</v>
@@ -14569,7 +14427,7 @@
       </c>
       <c r="B31" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C31" t="e" vm="29">
         <v>#VALUE!</v>
@@ -14624,7 +14482,7 @@
       </c>
       <c r="P31" s="22" cm="1">
         <f t="array" aca="1" ref="P31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>30348</v>
+        <v>31936</v>
       </c>
       <c r="Q31" s="22" cm="1">
         <f t="array" aca="1" ref="Q31" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14643,7 +14501,7 @@
       </c>
       <c r="V31" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3830942207644062E-3</v>
+        <v>1.4554664898620033E-3</v>
       </c>
       <c r="W31" s="23"/>
       <c r="X31" s="104">
@@ -14687,7 +14545,7 @@
       </c>
       <c r="B32" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C32" t="e" vm="30">
         <v>#VALUE!</v>
@@ -14742,7 +14600,7 @@
       </c>
       <c r="P32" s="22" cm="1">
         <f t="array" aca="1" ref="P32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>1291</v>
+        <v>1389</v>
       </c>
       <c r="Q32" s="22" cm="1">
         <f t="array" aca="1" ref="Q32" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14761,7 +14619,7 @@
       </c>
       <c r="V32" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.4306749339213249E-4</v>
+        <v>1.5392776787116346E-4</v>
       </c>
       <c r="W32" s="23"/>
       <c r="X32" s="104">
@@ -14805,7 +14663,7 @@
       </c>
       <c r="B33" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C33" t="e" vm="31">
         <v>#VALUE!</v>
@@ -14860,7 +14718,7 @@
       </c>
       <c r="P33" s="22" cm="1">
         <f t="array" aca="1" ref="P33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>10701</v>
+        <v>10800</v>
       </c>
       <c r="Q33" s="22" cm="1">
         <f t="array" aca="1" ref="Q33" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14879,7 +14737,7 @@
       </c>
       <c r="V33" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>8.8344181865674569E-4</v>
+        <v>8.9161495575113112E-4</v>
       </c>
       <c r="W33" s="23"/>
       <c r="X33" s="104">
@@ -14923,7 +14781,7 @@
       </c>
       <c r="B34" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C34" t="e" vm="32">
         <v>#VALUE!</v>
@@ -14978,7 +14836,7 @@
       </c>
       <c r="P34" s="22" cm="1">
         <f t="array" aca="1" ref="P34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>6724</v>
+        <v>6736</v>
       </c>
       <c r="Q34" s="22" cm="1">
         <f t="array" aca="1" ref="Q34" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -14997,7 +14855,7 @@
       </c>
       <c r="V34" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.4901725954068377E-3</v>
+        <v>1.492832034898938E-3</v>
       </c>
       <c r="W34" s="23"/>
       <c r="X34" s="104">
@@ -15041,7 +14899,7 @@
       </c>
       <c r="B35" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C35" t="e" vm="33">
         <v>#VALUE!</v>
@@ -15159,7 +15017,7 @@
       </c>
       <c r="B36" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C36" t="e" vm="34">
         <v>#VALUE!</v>
@@ -15277,7 +15135,7 @@
       </c>
       <c r="B37" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C37" t="e" vm="35">
         <v>#VALUE!</v>
@@ -15395,7 +15253,7 @@
       </c>
       <c r="B38" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C38" t="e" vm="36">
         <v>#VALUE!</v>
@@ -15450,7 +15308,7 @@
       </c>
       <c r="P38" s="22" cm="1">
         <f t="array" aca="1" ref="P38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>49556</v>
+        <v>49844</v>
       </c>
       <c r="Q38" s="22" cm="1">
         <f t="array" aca="1" ref="Q38" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15469,7 +15327,7 @@
       </c>
       <c r="V38" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>3.2149674393396771E-3</v>
+        <v>3.2336515668424984E-3</v>
       </c>
       <c r="W38" s="23"/>
       <c r="X38" s="104">
@@ -15513,7 +15371,7 @@
       </c>
       <c r="B39" s="15">
         <f ca="1">D103</f>
-        <v>0.61338403974728573</v>
+        <v>0.61334641805691847</v>
       </c>
       <c r="C39" t="e" vm="37">
         <v>#VALUE!</v>
@@ -15631,7 +15489,7 @@
       </c>
       <c r="B40" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C40" t="e" vm="38">
         <v>#VALUE!</v>
@@ -15749,7 +15607,7 @@
       </c>
       <c r="B41" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C41" t="e" vm="39">
         <v>#VALUE!</v>
@@ -15760,7 +15618,7 @@
       </c>
       <c r="E41" s="17" cm="1">
         <f t="array" aca="1" ref="E41" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433333333334</v>
+        <v>45975.436805555553</v>
       </c>
       <c r="F41" s="18" cm="1">
         <f t="array" aca="1" ref="F41" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15877,7 +15735,7 @@
       </c>
       <c r="E42" s="17" cm="1">
         <f t="array" aca="1" ref="E42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.43377314815</v>
+        <v>45975.437245370369</v>
       </c>
       <c r="F42" s="27" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -15889,11 +15747,11 @@
       </c>
       <c r="H42" s="27" cm="1">
         <f t="array" aca="1" ref="H42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>210.5</v>
+        <v>210.75</v>
       </c>
       <c r="I42" s="27" cm="1">
         <f t="array" aca="1" ref="I42" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
-        <v>210.4</v>
+        <v>210.35</v>
       </c>
       <c r="J42" s="27" cm="1">
         <f t="array" aca="1" ref="J42" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"High"),0)</f>
@@ -15901,15 +15759,15 @@
       </c>
       <c r="K42" s="19" cm="1">
         <f t="array" aca="1" ref="K42" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>34.674199999999999</v>
+        <v>34.715400000000002</v>
       </c>
       <c r="L42" s="20" cm="1">
         <f t="array" aca="1" ref="L42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-7.6</v>
+        <v>-7.35</v>
       </c>
       <c r="M42" s="21" cm="1">
         <f t="array" aca="1" ref="M42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-3.4846000000000002E-2</v>
+        <v>-3.3700000000000001E-2</v>
       </c>
       <c r="N42" s="27" cm="1">
         <f t="array" aca="1" ref="N42" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -15921,7 +15779,7 @@
       </c>
       <c r="P42" s="22" cm="1">
         <f t="array" aca="1" ref="P42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>260937</v>
+        <v>263672</v>
       </c>
       <c r="Q42" s="22" cm="1">
         <f t="array" aca="1" ref="Q42" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -15940,7 +15798,7 @@
       </c>
       <c r="V42" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.22274702292031243</v>
+        <v>0.22508173630970166</v>
       </c>
       <c r="W42" s="23"/>
       <c r="X42" s="104">
@@ -16097,7 +15955,7 @@
       </c>
       <c r="B44" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C44" t="e" vm="42">
         <v>#VALUE!</v>
@@ -16215,7 +16073,7 @@
       </c>
       <c r="B45" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C45" t="e" vm="43">
         <v>#VALUE!</v>
@@ -16270,7 +16128,7 @@
       </c>
       <c r="P45" s="22" cm="1">
         <f t="array" aca="1" ref="P45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>995766</v>
+        <v>1012731</v>
       </c>
       <c r="Q45" s="22" cm="1">
         <f t="array" aca="1" ref="Q45" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16289,7 +16147,7 @@
       </c>
       <c r="V45" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.2017193984009973E-2</v>
+        <v>1.2221932543007498E-2</v>
       </c>
       <c r="W45" s="23"/>
       <c r="X45" s="104">
@@ -16334,7 +16192,7 @@
       </c>
       <c r="B46" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C46" t="e" vm="44">
         <v>#VALUE!</v>
@@ -16389,7 +16247,7 @@
       </c>
       <c r="P46" s="22" cm="1">
         <f t="array" aca="1" ref="P46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>42049</v>
+        <v>42526</v>
       </c>
       <c r="Q46" s="22" cm="1">
         <f t="array" aca="1" ref="Q46" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -16408,7 +16266,7 @@
       </c>
       <c r="V46" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.9210942616812508E-3</v>
+        <v>2.9542308871140068E-3</v>
       </c>
       <c r="W46" s="23"/>
       <c r="X46" s="104">
@@ -16452,7 +16310,7 @@
       </c>
       <c r="B47" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C47" t="e" vm="45">
         <v>#VALUE!</v>
@@ -16685,7 +16543,7 @@
       </c>
       <c r="B49" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C49" t="e" vm="47">
         <v>#VALUE!</v>
@@ -16803,7 +16661,7 @@
       </c>
       <c r="B50" s="15">
         <f ca="1">D100</f>
-        <v>1.0873110796999021</v>
+        <v>1.087192868014786</v>
       </c>
       <c r="C50" t="e" vm="48">
         <v>#VALUE!</v>
@@ -16814,7 +16672,7 @@
       </c>
       <c r="E50" s="17" cm="1">
         <f t="array" aca="1" ref="E50" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.432430555556</v>
+        <v>45975.434641203705</v>
       </c>
       <c r="F50" s="35" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -16919,7 +16777,7 @@
       </c>
       <c r="B51" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C51" t="e" vm="49">
         <v>#VALUE!</v>
@@ -17037,7 +16895,7 @@
       </c>
       <c r="B52" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C52" t="e" vm="50">
         <v>#VALUE!</v>
@@ -17155,7 +17013,7 @@
       </c>
       <c r="B53" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C53" t="e" vm="51">
         <v>#VALUE!</v>
@@ -17273,7 +17131,7 @@
       </c>
       <c r="B54" s="15">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C54" t="e" vm="52">
         <v>#VALUE!</v>
@@ -17401,7 +17259,7 @@
       </c>
       <c r="E55" s="58" cm="1">
         <f t="array" aca="1" ref="E55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.432119490622</v>
+        <v>45975.435856481483</v>
       </c>
       <c r="F55" s="64" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17413,7 +17271,7 @@
       </c>
       <c r="H55" s="64" cm="1">
         <f t="array" aca="1" ref="H55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>0.69799999999999995</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="I55" s="64" cm="1">
         <f t="array" aca="1" ref="I55" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -17429,11 +17287,11 @@
       </c>
       <c r="L55" s="60" cm="1">
         <f t="array" aca="1" ref="L55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-2.1999999999999999E-2</v>
+        <v>-5.3999999999999999E-2</v>
       </c>
       <c r="M55" s="61" cm="1">
         <f t="array" aca="1" ref="M55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-3.0556E-2</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="N55" s="64" cm="1">
         <f t="array" aca="1" ref="N55" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -17445,7 +17303,7 @@
       </c>
       <c r="P55" s="62" cm="1">
         <f t="array" aca="1" ref="P55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7681</v>
+        <v>10854</v>
       </c>
       <c r="Q55" s="62" cm="1">
         <f t="array" aca="1" ref="Q55" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17467,7 +17325,7 @@
       </c>
       <c r="V55" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3265975820379965</v>
+        <v>1.8746113989637305</v>
       </c>
       <c r="W55" s="90"/>
       <c r="X55" s="104">
@@ -17511,7 +17369,7 @@
       </c>
       <c r="B56" s="112">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C56" t="e" vm="14">
         <v>#VALUE!</v>
@@ -17643,7 +17501,7 @@
       </c>
       <c r="E57" s="58" cm="1">
         <f t="array" aca="1" ref="E57" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433692129627</v>
+        <v>45975.437256944446</v>
       </c>
       <c r="F57" s="64" cm="1">
         <f t="array" aca="1" ref="F57" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17687,7 +17545,7 @@
       </c>
       <c r="P57" s="62" cm="1">
         <f t="array" aca="1" ref="P57" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>234662</v>
+        <v>236855</v>
       </c>
       <c r="Q57" s="62" cm="1">
         <f t="array" aca="1" ref="Q57" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17709,7 +17567,7 @@
       </c>
       <c r="V57" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.12560053952213754</v>
+        <v>0.12677432131540636</v>
       </c>
       <c r="W57" s="90"/>
       <c r="X57" s="104">
@@ -17766,7 +17624,7 @@
       </c>
       <c r="E58" s="58" cm="1">
         <f t="array" aca="1" ref="E58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433333333334</v>
+        <v>45975.436805555553</v>
       </c>
       <c r="F58" s="64" cm="1">
         <f t="array" aca="1" ref="F58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17778,7 +17636,7 @@
       </c>
       <c r="H58" s="64" cm="1">
         <f t="array" aca="1" ref="H58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>15.14</v>
+        <v>15.22</v>
       </c>
       <c r="I58" s="64" cm="1">
         <f t="array" aca="1" ref="I58" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -17790,15 +17648,15 @@
       </c>
       <c r="K58" s="59" cm="1">
         <f t="array" aca="1" ref="K58" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>12.5124</v>
+        <v>12.5785</v>
       </c>
       <c r="L58" s="60" cm="1">
         <f t="array" aca="1" ref="L58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-8.5000000000000006E-2</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="M58" s="61" cm="1">
         <f t="array" aca="1" ref="M58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-5.5830000000000003E-3</v>
+        <v>-3.2840000000000001E-4</v>
       </c>
       <c r="N58" s="64" cm="1">
         <f t="array" aca="1" ref="N58" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -17810,7 +17668,7 @@
       </c>
       <c r="P58" s="62" cm="1">
         <f t="array" aca="1" ref="P58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8580</v>
+        <v>8610</v>
       </c>
       <c r="Q58" s="62" cm="1">
         <f t="array" aca="1" ref="Q58" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17832,7 +17690,7 @@
       </c>
       <c r="V58" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.2154513530262343E-3</v>
+        <v>2.2231976864284238E-3</v>
       </c>
       <c r="W58" s="90"/>
       <c r="X58" s="104">
@@ -17884,7 +17742,7 @@
       </c>
       <c r="E59" s="58" cm="1">
         <f t="array" aca="1" ref="E59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433831018519</v>
+        <v>45975.437175925923</v>
       </c>
       <c r="F59" s="64" cm="1">
         <f t="array" aca="1" ref="F59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -17896,7 +17754,7 @@
       </c>
       <c r="H59" s="64" cm="1">
         <f t="array" aca="1" ref="H59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>16.423999999999999</v>
+        <v>16.411999999999999</v>
       </c>
       <c r="I59" s="64" cm="1">
         <f t="array" aca="1" ref="I59" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -17908,15 +17766,15 @@
       </c>
       <c r="K59" s="59" cm="1">
         <f t="array" aca="1" ref="K59" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>18.138000000000002</v>
+        <v>18.1248</v>
       </c>
       <c r="L59" s="60" cm="1">
         <f t="array" aca="1" ref="L59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-3.4000000000000002E-2</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="M59" s="61" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.0660000000000001E-3</v>
+        <v>-2.7950000000000002E-3</v>
       </c>
       <c r="N59" s="64" cm="1">
         <f t="array" aca="1" ref="N59" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -17928,7 +17786,7 @@
       </c>
       <c r="P59" s="62" cm="1">
         <f t="array" aca="1" ref="P59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2002696</v>
+        <v>2037548</v>
       </c>
       <c r="Q59" s="62" cm="1">
         <f t="array" aca="1" ref="Q59" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -17950,7 +17808,7 @@
       </c>
       <c r="V59" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.21541685131722177</v>
+        <v>0.21916565198497553</v>
       </c>
       <c r="W59" s="90"/>
       <c r="X59" s="104">
@@ -17997,7 +17855,7 @@
       </c>
       <c r="B60" s="112">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C60" t="e" vm="20">
         <v>#VALUE!</v>
@@ -18128,7 +17986,7 @@
       </c>
       <c r="E61" s="58" cm="1">
         <f t="array" aca="1" ref="E61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433796296296</v>
+        <v>45975.437175925923</v>
       </c>
       <c r="F61" s="64" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18140,7 +17998,7 @@
       </c>
       <c r="H61" s="64" cm="1">
         <f t="array" aca="1" ref="H61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>57.9</v>
+        <v>57.88</v>
       </c>
       <c r="I61" s="64" cm="1">
         <f t="array" aca="1" ref="I61" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -18152,15 +18010,15 @@
       </c>
       <c r="K61" s="59" cm="1">
         <f t="array" aca="1" ref="K61" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>9.2719000000000005</v>
+        <v>9.2687000000000008</v>
       </c>
       <c r="L61" s="60" cm="1">
         <f t="array" aca="1" ref="L61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-1.26</v>
+        <v>-1.28</v>
       </c>
       <c r="M61" s="61" cm="1">
         <f t="array" aca="1" ref="M61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.1297999999999997E-2</v>
+        <v>-2.1636000000000002E-2</v>
       </c>
       <c r="N61" s="64" cm="1">
         <f t="array" aca="1" ref="N61" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -18172,7 +18030,7 @@
       </c>
       <c r="P61" s="62" cm="1">
         <f t="array" aca="1" ref="P61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>429078</v>
+        <v>430071</v>
       </c>
       <c r="Q61" s="62" cm="1">
         <f t="array" aca="1" ref="Q61" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18194,7 +18052,7 @@
       </c>
       <c r="V61" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.19961294224372544</v>
+        <v>0.20007489939754833</v>
       </c>
       <c r="W61" s="90"/>
       <c r="X61" s="104">
@@ -18251,7 +18109,7 @@
       </c>
       <c r="E62" s="58" cm="1">
         <f t="array" aca="1" ref="E62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.43375081016</v>
+        <v>45975.4372337963</v>
       </c>
       <c r="F62" s="64" cm="1">
         <f t="array" aca="1" ref="F62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18263,11 +18121,11 @@
       </c>
       <c r="H62" s="64" cm="1">
         <f t="array" aca="1" ref="H62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>14.045</v>
+        <v>14.04</v>
       </c>
       <c r="I62" s="64" cm="1">
         <f t="array" aca="1" ref="I62" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
-        <v>14.045</v>
+        <v>14.025</v>
       </c>
       <c r="J62" s="64" cm="1">
         <f t="array" aca="1" ref="J62" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"High"),0)</f>
@@ -18275,15 +18133,15 @@
       </c>
       <c r="K62" s="59" cm="1">
         <f t="array" aca="1" ref="K62" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>44.362000000000002</v>
+        <v>44.346200000000003</v>
       </c>
       <c r="L62" s="60" cm="1">
         <f t="array" aca="1" ref="L62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-0.28499999999999998</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="M62" s="61" cm="1">
         <f t="array" aca="1" ref="M62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-1.9887999999999999E-2</v>
+        <v>-2.0236999999999998E-2</v>
       </c>
       <c r="N62" s="64" cm="1">
         <f t="array" aca="1" ref="N62" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -18295,7 +18153,7 @@
       </c>
       <c r="P62" s="62" cm="1">
         <f t="array" aca="1" ref="P62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>489474</v>
+        <v>500881</v>
       </c>
       <c r="Q62" s="62" cm="1">
         <f t="array" aca="1" ref="Q62" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18317,7 +18175,7 @@
       </c>
       <c r="V62" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.14691154224794103</v>
+        <v>0.15033525824189017</v>
       </c>
       <c r="W62" s="90"/>
       <c r="X62" s="104">
@@ -18374,7 +18232,7 @@
       </c>
       <c r="E63" s="58" cm="1">
         <f t="array" aca="1" ref="E63" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433333333334</v>
+        <v>45975.436805555553</v>
       </c>
       <c r="F63" s="64" cm="1">
         <f t="array" aca="1" ref="F63" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18492,7 +18350,7 @@
       </c>
       <c r="E64" s="58" cm="1">
         <f t="array" aca="1" ref="E64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.43377314815</v>
+        <v>45975.437245370369</v>
       </c>
       <c r="F64" s="64" cm="1">
         <f t="array" aca="1" ref="F64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18504,11 +18362,11 @@
       </c>
       <c r="H64" s="64" cm="1">
         <f t="array" aca="1" ref="H64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>210.5</v>
+        <v>210.75</v>
       </c>
       <c r="I64" s="64" cm="1">
         <f t="array" aca="1" ref="I64" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
-        <v>210.4</v>
+        <v>210.35</v>
       </c>
       <c r="J64" s="64" cm="1">
         <f t="array" aca="1" ref="J64" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"High"),0)</f>
@@ -18516,15 +18374,15 @@
       </c>
       <c r="K64" s="59" cm="1">
         <f t="array" aca="1" ref="K64" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>34.674199999999999</v>
+        <v>34.715400000000002</v>
       </c>
       <c r="L64" s="60" cm="1">
         <f t="array" aca="1" ref="L64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-7.6</v>
+        <v>-7.35</v>
       </c>
       <c r="M64" s="61" cm="1">
         <f t="array" aca="1" ref="M64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-3.4846000000000002E-2</v>
+        <v>-3.3700000000000001E-2</v>
       </c>
       <c r="N64" s="64" cm="1">
         <f t="array" aca="1" ref="N64" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -18536,7 +18394,7 @@
       </c>
       <c r="P64" s="62" cm="1">
         <f t="array" aca="1" ref="P64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>260937</v>
+        <v>263672</v>
       </c>
       <c r="Q64" s="62" cm="1">
         <f t="array" aca="1" ref="Q64" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18558,7 +18416,7 @@
       </c>
       <c r="V64" s="90">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.22274702292031243</v>
+        <v>0.22508173630970166</v>
       </c>
       <c r="W64" s="90"/>
       <c r="X64" s="104">
@@ -18722,7 +18580,7 @@
       </c>
       <c r="B66" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C66" t="e" vm="1">
         <v>#VALUE!</v>
@@ -18843,7 +18701,7 @@
       </c>
       <c r="B67" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C67" t="e" vm="4">
         <v>#VALUE!</v>
@@ -18898,7 +18756,7 @@
       </c>
       <c r="P67" s="22" cm="1">
         <f t="array" aca="1" ref="P67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>73714</v>
+        <v>74470</v>
       </c>
       <c r="Q67" s="22" cm="1">
         <f t="array" aca="1" ref="Q67" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -18920,7 +18778,7 @@
       </c>
       <c r="V67" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.3979648473495174E-3</v>
+        <v>1.4123021703084701E-3</v>
       </c>
       <c r="W67" s="23"/>
       <c r="X67" s="104">
@@ -18974,7 +18832,7 @@
       </c>
       <c r="E68" s="17" cm="1">
         <f t="array" aca="1" ref="E68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433807870373</v>
+        <v>45975.4372337963</v>
       </c>
       <c r="F68" s="27" cm="1">
         <f t="array" aca="1" ref="F68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -18986,7 +18844,7 @@
       </c>
       <c r="H68" s="27" cm="1">
         <f t="array" aca="1" ref="H68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>857.7</v>
+        <v>859.4</v>
       </c>
       <c r="I68" s="27" cm="1">
         <f t="array" aca="1" ref="I68" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -18998,15 +18856,15 @@
       </c>
       <c r="K68" s="19" cm="1">
         <f t="array" aca="1" ref="K68" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>32.932600000000001</v>
+        <v>32.997900000000001</v>
       </c>
       <c r="L68" s="20" cm="1">
         <f t="array" aca="1" ref="L68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-23.8</v>
+        <v>-22.1</v>
       </c>
       <c r="M68" s="21" cm="1">
         <f t="array" aca="1" ref="M68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.6998999999999999E-2</v>
+        <v>-2.5071E-2</v>
       </c>
       <c r="N68" s="27" cm="1">
         <f t="array" aca="1" ref="N68" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -19018,7 +18876,7 @@
       </c>
       <c r="P68" s="22" cm="1">
         <f t="array" aca="1" ref="P68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>153992</v>
+        <v>155625</v>
       </c>
       <c r="Q68" s="22" cm="1">
         <f t="array" aca="1" ref="Q68" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19040,7 +18898,7 @@
       </c>
       <c r="V68" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.28183531909441972</v>
+        <v>0.28482402679404822</v>
       </c>
       <c r="W68" s="23"/>
       <c r="X68" s="104">
@@ -19085,7 +18943,7 @@
       </c>
       <c r="B69" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C69" t="e" vm="14">
         <v>#VALUE!</v>
@@ -19206,7 +19064,7 @@
       </c>
       <c r="B70" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C70" t="e" vm="15">
         <v>#VALUE!</v>
@@ -19261,7 +19119,7 @@
       </c>
       <c r="P70" s="22" cm="1">
         <f t="array" aca="1" ref="P70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7555</v>
+        <v>8260</v>
       </c>
       <c r="Q70" s="22" cm="1">
         <f t="array" aca="1" ref="Q70" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19283,7 +19141,7 @@
       </c>
       <c r="V70" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>9.1920543176800739E-4</v>
+        <v>1.0049817162678678E-3</v>
       </c>
       <c r="W70" s="23"/>
       <c r="X70" s="104">
@@ -19327,7 +19185,7 @@
       </c>
       <c r="B71" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C71" t="e" vm="21">
         <v>#VALUE!</v>
@@ -19448,7 +19306,7 @@
       </c>
       <c r="B72" s="38">
         <f ca="1">D101/100</f>
-        <v>1.1318619128466328E-2</v>
+        <v>1.1316057485572026E-2</v>
       </c>
       <c r="C72" t="e" vm="24">
         <v>#VALUE!</v>
@@ -19459,7 +19317,7 @@
       </c>
       <c r="E72" s="17" cm="1">
         <f t="array" aca="1" ref="E72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433682233597</v>
+        <v>45975.437146122655</v>
       </c>
       <c r="F72" s="18" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -19471,7 +19329,7 @@
       </c>
       <c r="H72" s="18" cm="1">
         <f t="array" aca="1" ref="H72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>387.6</v>
+        <v>387.4</v>
       </c>
       <c r="I72" s="18" cm="1">
         <f t="array" aca="1" ref="I72" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -19483,15 +19341,15 @@
       </c>
       <c r="K72" s="19" cm="1">
         <f t="array" aca="1" ref="K72" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>6.9824999999999999</v>
+        <v>6.9789000000000003</v>
       </c>
       <c r="L72" s="20" cm="1">
         <f t="array" aca="1" ref="L72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-8.1999999999999993</v>
+        <v>-8.4</v>
       </c>
       <c r="M72" s="21" cm="1">
         <f t="array" aca="1" ref="M72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.0718E-2</v>
+        <v>-2.1223000000000002E-2</v>
       </c>
       <c r="N72" s="18" cm="1">
         <f t="array" aca="1" ref="N72" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -19503,7 +19361,7 @@
       </c>
       <c r="P72" s="22" cm="1">
         <f t="array" aca="1" ref="P72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2337191</v>
+        <v>2389916</v>
       </c>
       <c r="Q72" s="22" cm="1">
         <f t="array" aca="1" ref="Q72" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19525,7 +19383,7 @@
       </c>
       <c r="V72" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.12022488498037054</v>
+        <v>0.12293705401601633</v>
       </c>
       <c r="W72" s="23"/>
       <c r="X72" s="104">
@@ -19569,7 +19427,7 @@
       </c>
       <c r="B73" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C73" t="e" vm="28">
         <v>#VALUE!</v>
@@ -19690,7 +19548,7 @@
       </c>
       <c r="B74" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C74" t="e" vm="56">
         <v>#VALUE!</v>
@@ -19818,7 +19676,7 @@
       </c>
       <c r="E75" s="17" cm="1">
         <f t="array" aca="1" ref="E75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433831018519</v>
+        <v>45975.437175925923</v>
       </c>
       <c r="F75" s="18" cm="1">
         <f t="array" aca="1" ref="F75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -19830,7 +19688,7 @@
       </c>
       <c r="H75" s="18" cm="1">
         <f t="array" aca="1" ref="H75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>16.423999999999999</v>
+        <v>16.411999999999999</v>
       </c>
       <c r="I75" s="18" cm="1">
         <f t="array" aca="1" ref="I75" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -19842,15 +19700,15 @@
       </c>
       <c r="K75" s="19" cm="1">
         <f t="array" aca="1" ref="K75" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>18.138000000000002</v>
+        <v>18.1248</v>
       </c>
       <c r="L75" s="20" cm="1">
         <f t="array" aca="1" ref="L75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-3.4000000000000002E-2</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="M75" s="21" cm="1">
         <f t="array" aca="1" ref="M75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.0660000000000001E-3</v>
+        <v>-2.7950000000000002E-3</v>
       </c>
       <c r="N75" s="18" cm="1">
         <f t="array" aca="1" ref="N75" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -19862,7 +19720,7 @@
       </c>
       <c r="P75" s="22" cm="1">
         <f t="array" aca="1" ref="P75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>2002696</v>
+        <v>2037548</v>
       </c>
       <c r="Q75" s="22" cm="1">
         <f t="array" aca="1" ref="Q75" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19881,7 +19739,7 @@
       </c>
       <c r="V75" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.21541685131722177</v>
+        <v>0.21916565198497553</v>
       </c>
       <c r="W75" s="23"/>
       <c r="X75" s="104">
@@ -19923,7 +19781,7 @@
       </c>
       <c r="B76" s="15">
         <f ca="1">D101/100</f>
-        <v>1.1318619128466328E-2</v>
+        <v>1.1316057485572026E-2</v>
       </c>
       <c r="C76" t="e" vm="57">
         <v>#VALUE!</v>
@@ -19934,7 +19792,7 @@
       </c>
       <c r="E76" s="17" cm="1">
         <f t="array" aca="1" ref="E76" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433195346872</v>
+        <v>45975.437199375003</v>
       </c>
       <c r="F76" s="18" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -19978,7 +19836,7 @@
       </c>
       <c r="P76" s="22" cm="1">
         <f t="array" aca="1" ref="P76" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>677099</v>
+        <v>683767</v>
       </c>
       <c r="Q76" s="22" cm="1">
         <f t="array" aca="1" ref="Q76" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -19997,7 +19855,7 @@
       </c>
       <c r="V76" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.17205559861257574</v>
+        <v>0.17374998411831222</v>
       </c>
       <c r="W76" s="23"/>
       <c r="X76" s="104">
@@ -20039,7 +19897,7 @@
       </c>
       <c r="B77" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C77" t="e" vm="58">
         <v>#VALUE!</v>
@@ -20167,7 +20025,7 @@
       </c>
       <c r="E78" s="17" cm="1">
         <f t="array" aca="1" ref="E78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433796296296</v>
+        <v>45975.437175925923</v>
       </c>
       <c r="F78" s="27" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -20179,7 +20037,7 @@
       </c>
       <c r="H78" s="27" cm="1">
         <f t="array" aca="1" ref="H78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>57.9</v>
+        <v>57.88</v>
       </c>
       <c r="I78" s="27" cm="1">
         <f t="array" aca="1" ref="I78" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -20191,15 +20049,15 @@
       </c>
       <c r="K78" s="19" cm="1">
         <f t="array" aca="1" ref="K78" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>9.2719000000000005</v>
+        <v>9.2687000000000008</v>
       </c>
       <c r="L78" s="20" cm="1">
         <f t="array" aca="1" ref="L78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-1.26</v>
+        <v>-1.28</v>
       </c>
       <c r="M78" s="21" cm="1">
         <f t="array" aca="1" ref="M78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.1297999999999997E-2</v>
+        <v>-2.1636000000000002E-2</v>
       </c>
       <c r="N78" s="27" cm="1">
         <f t="array" aca="1" ref="N78" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -20211,7 +20069,7 @@
       </c>
       <c r="P78" s="22" cm="1">
         <f t="array" aca="1" ref="P78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>429078</v>
+        <v>430071</v>
       </c>
       <c r="Q78" s="22" cm="1">
         <f t="array" aca="1" ref="Q78" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20230,7 +20088,7 @@
       </c>
       <c r="V78" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.19961294224372544</v>
+        <v>0.20007489939754833</v>
       </c>
       <c r="W78" s="23"/>
       <c r="X78" s="104">
@@ -20272,7 +20130,7 @@
       </c>
       <c r="B79" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C79" t="e" vm="59">
         <v>#VALUE!</v>
@@ -20390,7 +20248,7 @@
       </c>
       <c r="B80" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C80" t="e" vm="60">
         <v>#VALUE!</v>
@@ -20445,7 +20303,7 @@
       </c>
       <c r="P80" s="22" cm="1">
         <f t="array" aca="1" ref="P80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>1775</v>
+        <v>1869</v>
       </c>
       <c r="Q80" s="22" cm="1">
         <f t="array" aca="1" ref="Q80" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20464,7 +20322,7 @@
       </c>
       <c r="V80" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>8.1673106955419824E-4</v>
+        <v>8.5998330647706848E-4</v>
       </c>
       <c r="W80" s="23"/>
       <c r="X80" s="104">
@@ -20508,7 +20366,7 @@
       </c>
       <c r="B81" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C81" t="e" vm="61">
         <v>#VALUE!</v>
@@ -20563,7 +20421,7 @@
       </c>
       <c r="P81" s="22" cm="1">
         <f t="array" aca="1" ref="P81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>47980</v>
+        <v>49873</v>
       </c>
       <c r="Q81" s="22" cm="1">
         <f t="array" aca="1" ref="Q81" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20582,7 +20440,7 @@
       </c>
       <c r="V81" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>4.548562301652158E-3</v>
+        <v>4.7280210018819935E-3</v>
       </c>
       <c r="W81" s="23"/>
       <c r="X81" s="104">
@@ -20626,7 +20484,7 @@
       </c>
       <c r="B82" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C82" t="e" vm="62">
         <v>#VALUE!</v>
@@ -20744,7 +20602,7 @@
       </c>
       <c r="B83" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C83" t="e" vm="63">
         <v>#VALUE!</v>
@@ -20799,7 +20657,7 @@
       </c>
       <c r="P83" s="22" cm="1">
         <f t="array" aca="1" ref="P83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="Q83" s="22" cm="1">
         <f t="array" aca="1" ref="Q83" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20818,7 +20676,7 @@
       </c>
       <c r="V83" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>7.4450497340545924E-5</v>
+        <v>7.7817605260470111E-5</v>
       </c>
       <c r="W83" s="23"/>
       <c r="X83" s="104">
@@ -20862,7 +20720,7 @@
       </c>
       <c r="B84" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C84" t="e" vm="64">
         <v>#VALUE!</v>
@@ -20917,7 +20775,7 @@
       </c>
       <c r="P84" s="22" cm="1">
         <f t="array" aca="1" ref="P84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>652</v>
+        <v>698</v>
       </c>
       <c r="Q84" s="22" cm="1">
         <f t="array" aca="1" ref="Q84" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -20936,7 +20794,7 @@
       </c>
       <c r="V84" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.4821405473872386E-4</v>
+        <v>1.5867087455157861E-4</v>
       </c>
       <c r="W84" s="23"/>
       <c r="X84" s="104">
@@ -20980,7 +20838,7 @@
       </c>
       <c r="B85" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C85" t="e" vm="65">
         <v>#VALUE!</v>
@@ -21108,7 +20966,7 @@
       </c>
       <c r="E86" s="17" cm="1">
         <f t="array" aca="1" ref="E86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.43375081016</v>
+        <v>45975.4372337963</v>
       </c>
       <c r="F86" s="27" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -21120,11 +20978,11 @@
       </c>
       <c r="H86" s="27" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>14.045</v>
+        <v>14.04</v>
       </c>
       <c r="I86" s="27" cm="1">
         <f t="array" aca="1" ref="I86" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
-        <v>14.045</v>
+        <v>14.025</v>
       </c>
       <c r="J86" s="27" cm="1">
         <f t="array" aca="1" ref="J86" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"High"),0)</f>
@@ -21132,15 +20990,15 @@
       </c>
       <c r="K86" s="19" cm="1">
         <f t="array" aca="1" ref="K86" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>44.362000000000002</v>
+        <v>44.346200000000003</v>
       </c>
       <c r="L86" s="20" cm="1">
         <f t="array" aca="1" ref="L86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-0.28499999999999998</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="M86" s="21" cm="1">
         <f t="array" aca="1" ref="M86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-1.9887999999999999E-2</v>
+        <v>-2.0236999999999998E-2</v>
       </c>
       <c r="N86" s="27" cm="1">
         <f t="array" aca="1" ref="N86" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -21152,7 +21010,7 @@
       </c>
       <c r="P86" s="22" cm="1">
         <f t="array" aca="1" ref="P86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>489474</v>
+        <v>500881</v>
       </c>
       <c r="Q86" s="22" cm="1">
         <f t="array" aca="1" ref="Q86" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21171,7 +21029,7 @@
       </c>
       <c r="V86" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.14691154224794103</v>
+        <v>0.15033525824189017</v>
       </c>
       <c r="W86" s="23"/>
       <c r="X86" s="104">
@@ -21213,7 +21071,7 @@
       </c>
       <c r="B87" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C87" t="e" vm="66">
         <v>#VALUE!</v>
@@ -21268,7 +21126,7 @@
       </c>
       <c r="P87" s="22" cm="1">
         <f t="array" aca="1" ref="P87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>7838</v>
+        <v>8177</v>
       </c>
       <c r="Q87" s="22" cm="1">
         <f t="array" aca="1" ref="Q87" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21287,7 +21145,7 @@
       </c>
       <c r="V87" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>7.5839644917969717E-4</v>
+        <v>7.9119772453972747E-4</v>
       </c>
       <c r="W87" s="23"/>
       <c r="X87" s="104">
@@ -21331,7 +21189,7 @@
       </c>
       <c r="B88" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C88" t="e" vm="67">
         <v>#VALUE!</v>
@@ -21386,7 +21244,7 @@
       </c>
       <c r="P88" s="22" cm="1">
         <f t="array" aca="1" ref="P88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>81475</v>
+        <v>85298</v>
       </c>
       <c r="Q88" s="22" cm="1">
         <f t="array" aca="1" ref="Q88" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -21405,7 +21263,7 @@
       </c>
       <c r="V88" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>1.0181416534890374E-3</v>
+        <v>1.0659152716699346E-3</v>
       </c>
       <c r="W88" s="23"/>
       <c r="X88" s="104">
@@ -21449,7 +21307,7 @@
       </c>
       <c r="B89" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C89" t="e" vm="68">
         <v>#VALUE!</v>
@@ -21567,7 +21425,7 @@
       </c>
       <c r="B90" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C90" t="e" vm="69">
         <v>#VALUE!</v>
@@ -21685,7 +21543,7 @@
       </c>
       <c r="B91" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C91" t="e" vm="70">
         <v>#VALUE!</v>
@@ -21803,7 +21661,7 @@
       </c>
       <c r="B92" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C92" t="e" vm="71">
         <v>#VALUE!</v>
@@ -21921,7 +21779,7 @@
       </c>
       <c r="B93" s="38">
         <f ca="1">D99</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="C93" t="e" vm="72">
         <v>#VALUE!</v>
@@ -22169,7 +22027,7 @@
       </c>
       <c r="E95" s="17" cm="1">
         <f t="array" aca="1" ref="E95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433807870373</v>
+        <v>45975.4372337963</v>
       </c>
       <c r="F95" s="27" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22181,7 +22039,7 @@
       </c>
       <c r="H95" s="27" cm="1">
         <f t="array" aca="1" ref="H95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>857.7</v>
+        <v>859.4</v>
       </c>
       <c r="I95" s="27" cm="1">
         <f t="array" aca="1" ref="I95" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -22193,15 +22051,15 @@
       </c>
       <c r="K95" s="19" cm="1">
         <f t="array" aca="1" ref="K95" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>32.932600000000001</v>
+        <v>32.997900000000001</v>
       </c>
       <c r="L95" s="20" cm="1">
         <f t="array" aca="1" ref="L95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-23.8</v>
+        <v>-22.1</v>
       </c>
       <c r="M95" s="21" cm="1">
         <f t="array" aca="1" ref="M95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-2.6998999999999999E-2</v>
+        <v>-2.5071E-2</v>
       </c>
       <c r="N95" s="27" cm="1">
         <f t="array" aca="1" ref="N95" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -22213,7 +22071,7 @@
       </c>
       <c r="P95" s="22" cm="1">
         <f t="array" aca="1" ref="P95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>153992</v>
+        <v>155625</v>
       </c>
       <c r="Q95" s="22" cm="1">
         <f t="array" aca="1" ref="Q95" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22235,7 +22093,7 @@
       </c>
       <c r="V95" s="23">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>0.28183531909441972</v>
+        <v>0.28482402679404822</v>
       </c>
       <c r="W95" s="23"/>
       <c r="X95" s="104">
@@ -22291,7 +22149,7 @@
       </c>
       <c r="E96" s="17" cm="1">
         <f t="array" aca="1" ref="E96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Last trade time",TRUE)</f>
-        <v>45975.433333333334</v>
+        <v>45975.436805555553</v>
       </c>
       <c r="F96" s="18" cm="1">
         <f t="array" aca="1" ref="F96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Previous close",TRUE)</f>
@@ -22303,7 +22161,7 @@
       </c>
       <c r="H96" s="18" cm="1">
         <f t="array" aca="1" ref="H96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Price")</f>
-        <v>15.14</v>
+        <v>15.22</v>
       </c>
       <c r="I96" s="18" cm="1">
         <f t="array" aca="1" ref="I96" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"Low"),0)</f>
@@ -22315,15 +22173,15 @@
       </c>
       <c r="K96" s="19" cm="1">
         <f t="array" aca="1" ref="K96" ca="1">IFERROR(_FV(RTData[[#This Row],[Company Name]],"P/E",TRUE),99)</f>
-        <v>12.5124</v>
+        <v>12.5785</v>
       </c>
       <c r="L96" s="20" cm="1">
         <f t="array" aca="1" ref="L96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change")</f>
-        <v>-8.5000000000000006E-2</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="M96" s="21" cm="1">
         <f t="array" aca="1" ref="M96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Change (%)",TRUE)</f>
-        <v>-5.5830000000000003E-3</v>
+        <v>-3.2840000000000001E-4</v>
       </c>
       <c r="N96" s="27" cm="1">
         <f t="array" aca="1" ref="N96" ca="1">_FV(RTData[[#This Row],[Company Name]],"52 week low",TRUE)</f>
@@ -22335,7 +22193,7 @@
       </c>
       <c r="P96" s="22" cm="1">
         <f t="array" aca="1" ref="P96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume")</f>
-        <v>8580</v>
+        <v>8610</v>
       </c>
       <c r="Q96" s="22" cm="1">
         <f t="array" aca="1" ref="Q96" ca="1">_FV(RTData[[#This Row],[Company Name]],"Volume average",TRUE)</f>
@@ -22357,7 +22215,7 @@
       </c>
       <c r="V96" s="103">
         <f ca="1">IFERROR(RTData[[#This Row],[Volume]]/RTData[[#This Row],[Volume average]],1)</f>
-        <v>2.2154513530262343E-3</v>
+        <v>2.2231976864284238E-3</v>
       </c>
       <c r="W96" s="103"/>
       <c r="X96" s="104">
@@ -22407,7 +22265,7 @@
       <c r="K97"/>
       <c r="L97" s="20">
         <f ca="1">SUBTOTAL(101,RTData[Change])</f>
-        <v>-2.9731936170212743</v>
+        <v>-2.9167893617021265</v>
       </c>
       <c r="M97" s="42">
         <f ca="1">SUBTOTAL(104,RTData[Change%])</f>
@@ -22458,7 +22316,7 @@
       </c>
       <c r="B99" s="46" cm="1">
         <f t="array" aca="1" ref="B99" ca="1">_FV(A99,"Price")</f>
-        <v>1.1613</v>
+        <v>1.1614</v>
       </c>
       <c r="C99" s="47" cm="1">
         <f t="array" aca="1" ref="C99" ca="1">_FV(A99,"52 week high",TRUE)</f>
@@ -22466,7 +22324,7 @@
       </c>
       <c r="D99" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>0.86110393524498408</v>
+        <v>0.86102979163079041</v>
       </c>
       <c r="P99" s="48"/>
       <c r="R99"/>
@@ -22479,7 +22337,7 @@
       </c>
       <c r="B100" s="46" cm="1">
         <f t="array" aca="1" ref="B100" ca="1">_FV(A100,"Price")</f>
-        <v>0.91969999999999996</v>
+        <v>0.91979999999999995</v>
       </c>
       <c r="C100" s="50" cm="1">
         <f t="array" aca="1" ref="C100" ca="1">_FV(A100,"52 week high",TRUE)</f>
@@ -22487,7 +22345,7 @@
       </c>
       <c r="D100" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>1.0873110796999021</v>
+        <v>1.087192868014786</v>
       </c>
       <c r="P100" s="48"/>
       <c r="R100"/>
@@ -22498,7 +22356,7 @@
       </c>
       <c r="B101" s="46" cm="1">
         <f t="array" aca="1" ref="B101" ca="1">_FV(A101,"Price")</f>
-        <v>0.88349999999999995</v>
+        <v>0.88370000000000004</v>
       </c>
       <c r="C101" s="51" cm="1">
         <f t="array" aca="1" ref="C101" ca="1">_FV(A101,"52 week high",TRUE)</f>
@@ -22506,7 +22364,7 @@
       </c>
       <c r="D101" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>1.1318619128466327</v>
+        <v>1.1316057485572026</v>
       </c>
       <c r="P101" s="48"/>
       <c r="R101"/>
@@ -22517,7 +22375,7 @@
       </c>
       <c r="B102" s="46" cm="1">
         <f t="array" aca="1" ref="B102" ca="1">_FV(A102,"Price")</f>
-        <v>1.7810999999999999</v>
+        <v>1.7806999999999999</v>
       </c>
       <c r="C102" s="47" cm="1">
         <f t="array" aca="1" ref="C102" ca="1">_FV(A102,"52 week high",TRUE)</f>
@@ -22525,7 +22383,7 @@
       </c>
       <c r="D102" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>0.56145078883835831</v>
+        <v>0.56157690795754478</v>
       </c>
       <c r="P102" s="48"/>
       <c r="R102"/>
@@ -22536,7 +22394,7 @@
       </c>
       <c r="B103" s="46" cm="1">
         <f t="array" aca="1" ref="B103" ca="1">_FV(A103,"Price")</f>
-        <v>1.6303000000000001</v>
+        <v>1.6304000000000001</v>
       </c>
       <c r="C103" s="47" cm="1">
         <f t="array" aca="1" ref="C103" ca="1">_FV(A103,"52 week high",TRUE)</f>
@@ -22544,7 +22402,7 @@
       </c>
       <c r="D103" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>0.61338403974728573</v>
+        <v>0.61334641805691847</v>
       </c>
       <c r="P103" s="48"/>
       <c r="R103"/>
@@ -22555,7 +22413,7 @@
       </c>
       <c r="B104" s="46" cm="1">
         <f t="array" aca="1" ref="B104" ca="1">_FV(A104,"Price")</f>
-        <v>154.71</v>
+        <v>154.69</v>
       </c>
       <c r="C104" s="52" cm="1">
         <f t="array" aca="1" ref="C104" ca="1">_FV(A104,"52 week high",TRUE)</f>
@@ -22563,7 +22421,7 @@
       </c>
       <c r="D104" s="18">
         <f ca="1">1/RTExR[[#This Row],[RT]]</f>
-        <v>6.4637062891862189E-3</v>
+        <v>6.4645419872002069E-3</v>
       </c>
       <c r="J104"/>
       <c r="P104" s="48"/>

</xml_diff>